<commit_message>
fixed page up down
</commit_message>
<xml_diff>
--- a/FxTextEditor Features.xlsx
+++ b/FxTextEditor Features.xlsx
@@ -1024,7 +1024,7 @@
           <c:yMode val="edge"/>
           <c:x val="3.8461559098965002E-2"/>
           <c:y val="2.2690437601296611E-2"/>
-          <c:w val="0.91978071330955369"/>
+          <c:w val="0.9197807133095538"/>
           <c:h val="0.89627228525119951"/>
         </c:manualLayout>
       </c:layout>
@@ -1110,7 +1110,7 @@
                   <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>94</c:v>
+                  <c:v>102</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1196,7 +1196,7 @@
                   <c:v>201</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>167</c:v>
+                  <c:v>159</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1380,11 +1380,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="162712960"/>
-        <c:axId val="162473088"/>
+        <c:axId val="153013632"/>
+        <c:axId val="152839296"/>
       </c:areaChart>
       <c:dateAx>
-        <c:axId val="162712960"/>
+        <c:axId val="153013632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1417,7 +1417,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="162473088"/>
+        <c:crossAx val="152839296"/>
         <c:crosses val="autoZero"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
@@ -1427,7 +1427,7 @@
         <c:minorTimeUnit val="months"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="162473088"/>
+        <c:axId val="152839296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1469,7 +1469,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="162712960"/>
+        <c:crossAx val="153013632"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1492,7 +1492,7 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="4.5828229804607823E-2"/>
-          <c:y val="0.33819556996218497"/>
+          <c:y val="0.33819556996218503"/>
           <c:w val="0.12857154394162268"/>
           <c:h val="0.11669367909238262"/>
         </c:manualLayout>
@@ -1613,7 +1613,7 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="4.4510450248127761E-2"/>
+          <c:x val="4.4510450248127775E-2"/>
           <c:y val="0.10032394165889739"/>
           <c:w val="0.79228601441663349"/>
           <c:h val="0.79935527708863363"/>
@@ -1701,17 +1701,17 @@
                   <c:v>0.22093023255813954</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.36015325670498083</c:v>
+                  <c:v>0.39080459770114945</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="162500992"/>
-        <c:axId val="162502528"/>
+        <c:axId val="152863104"/>
+        <c:axId val="152864640"/>
       </c:areaChart>
       <c:dateAx>
-        <c:axId val="162500992"/>
+        <c:axId val="152863104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1719,13 +1719,13 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="yyyy\/mm\/dd" sourceLinked="1"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="162502528"/>
+        <c:crossAx val="152864640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="162502528"/>
+        <c:axId val="152864640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1768,7 +1768,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="162500992"/>
+        <c:crossAx val="152863104"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1921,7 +1921,7 @@
                   <c:v>201</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>167</c:v>
+                  <c:v>159</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2013,11 +2013,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="162523392"/>
-        <c:axId val="162725888"/>
+        <c:axId val="152889600"/>
+        <c:axId val="153288704"/>
       </c:areaChart>
       <c:dateAx>
-        <c:axId val="162523392"/>
+        <c:axId val="152889600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2050,7 +2050,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="162725888"/>
+        <c:crossAx val="153288704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -2059,7 +2059,7 @@
         <c:minorTimeUnit val="months"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="162725888"/>
+        <c:axId val="153288704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2101,7 +2101,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="162523392"/>
+        <c:crossAx val="152889600"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2610,8 +2610,8 @@
   </sheetPr>
   <dimension ref="A1:D443"/>
   <sheetViews>
-    <sheetView topLeftCell="A140" workbookViewId="0">
-      <selection activeCell="C160" sqref="C160"/>
+    <sheetView topLeftCell="A272" workbookViewId="0">
+      <selection activeCell="C321" sqref="C321"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5"/>
@@ -3055,7 +3055,7 @@
         <v>70</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D57" s="4"/>
     </row>
@@ -3064,7 +3064,7 @@
         <v>69</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D58" s="4"/>
     </row>
@@ -4887,7 +4887,7 @@
         <v>70</v>
       </c>
       <c r="C294" s="7" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D294" s="4"/>
     </row>
@@ -4896,7 +4896,7 @@
         <v>229</v>
       </c>
       <c r="C295" s="7" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D295" s="4"/>
     </row>
@@ -4910,7 +4910,7 @@
         <v>69</v>
       </c>
       <c r="C297" s="7" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D297" s="4"/>
     </row>
@@ -4919,7 +4919,7 @@
         <v>229</v>
       </c>
       <c r="C298" s="7" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D298" s="4"/>
     </row>
@@ -5045,7 +5045,7 @@
         <v>69</v>
       </c>
       <c r="C319" s="7" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
     <row r="320" spans="2:4">
@@ -5053,7 +5053,7 @@
         <v>70</v>
       </c>
       <c r="C320" s="7" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
     <row r="321" spans="2:3">
@@ -5744,7 +5744,7 @@
       </c>
       <c r="C438" s="6">
         <f>COUNTIF(C5:C437,"y")</f>
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="D438" s="2"/>
     </row>
@@ -5755,7 +5755,7 @@
       </c>
       <c r="C439" s="6">
         <f>COUNTIF(C5:C437,"n")</f>
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="D439" s="2"/>
     </row>
@@ -5789,7 +5789,7 @@
       </c>
       <c r="D442" s="41">
         <f>C438/(C439+C438 + C440)</f>
-        <v>0.36015325670498083</v>
+        <v>0.39080459770114945</v>
       </c>
     </row>
     <row r="443" spans="1:4">
@@ -5827,7 +5827,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="10020" topLeftCell="A46" activePane="bottomLeft"/>
       <selection activeCell="R30" sqref="R30"/>
-      <selection pane="bottomLeft" activeCell="A55" sqref="A55"/>
+      <selection pane="bottomLeft" activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5"/>
@@ -6206,10 +6206,10 @@
         <v>43972</v>
       </c>
       <c r="B54" s="4">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="C54" s="4">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="D54" s="4">
         <v>0</v>
@@ -6220,7 +6220,7 @@
       <c r="F54" s="48"/>
       <c r="G54" s="30">
         <f t="shared" ref="G54" si="3">B54/SUM(B54:E54)</f>
-        <v>0.36015325670498083</v>
+        <v>0.39080459770114945</v>
       </c>
       <c r="H54" s="7"/>
     </row>
@@ -6265,7 +6265,7 @@
       </c>
       <c r="G57" s="38">
         <f>MIN(G54)</f>
-        <v>0.36015325670498083</v>
+        <v>0.39080459770114945</v>
       </c>
       <c r="H57" s="7"/>
     </row>
@@ -6276,11 +6276,11 @@
       </c>
       <c r="B58" s="15">
         <f>Features!C438</f>
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="C58" s="16">
         <f>Features!C439</f>
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="D58" s="17">
         <f>Features!C440</f>
@@ -6331,7 +6331,7 @@
       </c>
       <c r="B62" s="49">
         <f>(A54-A48)*A58/B58 +A48</f>
-        <v>44640</v>
+        <v>44558.117647058825</v>
       </c>
       <c r="C62" s="4"/>
       <c r="D62" s="7"/>

</xml_diff>

<commit_message>
scroll caret to visible
</commit_message>
<xml_diff>
--- a/FxTextEditor Features.xlsx
+++ b/FxTextEditor Features.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="244">
   <si>
     <t>Feature</t>
   </si>
@@ -311,18 +311,6 @@
     <t>shift window down</t>
   </si>
   <si>
-    <t>semantics</t>
-  </si>
-  <si>
-    <t>shift: selects</t>
-  </si>
-  <si>
-    <t>ctrl: adds selection block</t>
-  </si>
-  <si>
-    <t>alt: mimics rectangular selection</t>
-  </si>
-  <si>
     <t>alt + shift click</t>
   </si>
   <si>
@@ -410,9 +398,6 @@
     <t>block scroll down</t>
   </si>
   <si>
-    <t>ctrl-scroll wheel</t>
-  </si>
-  <si>
     <t>reset blinking animation cycle on mouse released to avoid flicker</t>
   </si>
   <si>
@@ -533,9 +518,6 @@
     <t>line markers</t>
   </si>
   <si>
-    <t>right click: invokes a popup</t>
-  </si>
-  <si>
     <t>highlights matching tokens if enabled</t>
   </si>
   <si>
@@ -765,6 +747,9 @@
   </si>
   <si>
     <t>to the last line + 1</t>
+  </si>
+  <si>
+    <t>scrollWheelStepSize</t>
   </si>
 </sst>
 </file>
@@ -1024,7 +1009,7 @@
           <c:yMode val="edge"/>
           <c:x val="3.8461559098965002E-2"/>
           <c:y val="2.2690437601296611E-2"/>
-          <c:w val="0.9197807133095538"/>
+          <c:w val="0.91978071330955391"/>
           <c:h val="0.89627228525119951"/>
         </c:manualLayout>
       </c:layout>
@@ -1080,7 +1065,7 @@
                   <c:v>43959</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43972</c:v>
+                  <c:v>43974</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1110,7 +1095,7 @@
                   <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>102</c:v>
+                  <c:v>106</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1166,7 +1151,7 @@
                   <c:v>43959</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43972</c:v>
+                  <c:v>43974</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1196,7 +1181,7 @@
                   <c:v>201</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>159</c:v>
+                  <c:v>149</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1252,7 +1237,7 @@
                   <c:v>43959</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43972</c:v>
+                  <c:v>43974</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1338,7 +1323,7 @@
                   <c:v>43959</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43972</c:v>
+                  <c:v>43974</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1380,11 +1365,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="153013632"/>
-        <c:axId val="152839296"/>
+        <c:axId val="164875648"/>
+        <c:axId val="164635776"/>
       </c:areaChart>
       <c:dateAx>
-        <c:axId val="153013632"/>
+        <c:axId val="164875648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1417,7 +1402,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="152839296"/>
+        <c:crossAx val="164635776"/>
         <c:crosses val="autoZero"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
@@ -1427,7 +1412,7 @@
         <c:minorTimeUnit val="months"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="152839296"/>
+        <c:axId val="164635776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1469,7 +1454,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="153013632"/>
+        <c:crossAx val="164875648"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1492,7 +1477,7 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="4.5828229804607823E-2"/>
-          <c:y val="0.33819556996218503"/>
+          <c:y val="0.33819556996218514"/>
           <c:w val="0.12857154394162268"/>
           <c:h val="0.11669367909238262"/>
         </c:manualLayout>
@@ -1613,7 +1598,7 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="4.4510450248127775E-2"/>
+          <c:x val="4.4510450248127796E-2"/>
           <c:y val="0.10032394165889739"/>
           <c:w val="0.79228601441663349"/>
           <c:h val="0.79935527708863363"/>
@@ -1671,7 +1656,7 @@
                   <c:v>43959</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43972</c:v>
+                  <c:v>43974</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1701,17 +1686,17 @@
                   <c:v>0.22093023255813954</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.39080459770114945</c:v>
+                  <c:v>0.41568627450980394</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="152863104"/>
-        <c:axId val="152864640"/>
+        <c:axId val="164659584"/>
+        <c:axId val="164661120"/>
       </c:areaChart>
       <c:dateAx>
-        <c:axId val="152863104"/>
+        <c:axId val="164659584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1719,13 +1704,13 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="yyyy\/mm\/dd" sourceLinked="1"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="152864640"/>
+        <c:crossAx val="164661120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="152864640"/>
+        <c:axId val="164661120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1768,7 +1753,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="152863104"/>
+        <c:crossAx val="164659584"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1891,7 +1876,7 @@
                   <c:v>43959</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43972</c:v>
+                  <c:v>43974</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1921,7 +1906,7 @@
                   <c:v>201</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>159</c:v>
+                  <c:v>149</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1977,7 +1962,7 @@
                   <c:v>43959</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43972</c:v>
+                  <c:v>43974</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2013,11 +1998,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="152889600"/>
-        <c:axId val="153288704"/>
+        <c:axId val="164686080"/>
+        <c:axId val="165019648"/>
       </c:areaChart>
       <c:dateAx>
-        <c:axId val="152889600"/>
+        <c:axId val="164686080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2050,7 +2035,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="153288704"/>
+        <c:crossAx val="165019648"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -2059,7 +2044,7 @@
         <c:minorTimeUnit val="months"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="153288704"/>
+        <c:axId val="165019648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2101,7 +2086,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="152889600"/>
+        <c:crossAx val="164686080"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2608,10 +2593,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D443"/>
+  <dimension ref="A1:D435"/>
   <sheetViews>
-    <sheetView topLeftCell="A272" workbookViewId="0">
-      <selection activeCell="C321" sqref="C321"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5"/>
@@ -2624,7 +2609,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="18">
       <c r="B1" s="1" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="D1" s="40"/>
     </row>
@@ -2691,7 +2676,7 @@
     </row>
     <row r="11" spans="1:4" s="6" customFormat="1">
       <c r="B11" s="20" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>14</v>
@@ -2700,7 +2685,7 @@
     </row>
     <row r="12" spans="1:4" s="6" customFormat="1">
       <c r="B12" s="22" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>14</v>
@@ -2709,7 +2694,7 @@
     </row>
     <row r="13" spans="1:4" s="6" customFormat="1">
       <c r="B13" s="20" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>14</v>
@@ -2723,7 +2708,7 @@
     </row>
     <row r="15" spans="1:4" s="6" customFormat="1">
       <c r="B15" s="22" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>14</v>
@@ -2732,7 +2717,7 @@
     </row>
     <row r="16" spans="1:4" s="6" customFormat="1">
       <c r="B16" s="22" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>14</v>
@@ -2806,7 +2791,7 @@
     </row>
     <row r="26" spans="2:4" s="6" customFormat="1">
       <c r="B26" s="3" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="C26" s="7"/>
       <c r="D26" s="4"/>
@@ -2818,7 +2803,7 @@
     </row>
     <row r="28" spans="2:4" s="6" customFormat="1">
       <c r="B28" s="22" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C28" s="7" t="s">
         <v>2</v>
@@ -2845,7 +2830,7 @@
     </row>
     <row r="31" spans="2:4" s="6" customFormat="1">
       <c r="B31" s="22" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="C31" s="7" t="s">
         <v>2</v>
@@ -2854,7 +2839,7 @@
     </row>
     <row r="32" spans="2:4" s="6" customFormat="1">
       <c r="B32" s="22" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="C32" s="7" t="s">
         <v>2</v>
@@ -2863,7 +2848,7 @@
     </row>
     <row r="33" spans="2:4" s="6" customFormat="1">
       <c r="B33" s="22" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="C33" s="7" t="s">
         <v>2</v>
@@ -2872,7 +2857,7 @@
     </row>
     <row r="34" spans="2:4" s="6" customFormat="1">
       <c r="B34" s="22" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="C34" s="7" t="s">
         <v>2</v>
@@ -2881,7 +2866,7 @@
     </row>
     <row r="35" spans="2:4" s="6" customFormat="1">
       <c r="B35" s="22" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="C35" s="7" t="s">
         <v>2</v>
@@ -2890,7 +2875,7 @@
     </row>
     <row r="36" spans="2:4">
       <c r="B36" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="C36" s="7" t="s">
         <v>2</v>
@@ -2898,7 +2883,7 @@
     </row>
     <row r="37" spans="2:4">
       <c r="B37" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="C37" s="7" t="s">
         <v>2</v>
@@ -2906,7 +2891,7 @@
     </row>
     <row r="38" spans="2:4">
       <c r="B38" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="C38" s="7" t="s">
         <v>2</v>
@@ -2914,7 +2899,7 @@
     </row>
     <row r="39" spans="2:4">
       <c r="B39" t="s">
-        <v>198</v>
+        <v>243</v>
       </c>
       <c r="C39" s="7" t="s">
         <v>2</v>
@@ -2922,24 +2907,27 @@
     </row>
     <row r="40" spans="2:4">
       <c r="B40" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="C40" s="7" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="2:4" s="6" customFormat="1">
-      <c r="B41" s="22" t="s">
-        <v>208</v>
+    <row r="41" spans="2:4">
+      <c r="B41" t="s">
+        <v>193</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D41" s="4"/>
+        <v>2</v>
+      </c>
     </row>
     <row r="42" spans="2:4" s="6" customFormat="1">
-      <c r="B42" s="22"/>
-      <c r="C42" s="7"/>
+      <c r="B42" s="22" t="s">
+        <v>202</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D42" s="4"/>
     </row>
     <row r="43" spans="2:4" s="6" customFormat="1">
@@ -2958,29 +2946,25 @@
       <c r="D45" s="4"/>
     </row>
     <row r="46" spans="2:4" s="6" customFormat="1">
-      <c r="B46" s="3" t="s">
-        <v>200</v>
-      </c>
+      <c r="B46" s="22"/>
       <c r="C46" s="7"/>
       <c r="D46" s="4"/>
     </row>
     <row r="47" spans="2:4" s="6" customFormat="1">
-      <c r="B47" s="22"/>
+      <c r="B47" s="3" t="s">
+        <v>194</v>
+      </c>
       <c r="C47" s="7"/>
       <c r="D47" s="4"/>
     </row>
     <row r="48" spans="2:4" s="6" customFormat="1">
-      <c r="B48" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="C48" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="B48" s="22"/>
+      <c r="C48" s="7"/>
       <c r="D48" s="4"/>
     </row>
     <row r="49" spans="2:4" s="6" customFormat="1">
       <c r="B49" s="22" t="s">
-        <v>39</v>
+        <v>75</v>
       </c>
       <c r="C49" s="7" t="s">
         <v>14</v>
@@ -2989,7 +2973,7 @@
     </row>
     <row r="50" spans="2:4" s="6" customFormat="1">
       <c r="B50" s="22" t="s">
-        <v>201</v>
+        <v>39</v>
       </c>
       <c r="C50" s="7" t="s">
         <v>14</v>
@@ -2998,25 +2982,25 @@
     </row>
     <row r="51" spans="2:4" s="6" customFormat="1">
       <c r="B51" s="22" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="D51" s="4"/>
     </row>
     <row r="52" spans="2:4" s="6" customFormat="1">
       <c r="B52" s="22" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D52" s="4"/>
     </row>
     <row r="53" spans="2:4" s="6" customFormat="1">
       <c r="B53" s="22" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C53" s="7" t="s">
         <v>14</v>
@@ -3025,16 +3009,16 @@
     </row>
     <row r="54" spans="2:4" s="6" customFormat="1">
       <c r="B54" s="22" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="D54" s="4"/>
     </row>
     <row r="55" spans="2:4" s="6" customFormat="1">
       <c r="B55" s="22" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="C55" s="7" t="s">
         <v>2</v>
@@ -3043,7 +3027,7 @@
     </row>
     <row r="56" spans="2:4" s="6" customFormat="1">
       <c r="B56" s="22" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="C56" s="7" t="s">
         <v>2</v>
@@ -3052,7 +3036,7 @@
     </row>
     <row r="57" spans="2:4" s="6" customFormat="1">
       <c r="B57" s="22" t="s">
-        <v>70</v>
+        <v>201</v>
       </c>
       <c r="C57" s="7" t="s">
         <v>2</v>
@@ -3061,7 +3045,7 @@
     </row>
     <row r="58" spans="2:4" s="6" customFormat="1">
       <c r="B58" s="22" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C58" s="7" t="s">
         <v>2</v>
@@ -3070,7 +3054,7 @@
     </row>
     <row r="59" spans="2:4" s="6" customFormat="1">
       <c r="B59" s="22" t="s">
-        <v>218</v>
+        <v>69</v>
       </c>
       <c r="C59" s="7" t="s">
         <v>2</v>
@@ -3079,7 +3063,7 @@
     </row>
     <row r="60" spans="2:4" s="6" customFormat="1">
       <c r="B60" s="22" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="C60" s="7" t="s">
         <v>2</v>
@@ -3087,31 +3071,31 @@
       <c r="D60" s="4"/>
     </row>
     <row r="61" spans="2:4" s="6" customFormat="1">
-      <c r="B61" s="22"/>
-      <c r="C61" s="7"/>
+      <c r="B61" s="22" t="s">
+        <v>213</v>
+      </c>
+      <c r="C61" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="D61" s="4"/>
     </row>
     <row r="62" spans="2:4" s="6" customFormat="1">
-      <c r="B62" s="22" t="s">
-        <v>122</v>
-      </c>
-      <c r="C62" s="7" t="s">
-        <v>2</v>
-      </c>
+      <c r="B62" s="22"/>
+      <c r="C62" s="7"/>
       <c r="D62" s="4"/>
     </row>
     <row r="63" spans="2:4" s="6" customFormat="1">
       <c r="B63" s="22" t="s">
-        <v>181</v>
+        <v>118</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D63" s="4"/>
     </row>
     <row r="64" spans="2:4" s="6" customFormat="1">
       <c r="B64" s="22" t="s">
-        <v>215</v>
+        <v>175</v>
       </c>
       <c r="C64" s="7" t="s">
         <v>14</v>
@@ -3120,7 +3104,7 @@
     </row>
     <row r="65" spans="2:4" s="6" customFormat="1">
       <c r="B65" s="22" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="C65" s="7" t="s">
         <v>14</v>
@@ -3129,7 +3113,7 @@
     </row>
     <row r="66" spans="2:4" s="6" customFormat="1">
       <c r="B66" s="22" t="s">
-        <v>134</v>
+        <v>210</v>
       </c>
       <c r="C66" s="7" t="s">
         <v>14</v>
@@ -3138,7 +3122,7 @@
     </row>
     <row r="67" spans="2:4" s="6" customFormat="1">
       <c r="B67" s="22" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="C67" s="7" t="s">
         <v>14</v>
@@ -3146,22 +3130,22 @@
       <c r="D67" s="4"/>
     </row>
     <row r="68" spans="2:4" s="6" customFormat="1">
-      <c r="B68" s="22"/>
-      <c r="C68" s="7"/>
+      <c r="B68" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="C68" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D68" s="4"/>
     </row>
     <row r="69" spans="2:4" s="6" customFormat="1">
-      <c r="B69" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="C69" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="B69" s="22"/>
+      <c r="C69" s="7"/>
       <c r="D69" s="4"/>
     </row>
     <row r="70" spans="2:4" s="6" customFormat="1">
       <c r="B70" s="22" t="s">
-        <v>155</v>
+        <v>39</v>
       </c>
       <c r="C70" s="7" t="s">
         <v>14</v>
@@ -3170,7 +3154,7 @@
     </row>
     <row r="71" spans="2:4" s="6" customFormat="1">
       <c r="B71" s="22" t="s">
-        <v>40</v>
+        <v>150</v>
       </c>
       <c r="C71" s="7" t="s">
         <v>14</v>
@@ -3179,53 +3163,53 @@
     </row>
     <row r="72" spans="2:4" s="6" customFormat="1">
       <c r="B72" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="C72" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D72" s="4"/>
+    </row>
+    <row r="73" spans="2:4" s="6" customFormat="1">
+      <c r="B73" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="C72" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D72" s="4"/>
-    </row>
-    <row r="73" spans="2:4" s="6" customFormat="1">
-      <c r="B73" s="22"/>
-      <c r="C73" s="7"/>
+      <c r="C73" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D73" s="4"/>
     </row>
     <row r="74" spans="2:4" s="6" customFormat="1">
-      <c r="B74" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="C74" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="B74" s="22"/>
+      <c r="C74" s="7"/>
       <c r="D74" s="4"/>
     </row>
     <row r="75" spans="2:4" s="6" customFormat="1">
       <c r="B75" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="C75" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D75" s="4"/>
+    </row>
+    <row r="76" spans="2:4" s="6" customFormat="1">
+      <c r="B76" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="C75" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D75" s="4"/>
-    </row>
-    <row r="76" spans="2:4" s="6" customFormat="1">
-      <c r="B76" s="22"/>
-      <c r="C76" s="7"/>
+      <c r="C76" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D76" s="4"/>
     </row>
     <row r="77" spans="2:4" s="6" customFormat="1">
-      <c r="B77" s="22" t="s">
-        <v>138</v>
-      </c>
-      <c r="C77" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="B77" s="22"/>
+      <c r="C77" s="7"/>
       <c r="D77" s="4"/>
     </row>
     <row r="78" spans="2:4" s="6" customFormat="1">
       <c r="B78" s="22" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="C78" s="7" t="s">
         <v>14</v>
@@ -3233,35 +3217,39 @@
       <c r="D78" s="4"/>
     </row>
     <row r="79" spans="2:4" s="6" customFormat="1">
-      <c r="C79" s="7"/>
+      <c r="B79" s="22" t="s">
+        <v>134</v>
+      </c>
+      <c r="C79" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D79" s="4"/>
     </row>
     <row r="80" spans="2:4" s="6" customFormat="1">
-      <c r="B80" s="9" t="s">
+      <c r="C80" s="7"/>
+      <c r="D80" s="4"/>
+    </row>
+    <row r="81" spans="2:4" s="6" customFormat="1">
+      <c r="B81" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="C81" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D81" s="4"/>
+    </row>
+    <row r="82" spans="2:4" s="6" customFormat="1">
+      <c r="B82" s="22"/>
+      <c r="C82" s="7"/>
+      <c r="D82" s="4"/>
+    </row>
+    <row r="83" spans="2:4" s="6" customFormat="1">
+      <c r="B83" s="22" t="s">
         <v>143</v>
       </c>
-      <c r="C80" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D80" s="4"/>
-    </row>
-    <row r="81" spans="2:4" s="6" customFormat="1">
-      <c r="B81" s="22"/>
-      <c r="C81" s="7"/>
-      <c r="D81" s="4"/>
-    </row>
-    <row r="82" spans="2:4" s="6" customFormat="1">
-      <c r="B82" s="22" t="s">
-        <v>148</v>
-      </c>
-      <c r="C82" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D82" s="4"/>
-    </row>
-    <row r="83" spans="2:4" s="6" customFormat="1">
-      <c r="B83" s="22"/>
-      <c r="C83" s="7"/>
+      <c r="C83" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D83" s="4"/>
     </row>
     <row r="84" spans="2:4" s="6" customFormat="1">
@@ -3285,29 +3273,25 @@
       <c r="D87" s="4"/>
     </row>
     <row r="88" spans="2:4" s="6" customFormat="1">
-      <c r="B88" s="3" t="s">
-        <v>209</v>
-      </c>
+      <c r="B88" s="22"/>
       <c r="C88" s="7"/>
       <c r="D88" s="4"/>
     </row>
     <row r="89" spans="2:4" s="6" customFormat="1">
-      <c r="B89" s="22"/>
+      <c r="B89" s="3" t="s">
+        <v>203</v>
+      </c>
       <c r="C89" s="7"/>
       <c r="D89" s="4"/>
     </row>
     <row r="90" spans="2:4" s="6" customFormat="1">
-      <c r="B90" s="22" t="s">
-        <v>166</v>
-      </c>
-      <c r="C90" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="B90" s="22"/>
+      <c r="C90" s="7"/>
       <c r="D90" s="4"/>
     </row>
     <row r="91" spans="2:4" s="6" customFormat="1">
       <c r="B91" s="22" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="C91" s="7" t="s">
         <v>14</v>
@@ -3316,7 +3300,7 @@
     </row>
     <row r="92" spans="2:4" s="6" customFormat="1">
       <c r="B92" s="22" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="C92" s="7" t="s">
         <v>14</v>
@@ -3325,7 +3309,7 @@
     </row>
     <row r="93" spans="2:4" s="6" customFormat="1">
       <c r="B93" s="22" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="C93" s="7" t="s">
         <v>14</v>
@@ -3334,7 +3318,7 @@
     </row>
     <row r="94" spans="2:4" s="6" customFormat="1">
       <c r="B94" s="22" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="C94" s="7" t="s">
         <v>14</v>
@@ -3343,7 +3327,7 @@
     </row>
     <row r="95" spans="2:4" s="6" customFormat="1">
       <c r="B95" s="22" t="s">
-        <v>210</v>
+        <v>165</v>
       </c>
       <c r="C95" s="7" t="s">
         <v>14</v>
@@ -3351,8 +3335,12 @@
       <c r="D95" s="4"/>
     </row>
     <row r="96" spans="2:4" s="6" customFormat="1">
-      <c r="B96" s="22"/>
-      <c r="C96" s="7"/>
+      <c r="B96" s="22" t="s">
+        <v>204</v>
+      </c>
+      <c r="C96" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D96" s="4"/>
     </row>
     <row r="97" spans="2:4" s="6" customFormat="1">
@@ -3401,29 +3389,25 @@
       <c r="D105" s="4"/>
     </row>
     <row r="106" spans="2:4" s="6" customFormat="1">
-      <c r="B106" s="3" t="s">
-        <v>232</v>
-      </c>
+      <c r="B106" s="22"/>
       <c r="C106" s="7"/>
       <c r="D106" s="4"/>
     </row>
     <row r="107" spans="2:4" s="6" customFormat="1">
-      <c r="B107" s="22"/>
+      <c r="B107" s="3" t="s">
+        <v>226</v>
+      </c>
       <c r="C107" s="7"/>
       <c r="D107" s="4"/>
     </row>
     <row r="108" spans="2:4" s="6" customFormat="1">
-      <c r="B108" s="22" t="s">
-        <v>125</v>
-      </c>
-      <c r="C108" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="B108" s="22"/>
+      <c r="C108" s="7"/>
       <c r="D108" s="4"/>
     </row>
     <row r="109" spans="2:4" s="6" customFormat="1">
       <c r="B109" s="22" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C109" s="7" t="s">
         <v>14</v>
@@ -3431,29 +3415,29 @@
       <c r="D109" s="4"/>
     </row>
     <row r="110" spans="2:4" s="6" customFormat="1">
-      <c r="B110" s="22"/>
-      <c r="C110" s="7"/>
+      <c r="B110" s="22" t="s">
+        <v>122</v>
+      </c>
+      <c r="C110" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D110" s="4"/>
     </row>
     <row r="111" spans="2:4" s="6" customFormat="1">
-      <c r="B111" s="27" t="s">
-        <v>236</v>
-      </c>
+      <c r="B111" s="22"/>
       <c r="C111" s="7"/>
       <c r="D111" s="4"/>
     </row>
     <row r="112" spans="2:4" s="6" customFormat="1">
-      <c r="B112" s="20" t="s">
-        <v>233</v>
-      </c>
-      <c r="C112" s="7" t="s">
-        <v>2</v>
-      </c>
+      <c r="B112" s="27" t="s">
+        <v>230</v>
+      </c>
+      <c r="C112" s="7"/>
       <c r="D112" s="4"/>
     </row>
     <row r="113" spans="2:4" s="6" customFormat="1">
-      <c r="B113" s="23" t="s">
-        <v>237</v>
+      <c r="B113" s="20" t="s">
+        <v>227</v>
       </c>
       <c r="C113" s="7" t="s">
         <v>2</v>
@@ -3461,8 +3445,8 @@
       <c r="D113" s="4"/>
     </row>
     <row r="114" spans="2:4" s="6" customFormat="1">
-      <c r="B114" s="20" t="s">
-        <v>234</v>
+      <c r="B114" s="23" t="s">
+        <v>231</v>
       </c>
       <c r="C114" s="7" t="s">
         <v>2</v>
@@ -3470,8 +3454,8 @@
       <c r="D114" s="4"/>
     </row>
     <row r="115" spans="2:4" s="6" customFormat="1">
-      <c r="B115" s="23" t="s">
-        <v>121</v>
+      <c r="B115" s="20" t="s">
+        <v>228</v>
       </c>
       <c r="C115" s="7" t="s">
         <v>2</v>
@@ -3480,7 +3464,7 @@
     </row>
     <row r="116" spans="2:4" s="6" customFormat="1">
       <c r="B116" s="23" t="s">
-        <v>235</v>
+        <v>117</v>
       </c>
       <c r="C116" s="7" t="s">
         <v>2</v>
@@ -3488,22 +3472,22 @@
       <c r="D116" s="4"/>
     </row>
     <row r="117" spans="2:4" s="6" customFormat="1">
-      <c r="B117" s="20"/>
-      <c r="C117" s="7"/>
+      <c r="B117" s="23" t="s">
+        <v>229</v>
+      </c>
+      <c r="C117" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="D117" s="4"/>
     </row>
     <row r="118" spans="2:4" s="6" customFormat="1">
-      <c r="B118" s="22" t="s">
-        <v>145</v>
-      </c>
-      <c r="C118" s="7" t="s">
-        <v>2</v>
-      </c>
+      <c r="B118" s="20"/>
+      <c r="C118" s="7"/>
       <c r="D118" s="4"/>
     </row>
     <row r="119" spans="2:4" s="6" customFormat="1">
-      <c r="B119" s="20" t="s">
-        <v>211</v>
+      <c r="B119" s="22" t="s">
+        <v>140</v>
       </c>
       <c r="C119" s="7" t="s">
         <v>2</v>
@@ -3512,7 +3496,7 @@
     </row>
     <row r="120" spans="2:4" s="6" customFormat="1">
       <c r="B120" s="20" t="s">
-        <v>240</v>
+        <v>205</v>
       </c>
       <c r="C120" s="7" t="s">
         <v>2</v>
@@ -3521,7 +3505,7 @@
     </row>
     <row r="121" spans="2:4" s="6" customFormat="1">
       <c r="B121" s="20" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="C121" s="7" t="s">
         <v>2</v>
@@ -3529,8 +3513,8 @@
       <c r="D121" s="4"/>
     </row>
     <row r="122" spans="2:4" s="6" customFormat="1">
-      <c r="B122" s="23" t="s">
-        <v>239</v>
+      <c r="B122" s="20" t="s">
+        <v>232</v>
       </c>
       <c r="C122" s="7" t="s">
         <v>2</v>
@@ -3538,45 +3522,45 @@
       <c r="D122" s="4"/>
     </row>
     <row r="123" spans="2:4" s="6" customFormat="1">
-      <c r="B123" s="20"/>
-      <c r="C123" s="7"/>
+      <c r="B123" s="23" t="s">
+        <v>233</v>
+      </c>
+      <c r="C123" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="D123" s="4"/>
     </row>
     <row r="124" spans="2:4" s="6" customFormat="1">
-      <c r="B124" s="22" t="s">
-        <v>212</v>
-      </c>
-      <c r="C124" s="7" t="s">
+      <c r="B124" s="20"/>
+      <c r="C124" s="7"/>
+      <c r="D124" s="4"/>
+    </row>
+    <row r="125" spans="2:4" s="6" customFormat="1">
+      <c r="B125" s="22" t="s">
+        <v>206</v>
+      </c>
+      <c r="C125" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D124" s="4"/>
-    </row>
-    <row r="125" spans="2:4" s="6" customFormat="1">
-      <c r="B125" s="22"/>
-      <c r="C125" s="7"/>
       <c r="D125" s="4"/>
     </row>
     <row r="126" spans="2:4" s="6" customFormat="1">
-      <c r="B126" s="22" t="s">
-        <v>150</v>
-      </c>
-      <c r="C126" s="7" t="s">
+      <c r="B126" s="22"/>
+      <c r="C126" s="7"/>
+      <c r="D126" s="4"/>
+    </row>
+    <row r="127" spans="2:4" s="6" customFormat="1">
+      <c r="B127" s="22" t="s">
+        <v>145</v>
+      </c>
+      <c r="C127" s="7" t="s">
         <v>2</v>
-      </c>
-      <c r="D126" s="4"/>
-    </row>
-    <row r="127" spans="2:4" s="6" customFormat="1">
-      <c r="B127" s="20" t="s">
-        <v>151</v>
-      </c>
-      <c r="C127" s="7" t="s">
-        <v>14</v>
       </c>
       <c r="D127" s="4"/>
     </row>
     <row r="128" spans="2:4" s="6" customFormat="1">
       <c r="B128" s="20" t="s">
-        <v>175</v>
+        <v>146</v>
       </c>
       <c r="C128" s="7" t="s">
         <v>14</v>
@@ -3584,22 +3568,22 @@
       <c r="D128" s="4"/>
     </row>
     <row r="129" spans="2:4" s="6" customFormat="1">
-      <c r="B129" s="22"/>
-      <c r="C129" s="7"/>
+      <c r="B129" s="20" t="s">
+        <v>169</v>
+      </c>
+      <c r="C129" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D129" s="4"/>
     </row>
     <row r="130" spans="2:4" s="6" customFormat="1">
-      <c r="B130" s="22" t="s">
-        <v>83</v>
-      </c>
-      <c r="C130" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="B130" s="22"/>
+      <c r="C130" s="7"/>
       <c r="D130" s="4"/>
     </row>
     <row r="131" spans="2:4" s="6" customFormat="1">
       <c r="B131" s="22" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C131" s="7" t="s">
         <v>14</v>
@@ -3608,44 +3592,44 @@
     </row>
     <row r="132" spans="2:4" s="6" customFormat="1">
       <c r="B132" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="C132" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D132" s="4"/>
+    </row>
+    <row r="133" spans="2:4" s="6" customFormat="1">
+      <c r="B133" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="C132" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D132" s="4"/>
-    </row>
-    <row r="133" spans="2:4" s="6" customFormat="1">
-      <c r="B133" s="22"/>
-      <c r="C133" s="7"/>
+      <c r="C133" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D133" s="4"/>
     </row>
     <row r="134" spans="2:4" s="6" customFormat="1">
-      <c r="B134" s="22" t="s">
-        <v>213</v>
-      </c>
-      <c r="C134" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="B134" s="22"/>
+      <c r="C134" s="7"/>
       <c r="D134" s="4"/>
     </row>
     <row r="135" spans="2:4" s="6" customFormat="1">
-      <c r="B135" s="22"/>
-      <c r="C135" s="7"/>
+      <c r="B135" s="22" t="s">
+        <v>207</v>
+      </c>
+      <c r="C135" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D135" s="4"/>
     </row>
     <row r="136" spans="2:4" s="6" customFormat="1">
-      <c r="B136" s="27" t="s">
-        <v>169</v>
-      </c>
-      <c r="C136" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="B136" s="22"/>
+      <c r="C136" s="7"/>
       <c r="D136" s="4"/>
     </row>
     <row r="137" spans="2:4" s="6" customFormat="1">
-      <c r="B137" s="20" t="s">
-        <v>119</v>
+      <c r="B137" s="27" t="s">
+        <v>164</v>
       </c>
       <c r="C137" s="7" t="s">
         <v>14</v>
@@ -3654,7 +3638,7 @@
     </row>
     <row r="138" spans="2:4" s="6" customFormat="1">
       <c r="B138" s="20" t="s">
-        <v>165</v>
+        <v>115</v>
       </c>
       <c r="C138" s="7" t="s">
         <v>14</v>
@@ -3662,22 +3646,22 @@
       <c r="D138" s="4"/>
     </row>
     <row r="139" spans="2:4" s="6" customFormat="1">
-      <c r="B139" s="20"/>
-      <c r="C139" s="7"/>
+      <c r="B139" s="20" t="s">
+        <v>160</v>
+      </c>
+      <c r="C139" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D139" s="4"/>
     </row>
     <row r="140" spans="2:4" s="6" customFormat="1">
-      <c r="B140" s="27" t="s">
+      <c r="B140" s="20"/>
+      <c r="C140" s="7"/>
+      <c r="D140" s="4"/>
+    </row>
+    <row r="141" spans="2:4" s="6" customFormat="1">
+      <c r="B141" s="27" t="s">
         <v>26</v>
-      </c>
-      <c r="C140" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D140" s="4"/>
-    </row>
-    <row r="141" spans="2:4" s="6" customFormat="1">
-      <c r="B141" s="20" t="s">
-        <v>124</v>
       </c>
       <c r="C141" s="7" t="s">
         <v>2</v>
@@ -3686,7 +3670,7 @@
     </row>
     <row r="142" spans="2:4" s="6" customFormat="1">
       <c r="B142" s="20" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C142" s="7" t="s">
         <v>2</v>
@@ -3695,7 +3679,7 @@
     </row>
     <row r="143" spans="2:4" s="6" customFormat="1">
       <c r="B143" s="20" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="C143" s="7" t="s">
         <v>2</v>
@@ -3704,7 +3688,7 @@
     </row>
     <row r="144" spans="2:4" s="6" customFormat="1">
       <c r="B144" s="20" t="s">
-        <v>182</v>
+        <v>126</v>
       </c>
       <c r="C144" s="7" t="s">
         <v>2</v>
@@ -3712,22 +3696,22 @@
       <c r="D144" s="4"/>
     </row>
     <row r="145" spans="2:4" s="6" customFormat="1">
-      <c r="B145" s="22"/>
-      <c r="C145" s="7"/>
+      <c r="B145" s="20" t="s">
+        <v>176</v>
+      </c>
+      <c r="C145" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="D145" s="4"/>
     </row>
     <row r="146" spans="2:4" s="6" customFormat="1">
-      <c r="B146" s="27" t="s">
+      <c r="B146" s="22"/>
+      <c r="C146" s="7"/>
+      <c r="D146" s="4"/>
+    </row>
+    <row r="147" spans="2:4" s="6" customFormat="1">
+      <c r="B147" s="27" t="s">
         <v>25</v>
-      </c>
-      <c r="C146" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D146" s="4"/>
-    </row>
-    <row r="147" spans="2:4" s="6" customFormat="1">
-      <c r="B147" s="20" t="s">
-        <v>152</v>
       </c>
       <c r="C147" s="7" t="s">
         <v>14</v>
@@ -3736,7 +3720,7 @@
     </row>
     <row r="148" spans="2:4" s="6" customFormat="1">
       <c r="B148" s="20" t="s">
-        <v>26</v>
+        <v>147</v>
       </c>
       <c r="C148" s="7" t="s">
         <v>14</v>
@@ -3745,7 +3729,7 @@
     </row>
     <row r="149" spans="2:4" s="6" customFormat="1">
       <c r="B149" s="20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C149" s="7" t="s">
         <v>14</v>
@@ -3754,7 +3738,7 @@
     </row>
     <row r="150" spans="2:4" s="6" customFormat="1">
       <c r="B150" s="20" t="s">
-        <v>153</v>
+        <v>27</v>
       </c>
       <c r="C150" s="7" t="s">
         <v>14</v>
@@ -3762,22 +3746,22 @@
       <c r="D150" s="4"/>
     </row>
     <row r="151" spans="2:4" s="6" customFormat="1">
-      <c r="B151" s="22"/>
-      <c r="C151" s="7"/>
+      <c r="B151" s="20" t="s">
+        <v>148</v>
+      </c>
+      <c r="C151" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D151" s="4"/>
     </row>
     <row r="152" spans="2:4" s="6" customFormat="1">
-      <c r="B152" s="27" t="s">
+      <c r="B152" s="22"/>
+      <c r="C152" s="7"/>
+      <c r="D152" s="4"/>
+    </row>
+    <row r="153" spans="2:4" s="6" customFormat="1">
+      <c r="B153" s="27" t="s">
         <v>29</v>
-      </c>
-      <c r="C152" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D152" s="4"/>
-    </row>
-    <row r="153" spans="2:4" s="6" customFormat="1">
-      <c r="B153" s="20" t="s">
-        <v>32</v>
       </c>
       <c r="C153" s="7" t="s">
         <v>2</v>
@@ -3786,25 +3770,25 @@
     </row>
     <row r="154" spans="2:4" s="6" customFormat="1">
       <c r="B154" s="20" t="s">
-        <v>170</v>
+        <v>32</v>
       </c>
       <c r="C154" s="7" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D154" s="4"/>
     </row>
     <row r="155" spans="2:4" s="6" customFormat="1">
       <c r="B155" s="20" t="s">
-        <v>47</v>
+        <v>165</v>
       </c>
       <c r="C155" s="7" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="D155" s="4"/>
     </row>
     <row r="156" spans="2:4" s="6" customFormat="1">
       <c r="B156" s="20" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C156" s="7" t="s">
         <v>2</v>
@@ -3813,7 +3797,7 @@
     </row>
     <row r="157" spans="2:4" s="6" customFormat="1">
       <c r="B157" s="20" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C157" s="7" t="s">
         <v>2</v>
@@ -3822,7 +3806,7 @@
     </row>
     <row r="158" spans="2:4" s="6" customFormat="1">
       <c r="B158" s="20" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C158" s="7" t="s">
         <v>2</v>
@@ -3831,7 +3815,7 @@
     </row>
     <row r="159" spans="2:4" s="6" customFormat="1">
       <c r="B159" s="20" t="s">
-        <v>248</v>
+        <v>50</v>
       </c>
       <c r="C159" s="7" t="s">
         <v>2</v>
@@ -3840,7 +3824,7 @@
     </row>
     <row r="160" spans="2:4" s="6" customFormat="1">
       <c r="B160" s="20" t="s">
-        <v>154</v>
+        <v>242</v>
       </c>
       <c r="C160" s="7" t="s">
         <v>2</v>
@@ -3848,22 +3832,22 @@
       <c r="D160" s="4"/>
     </row>
     <row r="161" spans="2:4" s="6" customFormat="1">
-      <c r="B161" s="20"/>
-      <c r="C161" s="9"/>
+      <c r="B161" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="C161" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="D161" s="4"/>
     </row>
     <row r="162" spans="2:4" s="6" customFormat="1">
-      <c r="B162" s="27" t="s">
+      <c r="B162" s="20"/>
+      <c r="C162" s="9"/>
+      <c r="D162" s="4"/>
+    </row>
+    <row r="163" spans="2:4" s="6" customFormat="1">
+      <c r="B163" s="27" t="s">
         <v>30</v>
-      </c>
-      <c r="C162" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D162" s="4"/>
-    </row>
-    <row r="163" spans="2:4" s="6" customFormat="1">
-      <c r="B163" s="20" t="s">
-        <v>31</v>
       </c>
       <c r="C163" s="7" t="s">
         <v>2</v>
@@ -3872,7 +3856,7 @@
     </row>
     <row r="164" spans="2:4" s="6" customFormat="1">
       <c r="B164" s="20" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="C164" s="7" t="s">
         <v>2</v>
@@ -3881,7 +3865,7 @@
     </row>
     <row r="165" spans="2:4" s="6" customFormat="1">
       <c r="B165" s="20" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C165" s="7" t="s">
         <v>2</v>
@@ -3890,7 +3874,7 @@
     </row>
     <row r="166" spans="2:4" s="6" customFormat="1">
       <c r="B166" s="20" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C166" s="7" t="s">
         <v>2</v>
@@ -3899,7 +3883,7 @@
     </row>
     <row r="167" spans="2:4" s="6" customFormat="1">
       <c r="B167" s="20" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C167" s="7" t="s">
         <v>2</v>
@@ -3908,7 +3892,7 @@
     </row>
     <row r="168" spans="2:4" s="6" customFormat="1">
       <c r="B168" s="20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C168" s="7" t="s">
         <v>2</v>
@@ -3916,8 +3900,12 @@
       <c r="D168" s="4"/>
     </row>
     <row r="169" spans="2:4" s="6" customFormat="1">
-      <c r="B169" s="22"/>
-      <c r="C169" s="7"/>
+      <c r="B169" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="C169" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="D169" s="4"/>
     </row>
     <row r="170" spans="2:4" s="6" customFormat="1">
@@ -3946,54 +3934,52 @@
       <c r="D174" s="4"/>
     </row>
     <row r="175" spans="2:4" s="6" customFormat="1">
-      <c r="B175" s="3" t="s">
-        <v>21</v>
-      </c>
+      <c r="B175" s="22"/>
       <c r="C175" s="7"/>
       <c r="D175" s="4"/>
     </row>
     <row r="176" spans="2:4" s="6" customFormat="1">
-      <c r="B176" s="22"/>
+      <c r="B176" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="C176" s="7"/>
       <c r="D176" s="4"/>
     </row>
     <row r="177" spans="2:4" s="6" customFormat="1">
-      <c r="B177" s="22" t="s">
-        <v>97</v>
-      </c>
+      <c r="B177" s="22"/>
       <c r="C177" s="7"/>
       <c r="D177" s="4"/>
     </row>
     <row r="178" spans="2:4" s="6" customFormat="1">
-      <c r="B178" s="20" t="s">
-        <v>98</v>
+      <c r="B178" s="27" t="s">
+        <v>43</v>
       </c>
       <c r="C178" s="7" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D178" s="4"/>
     </row>
     <row r="179" spans="2:4" s="6" customFormat="1">
       <c r="B179" s="20" t="s">
-        <v>99</v>
+        <v>43</v>
       </c>
       <c r="C179" s="7" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D179" s="4"/>
     </row>
     <row r="180" spans="2:4" s="6" customFormat="1">
-      <c r="B180" s="20" t="s">
-        <v>100</v>
+      <c r="B180" s="23" t="s">
+        <v>42</v>
       </c>
       <c r="C180" s="7" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D180" s="4"/>
     </row>
     <row r="181" spans="2:4" s="6" customFormat="1">
-      <c r="B181" s="20" t="s">
-        <v>171</v>
+      <c r="B181" s="23" t="s">
+        <v>166</v>
       </c>
       <c r="C181" s="7" t="s">
         <v>14</v>
@@ -4001,22 +3987,26 @@
       <c r="D181" s="4"/>
     </row>
     <row r="182" spans="2:4" s="6" customFormat="1">
-      <c r="B182" s="22"/>
-      <c r="C182" s="7"/>
+      <c r="B182" s="20" t="s">
+        <v>127</v>
+      </c>
+      <c r="C182" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D182" s="4"/>
     </row>
     <row r="183" spans="2:4" s="6" customFormat="1">
-      <c r="B183" s="27" t="s">
-        <v>43</v>
+      <c r="B183" s="23" t="s">
+        <v>128</v>
       </c>
       <c r="C183" s="7" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="D183" s="4"/>
     </row>
     <row r="184" spans="2:4" s="6" customFormat="1">
       <c r="B184" s="20" t="s">
-        <v>43</v>
+        <v>235</v>
       </c>
       <c r="C184" s="7" t="s">
         <v>2</v>
@@ -4025,7 +4015,7 @@
     </row>
     <row r="185" spans="2:4" s="6" customFormat="1">
       <c r="B185" s="23" t="s">
-        <v>42</v>
+        <v>236</v>
       </c>
       <c r="C185" s="7" t="s">
         <v>2</v>
@@ -4033,44 +4023,36 @@
       <c r="D185" s="4"/>
     </row>
     <row r="186" spans="2:4" s="6" customFormat="1">
-      <c r="B186" s="23" t="s">
-        <v>172</v>
-      </c>
-      <c r="C186" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="B186" s="20"/>
+      <c r="C186" s="7"/>
       <c r="D186" s="4"/>
     </row>
     <row r="187" spans="2:4" s="6" customFormat="1">
       <c r="B187" s="20" t="s">
-        <v>132</v>
+        <v>46</v>
       </c>
       <c r="C187" s="7" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D187" s="4"/>
     </row>
     <row r="188" spans="2:4" s="6" customFormat="1">
       <c r="B188" s="23" t="s">
-        <v>133</v>
+        <v>167</v>
       </c>
       <c r="C188" s="7" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D188" s="4"/>
     </row>
     <row r="189" spans="2:4" s="6" customFormat="1">
-      <c r="B189" s="20" t="s">
-        <v>241</v>
-      </c>
-      <c r="C189" s="7" t="s">
-        <v>2</v>
-      </c>
+      <c r="B189" s="22"/>
+      <c r="C189" s="7"/>
       <c r="D189" s="4"/>
     </row>
     <row r="190" spans="2:4" s="6" customFormat="1">
-      <c r="B190" s="23" t="s">
-        <v>242</v>
+      <c r="B190" s="20" t="s">
+        <v>53</v>
       </c>
       <c r="C190" s="7" t="s">
         <v>2</v>
@@ -4078,22 +4060,22 @@
       <c r="D190" s="4"/>
     </row>
     <row r="191" spans="2:4" s="6" customFormat="1">
-      <c r="B191" s="20"/>
-      <c r="C191" s="7"/>
+      <c r="B191" s="23" t="s">
+        <v>237</v>
+      </c>
+      <c r="C191" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="D191" s="4"/>
     </row>
     <row r="192" spans="2:4" s="6" customFormat="1">
-      <c r="B192" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="C192" s="7" t="s">
-        <v>2</v>
-      </c>
+      <c r="B192" s="20"/>
+      <c r="C192" s="7"/>
       <c r="D192" s="4"/>
     </row>
     <row r="193" spans="2:4" s="6" customFormat="1">
-      <c r="B193" s="23" t="s">
-        <v>173</v>
+      <c r="B193" s="20" t="s">
+        <v>54</v>
       </c>
       <c r="C193" s="7" t="s">
         <v>2</v>
@@ -4101,36 +4083,40 @@
       <c r="D193" s="4"/>
     </row>
     <row r="194" spans="2:4" s="6" customFormat="1">
-      <c r="B194" s="22"/>
-      <c r="C194" s="7"/>
+      <c r="B194" s="23" t="s">
+        <v>238</v>
+      </c>
+      <c r="C194" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="D194" s="4"/>
     </row>
     <row r="195" spans="2:4" s="6" customFormat="1">
-      <c r="B195" s="20" t="s">
-        <v>53</v>
+      <c r="B195" s="23" t="s">
+        <v>123</v>
       </c>
       <c r="C195" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D195" s="4"/>
+    </row>
+    <row r="196" spans="2:4" s="6" customFormat="1">
+      <c r="B196" s="22"/>
+      <c r="C196" s="7"/>
+      <c r="D196" s="4"/>
+    </row>
+    <row r="197" spans="2:4" s="6" customFormat="1">
+      <c r="B197" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="C197" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D195" s="4"/>
-    </row>
-    <row r="196" spans="2:4" s="6" customFormat="1">
-      <c r="B196" s="23" t="s">
-        <v>243</v>
-      </c>
-      <c r="C196" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D196" s="4"/>
-    </row>
-    <row r="197" spans="2:4" s="6" customFormat="1">
-      <c r="B197" s="20"/>
-      <c r="C197" s="7"/>
       <c r="D197" s="4"/>
     </row>
     <row r="198" spans="2:4" s="6" customFormat="1">
-      <c r="B198" s="20" t="s">
-        <v>54</v>
+      <c r="B198" s="23" t="s">
+        <v>61</v>
       </c>
       <c r="C198" s="7" t="s">
         <v>2</v>
@@ -4139,30 +4125,30 @@
     </row>
     <row r="199" spans="2:4" s="6" customFormat="1">
       <c r="B199" s="23" t="s">
-        <v>244</v>
+        <v>123</v>
       </c>
       <c r="C199" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D199" s="4"/>
+    </row>
+    <row r="200" spans="2:4" s="6" customFormat="1">
+      <c r="B200" s="22"/>
+      <c r="C200" s="7"/>
+      <c r="D200" s="4"/>
+    </row>
+    <row r="201" spans="2:4" s="6" customFormat="1">
+      <c r="B201" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="C201" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D199" s="4"/>
-    </row>
-    <row r="200" spans="2:4" s="6" customFormat="1">
-      <c r="B200" s="23" t="s">
-        <v>127</v>
-      </c>
-      <c r="C200" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D200" s="4"/>
-    </row>
-    <row r="201" spans="2:4" s="6" customFormat="1">
-      <c r="B201" s="22"/>
-      <c r="C201" s="7"/>
       <c r="D201" s="4"/>
     </row>
     <row r="202" spans="2:4" s="6" customFormat="1">
-      <c r="B202" s="20" t="s">
-        <v>57</v>
+      <c r="B202" s="23" t="s">
+        <v>238</v>
       </c>
       <c r="C202" s="7" t="s">
         <v>2</v>
@@ -4170,20 +4156,16 @@
       <c r="D202" s="4"/>
     </row>
     <row r="203" spans="2:4" s="6" customFormat="1">
-      <c r="B203" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="C203" s="7" t="s">
+      <c r="B203" s="22"/>
+      <c r="C203" s="7"/>
+      <c r="D203" s="4"/>
+    </row>
+    <row r="204" spans="2:4" s="6" customFormat="1">
+      <c r="B204" s="20" t="s">
+        <v>173</v>
+      </c>
+      <c r="C204" s="7" t="s">
         <v>2</v>
-      </c>
-      <c r="D203" s="4"/>
-    </row>
-    <row r="204" spans="2:4" s="6" customFormat="1">
-      <c r="B204" s="23" t="s">
-        <v>127</v>
-      </c>
-      <c r="C204" s="7" t="s">
-        <v>14</v>
       </c>
       <c r="D204" s="4"/>
     </row>
@@ -4194,69 +4176,73 @@
     </row>
     <row r="206" spans="2:4" s="6" customFormat="1">
       <c r="B206" s="20" t="s">
-        <v>59</v>
+        <v>97</v>
       </c>
       <c r="C206" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D206" s="4"/>
+        <v>14</v>
+      </c>
+      <c r="D206" s="7" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="207" spans="2:4" s="6" customFormat="1">
       <c r="B207" s="23" t="s">
-        <v>244</v>
+        <v>98</v>
       </c>
       <c r="C207" s="7" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="D207" s="4"/>
     </row>
     <row r="208" spans="2:4" s="6" customFormat="1">
-      <c r="B208" s="22"/>
+      <c r="B208" s="20"/>
       <c r="C208" s="7"/>
       <c r="D208" s="4"/>
     </row>
     <row r="209" spans="2:4" s="6" customFormat="1">
       <c r="B209" s="20" t="s">
-        <v>179</v>
+        <v>99</v>
       </c>
       <c r="C209" s="7" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="D209" s="4"/>
     </row>
     <row r="210" spans="2:4" s="6" customFormat="1">
-      <c r="B210" s="22"/>
-      <c r="C210" s="7"/>
+      <c r="B210" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="C210" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D210" s="4"/>
     </row>
     <row r="211" spans="2:4" s="6" customFormat="1">
-      <c r="B211" s="20" t="s">
+      <c r="B211" s="23" t="s">
         <v>101</v>
       </c>
       <c r="C211" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D211" s="7" t="s">
-        <v>245</v>
-      </c>
+      <c r="D211" s="4"/>
     </row>
     <row r="212" spans="2:4" s="6" customFormat="1">
-      <c r="B212" s="23" t="s">
-        <v>102</v>
-      </c>
-      <c r="C212" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="B212" s="22"/>
+      <c r="C212" s="7"/>
       <c r="D212" s="4"/>
     </row>
     <row r="213" spans="2:4" s="6" customFormat="1">
-      <c r="B213" s="20"/>
-      <c r="C213" s="7"/>
+      <c r="B213" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="C213" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D213" s="4"/>
     </row>
     <row r="214" spans="2:4" s="6" customFormat="1">
-      <c r="B214" s="20" t="s">
-        <v>103</v>
+      <c r="B214" s="23" t="s">
+        <v>42</v>
       </c>
       <c r="C214" s="7" t="s">
         <v>14</v>
@@ -4273,22 +4259,22 @@
       <c r="D215" s="4"/>
     </row>
     <row r="216" spans="2:4" s="6" customFormat="1">
-      <c r="B216" s="23" t="s">
+      <c r="B216" s="20"/>
+      <c r="C216" s="7"/>
+      <c r="D216" s="4"/>
+    </row>
+    <row r="217" spans="2:4" s="6" customFormat="1">
+      <c r="B217" s="20" t="s">
         <v>105</v>
       </c>
-      <c r="C216" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D216" s="4"/>
-    </row>
-    <row r="217" spans="2:4" s="6" customFormat="1">
-      <c r="B217" s="22"/>
-      <c r="C217" s="7"/>
+      <c r="C217" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D217" s="4"/>
     </row>
     <row r="218" spans="2:4" s="6" customFormat="1">
-      <c r="B218" s="20" t="s">
-        <v>107</v>
+      <c r="B218" s="23" t="s">
+        <v>42</v>
       </c>
       <c r="C218" s="7" t="s">
         <v>14</v>
@@ -4297,7 +4283,7 @@
     </row>
     <row r="219" spans="2:4" s="6" customFormat="1">
       <c r="B219" s="23" t="s">
-        <v>42</v>
+        <v>104</v>
       </c>
       <c r="C219" s="7" t="s">
         <v>14</v>
@@ -4305,22 +4291,22 @@
       <c r="D219" s="4"/>
     </row>
     <row r="220" spans="2:4" s="6" customFormat="1">
-      <c r="B220" s="23" t="s">
-        <v>108</v>
-      </c>
-      <c r="C220" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="B220" s="20"/>
+      <c r="C220" s="7"/>
       <c r="D220" s="4"/>
     </row>
     <row r="221" spans="2:4" s="6" customFormat="1">
-      <c r="B221" s="20"/>
-      <c r="C221" s="7"/>
+      <c r="B221" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="C221" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D221" s="4"/>
     </row>
     <row r="222" spans="2:4" s="6" customFormat="1">
-      <c r="B222" s="20" t="s">
-        <v>109</v>
+      <c r="B222" s="23" t="s">
+        <v>107</v>
       </c>
       <c r="C222" s="7" t="s">
         <v>14</v>
@@ -4329,7 +4315,7 @@
     </row>
     <row r="223" spans="2:4" s="6" customFormat="1">
       <c r="B223" s="23" t="s">
-        <v>42</v>
+        <v>101</v>
       </c>
       <c r="C223" s="7" t="s">
         <v>14</v>
@@ -4337,40 +4323,34 @@
       <c r="D223" s="4"/>
     </row>
     <row r="224" spans="2:4" s="6" customFormat="1">
-      <c r="B224" s="23" t="s">
-        <v>108</v>
-      </c>
-      <c r="C224" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="B224" s="23"/>
+      <c r="C224" s="7"/>
       <c r="D224" s="4"/>
     </row>
     <row r="225" spans="2:4" s="6" customFormat="1">
-      <c r="B225" s="20"/>
-      <c r="C225" s="7"/>
+      <c r="B225" s="20" t="s">
+        <v>102</v>
+      </c>
+      <c r="C225" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="D225" s="4"/>
     </row>
     <row r="226" spans="2:4" s="6" customFormat="1">
-      <c r="B226" s="20" t="s">
-        <v>110</v>
-      </c>
-      <c r="C226" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="B226" s="20"/>
+      <c r="C226" s="7"/>
       <c r="D226" s="4"/>
     </row>
     <row r="227" spans="2:4" s="6" customFormat="1">
-      <c r="B227" s="23" t="s">
-        <v>111</v>
-      </c>
-      <c r="C227" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="B227" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="C227" s="7"/>
       <c r="D227" s="4"/>
     </row>
     <row r="228" spans="2:4" s="6" customFormat="1">
-      <c r="B228" s="23" t="s">
-        <v>105</v>
+      <c r="B228" s="20" t="s">
+        <v>44</v>
       </c>
       <c r="C228" s="7" t="s">
         <v>14</v>
@@ -4378,61 +4358,63 @@
       <c r="D228" s="4"/>
     </row>
     <row r="229" spans="2:4" s="6" customFormat="1">
-      <c r="B229" s="23"/>
-      <c r="C229" s="7"/>
+      <c r="B229" s="23" t="s">
+        <v>240</v>
+      </c>
+      <c r="C229" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D229" s="4"/>
     </row>
     <row r="230" spans="2:4" s="6" customFormat="1">
-      <c r="B230" s="20" t="s">
-        <v>106</v>
+      <c r="B230" s="23" t="s">
+        <v>45</v>
       </c>
       <c r="C230" s="7" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="D230" s="4"/>
     </row>
     <row r="231" spans="2:4" s="6" customFormat="1">
-      <c r="B231" s="20"/>
-      <c r="C231" s="7"/>
+      <c r="B231" s="20" t="s">
+        <v>168</v>
+      </c>
+      <c r="C231" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D231" s="4"/>
     </row>
     <row r="232" spans="2:4" s="6" customFormat="1">
-      <c r="B232" s="27" t="s">
-        <v>44</v>
-      </c>
+      <c r="B232" s="22"/>
       <c r="C232" s="7"/>
       <c r="D232" s="4"/>
     </row>
     <row r="233" spans="2:4" s="6" customFormat="1">
       <c r="B233" s="20" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="C233" s="7" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D233" s="4"/>
     </row>
     <row r="234" spans="2:4" s="6" customFormat="1">
       <c r="B234" s="23" t="s">
-        <v>246</v>
+        <v>56</v>
       </c>
       <c r="C234" s="7" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D234" s="4"/>
     </row>
     <row r="235" spans="2:4" s="6" customFormat="1">
-      <c r="B235" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="C235" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="B235" s="22"/>
+      <c r="C235" s="7"/>
       <c r="D235" s="4"/>
     </row>
     <row r="236" spans="2:4" s="6" customFormat="1">
       <c r="B236" s="20" t="s">
-        <v>174</v>
+        <v>58</v>
       </c>
       <c r="C236" s="7" t="s">
         <v>14</v>
@@ -4440,45 +4422,45 @@
       <c r="D236" s="4"/>
     </row>
     <row r="237" spans="2:4" s="6" customFormat="1">
-      <c r="B237" s="22"/>
-      <c r="C237" s="7"/>
+      <c r="B237" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="C237" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D237" s="4"/>
     </row>
     <row r="238" spans="2:4" s="6" customFormat="1">
-      <c r="B238" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="C238" s="7" t="s">
-        <v>2</v>
-      </c>
+      <c r="B238" s="22"/>
+      <c r="C238" s="7"/>
       <c r="D238" s="4"/>
     </row>
     <row r="239" spans="2:4" s="6" customFormat="1">
-      <c r="B239" s="23" t="s">
+      <c r="B239" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="C239" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D239" s="4"/>
+    </row>
+    <row r="240" spans="2:4" s="6" customFormat="1">
+      <c r="B240" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="C239" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D239" s="4"/>
-    </row>
-    <row r="240" spans="2:4" s="6" customFormat="1">
-      <c r="B240" s="22"/>
-      <c r="C240" s="7"/>
+      <c r="C240" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D240" s="4"/>
     </row>
     <row r="241" spans="2:4" s="6" customFormat="1">
-      <c r="B241" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="C241" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="B241" s="20"/>
+      <c r="C241" s="7"/>
       <c r="D241" s="4"/>
     </row>
     <row r="242" spans="2:4" s="6" customFormat="1">
-      <c r="B242" s="23" t="s">
-        <v>56</v>
+      <c r="B242" s="27" t="s">
+        <v>170</v>
       </c>
       <c r="C242" s="7" t="s">
         <v>14</v>
@@ -4486,13 +4468,17 @@
       <c r="D242" s="4"/>
     </row>
     <row r="243" spans="2:4" s="6" customFormat="1">
-      <c r="B243" s="22"/>
-      <c r="C243" s="7"/>
+      <c r="B243" s="20" t="s">
+        <v>171</v>
+      </c>
+      <c r="C243" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D243" s="4"/>
     </row>
     <row r="244" spans="2:4" s="6" customFormat="1">
       <c r="B244" s="20" t="s">
-        <v>60</v>
+        <v>174</v>
       </c>
       <c r="C244" s="7" t="s">
         <v>14</v>
@@ -4500,8 +4486,8 @@
       <c r="D244" s="4"/>
     </row>
     <row r="245" spans="2:4" s="6" customFormat="1">
-      <c r="B245" s="23" t="s">
-        <v>56</v>
+      <c r="B245" s="20" t="s">
+        <v>172</v>
       </c>
       <c r="C245" s="7" t="s">
         <v>14</v>
@@ -4515,75 +4501,61 @@
     </row>
     <row r="247" spans="2:4" s="6" customFormat="1">
       <c r="B247" s="27" t="s">
-        <v>176</v>
+        <v>108</v>
       </c>
       <c r="C247" s="7" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D247" s="4"/>
     </row>
     <row r="248" spans="2:4" s="6" customFormat="1">
       <c r="B248" s="20" t="s">
-        <v>177</v>
+        <v>124</v>
       </c>
       <c r="C248" s="7" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D248" s="4"/>
     </row>
     <row r="249" spans="2:4" s="6" customFormat="1">
       <c r="B249" s="20" t="s">
-        <v>180</v>
+        <v>125</v>
       </c>
       <c r="C249" s="7" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D249" s="4"/>
     </row>
     <row r="250" spans="2:4" s="6" customFormat="1">
-      <c r="B250" s="20" t="s">
-        <v>178</v>
-      </c>
-      <c r="C250" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="B250" s="22"/>
+      <c r="C250" s="7"/>
       <c r="D250" s="4"/>
     </row>
     <row r="251" spans="2:4" s="6" customFormat="1">
-      <c r="B251" s="20"/>
+      <c r="B251" s="22"/>
       <c r="C251" s="7"/>
       <c r="D251" s="4"/>
     </row>
     <row r="252" spans="2:4" s="6" customFormat="1">
-      <c r="B252" s="27" t="s">
-        <v>112</v>
-      </c>
-      <c r="C252" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="B252" s="22"/>
+      <c r="C252" s="7"/>
       <c r="D252" s="4"/>
     </row>
     <row r="253" spans="2:4" s="6" customFormat="1">
-      <c r="B253" s="20" t="s">
-        <v>128</v>
-      </c>
-      <c r="C253" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="B253" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C253" s="7"/>
       <c r="D253" s="4"/>
     </row>
     <row r="254" spans="2:4" s="6" customFormat="1">
-      <c r="B254" s="20" t="s">
-        <v>129</v>
-      </c>
-      <c r="C254" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="B254" s="22"/>
+      <c r="C254" s="7"/>
       <c r="D254" s="4"/>
     </row>
     <row r="255" spans="2:4" s="6" customFormat="1">
       <c r="B255" s="22" t="s">
-        <v>130</v>
+        <v>71</v>
       </c>
       <c r="C255" s="7" t="s">
         <v>14</v>
@@ -4592,7 +4564,7 @@
     </row>
     <row r="256" spans="2:4" s="6" customFormat="1">
       <c r="B256" s="20" t="s">
-        <v>69</v>
+        <v>219</v>
       </c>
       <c r="C256" s="7" t="s">
         <v>14</v>
@@ -4601,7 +4573,7 @@
     </row>
     <row r="257" spans="2:4" s="6" customFormat="1">
       <c r="B257" s="20" t="s">
-        <v>70</v>
+        <v>220</v>
       </c>
       <c r="C257" s="7" t="s">
         <v>14</v>
@@ -4609,35 +4581,49 @@
       <c r="D257" s="4"/>
     </row>
     <row r="258" spans="2:4" s="6" customFormat="1">
-      <c r="B258" s="22"/>
-      <c r="C258" s="7"/>
+      <c r="B258" s="20" t="s">
+        <v>221</v>
+      </c>
+      <c r="C258" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D258" s="4"/>
     </row>
     <row r="259" spans="2:4" s="6" customFormat="1">
-      <c r="B259" s="22"/>
-      <c r="C259" s="7"/>
+      <c r="B259" s="20" t="s">
+        <v>222</v>
+      </c>
+      <c r="C259" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D259" s="4"/>
     </row>
     <row r="260" spans="2:4" s="6" customFormat="1">
-      <c r="B260" s="22"/>
+      <c r="B260" s="20"/>
       <c r="C260" s="7"/>
       <c r="D260" s="4"/>
     </row>
     <row r="261" spans="2:4" s="6" customFormat="1">
-      <c r="B261" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="C261" s="7"/>
+      <c r="B261" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="C261" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D261" s="4"/>
     </row>
     <row r="262" spans="2:4" s="6" customFormat="1">
-      <c r="B262" s="22"/>
-      <c r="C262" s="7"/>
+      <c r="B262" s="20" t="s">
+        <v>217</v>
+      </c>
+      <c r="C262" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D262" s="4"/>
     </row>
     <row r="263" spans="2:4" s="6" customFormat="1">
-      <c r="B263" s="22" t="s">
-        <v>71</v>
+      <c r="B263" s="20" t="s">
+        <v>218</v>
       </c>
       <c r="C263" s="7" t="s">
         <v>14</v>
@@ -4646,7 +4632,7 @@
     </row>
     <row r="264" spans="2:4" s="6" customFormat="1">
       <c r="B264" s="20" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="C264" s="7" t="s">
         <v>14</v>
@@ -4655,7 +4641,7 @@
     </row>
     <row r="265" spans="2:4" s="6" customFormat="1">
       <c r="B265" s="20" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="C265" s="7" t="s">
         <v>14</v>
@@ -4663,90 +4649,82 @@
       <c r="D265" s="4"/>
     </row>
     <row r="266" spans="2:4" s="6" customFormat="1">
-      <c r="B266" s="20" t="s">
-        <v>227</v>
-      </c>
-      <c r="C266" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="B266" s="22"/>
+      <c r="C266" s="7"/>
       <c r="D266" s="4"/>
     </row>
     <row r="267" spans="2:4" s="6" customFormat="1">
-      <c r="B267" s="20" t="s">
-        <v>228</v>
+      <c r="B267" s="22" t="s">
+        <v>199</v>
       </c>
       <c r="C267" s="7" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D267" s="4"/>
     </row>
     <row r="268" spans="2:4" s="6" customFormat="1">
-      <c r="B268" s="20"/>
-      <c r="C268" s="7"/>
+      <c r="B268" s="20" t="s">
+        <v>222</v>
+      </c>
+      <c r="C268" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="D268" s="4"/>
     </row>
     <row r="269" spans="2:4" s="6" customFormat="1">
-      <c r="B269" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="C269" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="B269" s="22"/>
+      <c r="C269" s="7"/>
       <c r="D269" s="4"/>
     </row>
     <row r="270" spans="2:4" s="6" customFormat="1">
-      <c r="B270" s="20" t="s">
-        <v>223</v>
+      <c r="B270" s="22" t="s">
+        <v>200</v>
       </c>
       <c r="C270" s="7" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D270" s="4"/>
     </row>
     <row r="271" spans="2:4" s="6" customFormat="1">
       <c r="B271" s="20" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C271" s="7" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D271" s="4"/>
     </row>
     <row r="272" spans="2:4" s="6" customFormat="1">
-      <c r="B272" s="20" t="s">
-        <v>222</v>
-      </c>
-      <c r="C272" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="B272" s="22"/>
+      <c r="C272" s="7"/>
       <c r="D272" s="4"/>
     </row>
     <row r="273" spans="2:4" s="6" customFormat="1">
-      <c r="B273" s="20" t="s">
-        <v>228</v>
+      <c r="B273" s="22" t="s">
+        <v>201</v>
       </c>
       <c r="C273" s="7" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D273" s="4"/>
     </row>
     <row r="274" spans="2:4" s="6" customFormat="1">
-      <c r="B274" s="22"/>
-      <c r="C274" s="7"/>
+      <c r="B274" s="20" t="s">
+        <v>223</v>
+      </c>
+      <c r="C274" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="D274" s="4"/>
     </row>
     <row r="275" spans="2:4" s="6" customFormat="1">
-      <c r="B275" s="22" t="s">
-        <v>205</v>
-      </c>
-      <c r="C275" s="7" t="s">
-        <v>2</v>
-      </c>
+      <c r="B275" s="22"/>
+      <c r="C275" s="7"/>
       <c r="D275" s="4"/>
     </row>
     <row r="276" spans="2:4" s="6" customFormat="1">
-      <c r="B276" s="20" t="s">
-        <v>228</v>
+      <c r="B276" s="22" t="s">
+        <v>196</v>
       </c>
       <c r="C276" s="7" t="s">
         <v>2</v>
@@ -4754,22 +4732,22 @@
       <c r="D276" s="4"/>
     </row>
     <row r="277" spans="2:4" s="6" customFormat="1">
-      <c r="B277" s="22"/>
-      <c r="C277" s="7"/>
+      <c r="B277" s="20" t="s">
+        <v>223</v>
+      </c>
+      <c r="C277" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="D277" s="4"/>
     </row>
     <row r="278" spans="2:4" s="6" customFormat="1">
-      <c r="B278" s="22" t="s">
-        <v>206</v>
-      </c>
-      <c r="C278" s="7" t="s">
-        <v>2</v>
-      </c>
+      <c r="B278" s="22"/>
+      <c r="C278" s="7"/>
       <c r="D278" s="4"/>
     </row>
     <row r="279" spans="2:4" s="6" customFormat="1">
-      <c r="B279" s="20" t="s">
-        <v>228</v>
+      <c r="B279" s="22" t="s">
+        <v>224</v>
       </c>
       <c r="C279" s="7" t="s">
         <v>2</v>
@@ -4777,22 +4755,22 @@
       <c r="D279" s="4"/>
     </row>
     <row r="280" spans="2:4" s="6" customFormat="1">
-      <c r="B280" s="22"/>
-      <c r="C280" s="7"/>
+      <c r="B280" s="20" t="s">
+        <v>222</v>
+      </c>
+      <c r="C280" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="D280" s="4"/>
     </row>
     <row r="281" spans="2:4" s="6" customFormat="1">
-      <c r="B281" s="22" t="s">
-        <v>207</v>
-      </c>
-      <c r="C281" s="7" t="s">
-        <v>2</v>
-      </c>
+      <c r="B281" s="22"/>
+      <c r="C281" s="7"/>
       <c r="D281" s="4"/>
     </row>
     <row r="282" spans="2:4" s="6" customFormat="1">
-      <c r="B282" s="20" t="s">
-        <v>229</v>
+      <c r="B282" s="22" t="s">
+        <v>225</v>
       </c>
       <c r="C282" s="7" t="s">
         <v>2</v>
@@ -4800,13 +4778,17 @@
       <c r="D282" s="4"/>
     </row>
     <row r="283" spans="2:4" s="6" customFormat="1">
-      <c r="B283" s="22"/>
-      <c r="C283" s="7"/>
+      <c r="B283" s="20" t="s">
+        <v>222</v>
+      </c>
+      <c r="C283" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="D283" s="4"/>
     </row>
     <row r="284" spans="2:4" s="6" customFormat="1">
-      <c r="B284" s="22" t="s">
-        <v>202</v>
+      <c r="B284" s="20" t="s">
+        <v>241</v>
       </c>
       <c r="C284" s="7" t="s">
         <v>2</v>
@@ -4814,22 +4796,22 @@
       <c r="D284" s="4"/>
     </row>
     <row r="285" spans="2:4" s="6" customFormat="1">
-      <c r="B285" s="20" t="s">
-        <v>229</v>
-      </c>
-      <c r="C285" s="7" t="s">
+      <c r="B285" s="22"/>
+      <c r="C285" s="7"/>
+      <c r="D285" s="4"/>
+    </row>
+    <row r="286" spans="2:4" s="6" customFormat="1">
+      <c r="B286" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="C286" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D285" s="4"/>
-    </row>
-    <row r="286" spans="2:4" s="6" customFormat="1">
-      <c r="B286" s="22"/>
-      <c r="C286" s="7"/>
       <c r="D286" s="4"/>
     </row>
     <row r="287" spans="2:4" s="6" customFormat="1">
-      <c r="B287" s="22" t="s">
-        <v>230</v>
+      <c r="B287" s="20" t="s">
+        <v>223</v>
       </c>
       <c r="C287" s="7" t="s">
         <v>2</v>
@@ -4837,22 +4819,22 @@
       <c r="D287" s="4"/>
     </row>
     <row r="288" spans="2:4" s="6" customFormat="1">
-      <c r="B288" s="20" t="s">
-        <v>228</v>
-      </c>
-      <c r="C288" s="7" t="s">
+      <c r="B288" s="22"/>
+      <c r="C288" s="7"/>
+      <c r="D288" s="4"/>
+    </row>
+    <row r="289" spans="2:4" s="6" customFormat="1">
+      <c r="B289" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="C289" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D288" s="4"/>
-    </row>
-    <row r="289" spans="2:4" s="6" customFormat="1">
-      <c r="B289" s="22"/>
-      <c r="C289" s="7"/>
       <c r="D289" s="4"/>
     </row>
     <row r="290" spans="2:4" s="6" customFormat="1">
-      <c r="B290" s="22" t="s">
-        <v>231</v>
+      <c r="B290" s="20" t="s">
+        <v>223</v>
       </c>
       <c r="C290" s="7" t="s">
         <v>2</v>
@@ -4860,21 +4842,13 @@
       <c r="D290" s="4"/>
     </row>
     <row r="291" spans="2:4" s="6" customFormat="1">
-      <c r="B291" s="20" t="s">
-        <v>228</v>
-      </c>
-      <c r="C291" s="7" t="s">
-        <v>2</v>
-      </c>
+      <c r="B291" s="22"/>
+      <c r="C291" s="7"/>
       <c r="D291" s="4"/>
     </row>
     <row r="292" spans="2:4" s="6" customFormat="1">
-      <c r="B292" s="20" t="s">
-        <v>247</v>
-      </c>
-      <c r="C292" s="7" t="s">
-        <v>2</v>
-      </c>
+      <c r="B292" s="22"/>
+      <c r="C292" s="7"/>
       <c r="D292" s="4"/>
     </row>
     <row r="293" spans="2:4" s="6" customFormat="1">
@@ -4883,21 +4857,13 @@
       <c r="D293" s="4"/>
     </row>
     <row r="294" spans="2:4" s="6" customFormat="1">
-      <c r="B294" s="22" t="s">
-        <v>70</v>
-      </c>
-      <c r="C294" s="7" t="s">
-        <v>2</v>
-      </c>
+      <c r="B294" s="22"/>
+      <c r="C294" s="7"/>
       <c r="D294" s="4"/>
     </row>
     <row r="295" spans="2:4" s="6" customFormat="1">
-      <c r="B295" s="20" t="s">
-        <v>229</v>
-      </c>
-      <c r="C295" s="7" t="s">
-        <v>2</v>
-      </c>
+      <c r="B295" s="22"/>
+      <c r="C295" s="7"/>
       <c r="D295" s="4"/>
     </row>
     <row r="296" spans="2:4" s="6" customFormat="1">
@@ -4906,461 +4872,477 @@
       <c r="D296" s="4"/>
     </row>
     <row r="297" spans="2:4" s="6" customFormat="1">
-      <c r="B297" s="22" t="s">
-        <v>69</v>
-      </c>
-      <c r="C297" s="7" t="s">
-        <v>2</v>
-      </c>
+      <c r="B297" s="22"/>
+      <c r="C297" s="7"/>
       <c r="D297" s="4"/>
     </row>
     <row r="298" spans="2:4" s="6" customFormat="1">
-      <c r="B298" s="20" t="s">
-        <v>229</v>
-      </c>
-      <c r="C298" s="7" t="s">
-        <v>2</v>
-      </c>
+      <c r="B298" s="20"/>
+      <c r="C298" s="7"/>
       <c r="D298" s="4"/>
     </row>
     <row r="299" spans="2:4" s="6" customFormat="1">
-      <c r="B299" s="22"/>
+      <c r="B299" s="19"/>
       <c r="C299" s="7"/>
       <c r="D299" s="4"/>
     </row>
     <row r="300" spans="2:4" s="6" customFormat="1">
-      <c r="B300" s="22"/>
+      <c r="B300" s="4"/>
       <c r="C300" s="7"/>
       <c r="D300" s="4"/>
     </row>
     <row r="301" spans="2:4" s="6" customFormat="1">
-      <c r="B301" s="22"/>
+      <c r="B301" s="3" t="s">
+        <v>208</v>
+      </c>
       <c r="C301" s="7"/>
       <c r="D301" s="4"/>
     </row>
-    <row r="302" spans="2:4" s="6" customFormat="1">
-      <c r="B302" s="22"/>
+    <row r="302" spans="2:4">
       <c r="C302" s="7"/>
-      <c r="D302" s="4"/>
-    </row>
-    <row r="303" spans="2:4" s="6" customFormat="1">
-      <c r="B303" s="22"/>
+    </row>
+    <row r="303" spans="2:4">
+      <c r="B303" s="43" t="s">
+        <v>111</v>
+      </c>
       <c r="C303" s="7"/>
-      <c r="D303" s="4"/>
-    </row>
-    <row r="304" spans="2:4" s="6" customFormat="1">
-      <c r="B304" s="22"/>
+    </row>
+    <row r="304" spans="2:4">
       <c r="C304" s="7"/>
-      <c r="D304" s="4"/>
-    </row>
-    <row r="305" spans="2:4" s="6" customFormat="1">
-      <c r="B305" s="22"/>
-      <c r="C305" s="7"/>
-      <c r="D305" s="4"/>
-    </row>
-    <row r="306" spans="2:4" s="6" customFormat="1">
-      <c r="B306" s="20"/>
-      <c r="C306" s="7"/>
-      <c r="D306" s="4"/>
-    </row>
-    <row r="307" spans="2:4" s="6" customFormat="1">
-      <c r="B307" s="19"/>
-      <c r="C307" s="7"/>
-      <c r="D307" s="4"/>
-    </row>
-    <row r="308" spans="2:4" s="6" customFormat="1">
-      <c r="B308" s="4"/>
-      <c r="C308" s="7"/>
-      <c r="D308" s="4"/>
-    </row>
-    <row r="309" spans="2:4" s="6" customFormat="1">
-      <c r="B309" s="3" t="s">
+    </row>
+    <row r="305" spans="2:3">
+      <c r="B305" t="s">
+        <v>65</v>
+      </c>
+      <c r="C305" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="306" spans="2:3">
+      <c r="B306" t="s">
+        <v>66</v>
+      </c>
+      <c r="C306" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="307" spans="2:3">
+      <c r="B307" t="s">
+        <v>67</v>
+      </c>
+      <c r="C307" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="308" spans="2:3">
+      <c r="B308" t="s">
+        <v>68</v>
+      </c>
+      <c r="C308" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="309" spans="2:3">
+      <c r="B309" t="s">
         <v>214</v>
       </c>
-      <c r="C309" s="7"/>
-      <c r="D309" s="4"/>
-    </row>
-    <row r="310" spans="2:4">
-      <c r="C310" s="7"/>
-    </row>
-    <row r="311" spans="2:4">
-      <c r="B311" s="43" t="s">
-        <v>115</v>
-      </c>
-      <c r="C311" s="7"/>
-    </row>
-    <row r="312" spans="2:4">
-      <c r="C312" s="7"/>
-    </row>
-    <row r="313" spans="2:4">
+      <c r="C309" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="310" spans="2:3">
+      <c r="B310" t="s">
+        <v>215</v>
+      </c>
+      <c r="C310" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="311" spans="2:3">
+      <c r="B311" t="s">
+        <v>69</v>
+      </c>
+      <c r="C311" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="312" spans="2:3">
+      <c r="B312" t="s">
+        <v>70</v>
+      </c>
+      <c r="C312" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="313" spans="2:3">
       <c r="B313" t="s">
-        <v>65</v>
-      </c>
-      <c r="C313" s="7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="314" spans="2:4">
+        <v>71</v>
+      </c>
+      <c r="C313" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="314" spans="2:3">
       <c r="B314" t="s">
-        <v>66</v>
-      </c>
-      <c r="C314" s="7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="315" spans="2:4">
+        <v>72</v>
+      </c>
+      <c r="C314" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="315" spans="2:3">
       <c r="B315" t="s">
-        <v>67</v>
-      </c>
-      <c r="C315" s="7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="316" spans="2:4">
-      <c r="B316" t="s">
-        <v>68</v>
-      </c>
-      <c r="C316" s="7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="317" spans="2:4">
-      <c r="B317" t="s">
-        <v>220</v>
-      </c>
-      <c r="C317" s="7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="318" spans="2:4">
-      <c r="B318" t="s">
-        <v>221</v>
-      </c>
-      <c r="C318" s="7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="319" spans="2:4">
-      <c r="B319" t="s">
-        <v>69</v>
-      </c>
-      <c r="C319" s="7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="320" spans="2:4">
-      <c r="B320" t="s">
-        <v>70</v>
-      </c>
-      <c r="C320" s="7" t="s">
-        <v>2</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="C315" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="316" spans="2:3">
+      <c r="B316" s="44" t="s">
+        <v>74</v>
+      </c>
+      <c r="C316" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="317" spans="2:3">
+      <c r="B317" s="45" t="s">
+        <v>82</v>
+      </c>
+      <c r="C317" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="318" spans="2:3">
+      <c r="B318" s="45" t="s">
+        <v>96</v>
+      </c>
+      <c r="C318" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="319" spans="2:3">
+      <c r="B319" s="44"/>
+      <c r="C319" s="9"/>
+    </row>
+    <row r="320" spans="2:3">
+      <c r="B320" s="44"/>
+      <c r="C320" s="9"/>
     </row>
     <row r="321" spans="2:3">
-      <c r="B321" t="s">
-        <v>71</v>
-      </c>
-      <c r="C321" s="9" t="s">
-        <v>14</v>
-      </c>
+      <c r="B321" s="44"/>
+      <c r="C321" s="9"/>
     </row>
     <row r="322" spans="2:3">
-      <c r="B322" t="s">
-        <v>72</v>
-      </c>
-      <c r="C322" s="9" t="s">
-        <v>14</v>
-      </c>
+      <c r="C322" s="9"/>
     </row>
     <row r="323" spans="2:3">
-      <c r="B323" t="s">
-        <v>73</v>
-      </c>
-      <c r="C323" s="9" t="s">
-        <v>14</v>
-      </c>
+      <c r="C323" s="9"/>
     </row>
     <row r="324" spans="2:3">
-      <c r="B324" s="44" t="s">
-        <v>74</v>
-      </c>
-      <c r="C324" s="9" t="s">
-        <v>14</v>
-      </c>
+      <c r="C324" s="9"/>
     </row>
     <row r="325" spans="2:3">
-      <c r="B325" s="45" t="s">
-        <v>82</v>
-      </c>
-      <c r="C325" s="9" t="s">
-        <v>14</v>
-      </c>
+      <c r="C325" s="9"/>
     </row>
     <row r="326" spans="2:3">
-      <c r="B326" s="45" t="s">
-        <v>96</v>
-      </c>
-      <c r="C326" s="9" t="s">
-        <v>14</v>
-      </c>
+      <c r="B326" s="43" t="s">
+        <v>112</v>
+      </c>
+      <c r="C326" s="9"/>
     </row>
     <row r="327" spans="2:3">
-      <c r="B327" s="44"/>
       <c r="C327" s="9"/>
     </row>
     <row r="328" spans="2:3">
-      <c r="B328" s="44"/>
-      <c r="C328" s="9"/>
+      <c r="B328" t="s">
+        <v>90</v>
+      </c>
+      <c r="C328" s="7" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="329" spans="2:3">
-      <c r="B329" s="44"/>
-      <c r="C329" s="9"/>
+      <c r="B329" t="s">
+        <v>91</v>
+      </c>
+      <c r="C329" s="7" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="330" spans="2:3">
-      <c r="C330" s="9"/>
+      <c r="B330" t="s">
+        <v>92</v>
+      </c>
+      <c r="C330" s="7" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="331" spans="2:3">
-      <c r="C331" s="9"/>
+      <c r="B331" t="s">
+        <v>93</v>
+      </c>
+      <c r="C331" s="7" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="332" spans="2:3">
-      <c r="C332" s="9"/>
+      <c r="B332" t="s">
+        <v>94</v>
+      </c>
+      <c r="C332" s="7" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="333" spans="2:3">
-      <c r="C333" s="9"/>
+      <c r="B333" t="s">
+        <v>95</v>
+      </c>
+      <c r="C333" s="7" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="334" spans="2:3">
-      <c r="B334" s="43" t="s">
-        <v>116</v>
-      </c>
-      <c r="C334" s="9"/>
+      <c r="B334" t="s">
+        <v>118</v>
+      </c>
+      <c r="C334" s="7" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="335" spans="2:3">
       <c r="C335" s="9"/>
     </row>
     <row r="336" spans="2:3">
-      <c r="B336" t="s">
-        <v>90</v>
-      </c>
-      <c r="C336" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="C336" s="9"/>
     </row>
     <row r="337" spans="2:3">
-      <c r="B337" t="s">
-        <v>91</v>
-      </c>
-      <c r="C337" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="C337" s="9"/>
     </row>
     <row r="338" spans="2:3">
-      <c r="B338" t="s">
-        <v>92</v>
-      </c>
-      <c r="C338" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="339" spans="2:3">
-      <c r="B339" t="s">
-        <v>93</v>
-      </c>
-      <c r="C339" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="340" spans="2:3">
-      <c r="B340" t="s">
-        <v>94</v>
-      </c>
-      <c r="C340" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="341" spans="2:3">
-      <c r="B341" t="s">
-        <v>95</v>
-      </c>
-      <c r="C341" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="342" spans="2:3">
-      <c r="B342" t="s">
-        <v>122</v>
-      </c>
-      <c r="C342" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="343" spans="2:3">
-      <c r="C343" s="9"/>
-    </row>
-    <row r="344" spans="2:3">
-      <c r="C344" s="9"/>
-    </row>
-    <row r="345" spans="2:3">
-      <c r="C345" s="9"/>
-    </row>
-    <row r="346" spans="2:3">
-      <c r="B346" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="C346" s="9"/>
+      <c r="B338" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C338" s="9"/>
+    </row>
+    <row r="352" spans="2:3">
+      <c r="B352" t="s">
+        <v>64</v>
+      </c>
+      <c r="C352" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="353" spans="2:3">
+      <c r="B353" s="44" t="s">
+        <v>109</v>
+      </c>
+      <c r="C353" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="354" spans="2:3">
+      <c r="B354" s="44" t="s">
+        <v>177</v>
+      </c>
+      <c r="C354" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="355" spans="2:3">
+      <c r="B355" s="44" t="s">
+        <v>81</v>
+      </c>
+      <c r="C355" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="356" spans="2:3">
+      <c r="B356" s="44"/>
+      <c r="C356" s="7"/>
+    </row>
+    <row r="357" spans="2:3">
+      <c r="B357" t="s">
+        <v>75</v>
+      </c>
+      <c r="C357" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="358" spans="2:3">
+      <c r="C358" s="9"/>
+    </row>
+    <row r="359" spans="2:3">
+      <c r="B359" s="45" t="s">
+        <v>80</v>
+      </c>
+      <c r="C359" s="9" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="360" spans="2:3">
-      <c r="B360" t="s">
-        <v>64</v>
-      </c>
-      <c r="C360" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="C360" s="9"/>
     </row>
     <row r="361" spans="2:3">
-      <c r="B361" s="44" t="s">
-        <v>113</v>
-      </c>
-      <c r="C361" s="7" t="s">
+      <c r="B361" s="45" t="s">
+        <v>78</v>
+      </c>
+      <c r="C361" s="9" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="362" spans="2:3">
-      <c r="B362" s="44" t="s">
-        <v>183</v>
-      </c>
-      <c r="C362" s="7" t="s">
+      <c r="B362" t="s">
+        <v>79</v>
+      </c>
+      <c r="C362" s="9" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="363" spans="2:3">
-      <c r="B363" s="44" t="s">
-        <v>81</v>
-      </c>
-      <c r="C363" s="9" t="s">
-        <v>14</v>
-      </c>
+      <c r="C363" s="9"/>
     </row>
     <row r="364" spans="2:3">
-      <c r="B364" s="44"/>
-      <c r="C364" s="7"/>
+      <c r="B364" t="s">
+        <v>144</v>
+      </c>
+      <c r="C364" s="7" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="365" spans="2:3">
-      <c r="B365" t="s">
-        <v>75</v>
-      </c>
-      <c r="C365" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="C365" s="9"/>
     </row>
     <row r="366" spans="2:3">
-      <c r="C366" s="9"/>
+      <c r="B366" t="s">
+        <v>39</v>
+      </c>
+      <c r="C366" s="7" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="367" spans="2:3">
-      <c r="B367" s="45" t="s">
-        <v>80</v>
-      </c>
-      <c r="C367" s="9" t="s">
+      <c r="B367" t="s">
+        <v>40</v>
+      </c>
+      <c r="C367" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="368" spans="2:3">
-      <c r="C368" s="9"/>
+      <c r="B368" t="s">
+        <v>41</v>
+      </c>
+      <c r="C368" s="7" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="369" spans="2:4">
-      <c r="B369" s="45" t="s">
-        <v>78</v>
-      </c>
-      <c r="C369" s="9" t="s">
-        <v>14</v>
-      </c>
+      <c r="C369" s="9"/>
     </row>
     <row r="370" spans="2:4">
       <c r="B370" t="s">
-        <v>79</v>
-      </c>
-      <c r="C370" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C370" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="371" spans="2:4">
-      <c r="C371" s="9"/>
+      <c r="B371" t="s">
+        <v>77</v>
+      </c>
+      <c r="C371" s="7" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="372" spans="2:4">
-      <c r="B372" t="s">
-        <v>149</v>
-      </c>
-      <c r="C372" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="373" spans="2:4">
-      <c r="C373" s="9"/>
-    </row>
-    <row r="374" spans="2:4">
-      <c r="B374" t="s">
-        <v>39</v>
+      <c r="C372" s="9"/>
+    </row>
+    <row r="373" spans="2:4" s="6" customFormat="1">
+      <c r="B373" s="22" t="s">
+        <v>137</v>
+      </c>
+      <c r="C373" s="7"/>
+      <c r="D373" s="4"/>
+    </row>
+    <row r="374" spans="2:4" s="6" customFormat="1">
+      <c r="B374" s="20" t="s">
+        <v>131</v>
       </c>
       <c r="C374" s="7" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="375" spans="2:4">
-      <c r="B375" t="s">
-        <v>40</v>
+      <c r="D374" s="4"/>
+    </row>
+    <row r="375" spans="2:4" s="6" customFormat="1">
+      <c r="B375" s="20" t="s">
+        <v>132</v>
       </c>
       <c r="C375" s="7" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="376" spans="2:4">
-      <c r="B376" t="s">
-        <v>41</v>
+      <c r="D375" s="4"/>
+    </row>
+    <row r="376" spans="2:4" s="6" customFormat="1">
+      <c r="B376" s="20" t="s">
+        <v>135</v>
       </c>
       <c r="C376" s="7" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="377" spans="2:4">
-      <c r="C377" s="9"/>
-    </row>
-    <row r="378" spans="2:4">
-      <c r="B378" t="s">
-        <v>76</v>
+      <c r="D376" s="4"/>
+    </row>
+    <row r="377" spans="2:4" s="6" customFormat="1">
+      <c r="B377" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="C377" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D377" s="4"/>
+    </row>
+    <row r="378" spans="2:4" s="6" customFormat="1">
+      <c r="B378" s="20" t="s">
+        <v>139</v>
       </c>
       <c r="C378" s="7" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="379" spans="2:4">
-      <c r="B379" t="s">
-        <v>77</v>
-      </c>
-      <c r="C379" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="380" spans="2:4">
-      <c r="C380" s="9"/>
+      <c r="D378" s="4"/>
+    </row>
+    <row r="379" spans="2:4" s="6" customFormat="1">
+      <c r="B379" s="22"/>
+      <c r="C379" s="7"/>
+      <c r="D379" s="4"/>
+    </row>
+    <row r="380" spans="2:4" s="6" customFormat="1">
+      <c r="B380" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="C380" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D380" s="4"/>
     </row>
     <row r="381" spans="2:4" s="6" customFormat="1">
       <c r="B381" s="22" t="s">
         <v>142</v>
       </c>
-      <c r="C381" s="7"/>
+      <c r="C381" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D381" s="4"/>
     </row>
     <row r="382" spans="2:4" s="6" customFormat="1">
-      <c r="B382" s="20" t="s">
-        <v>136</v>
-      </c>
-      <c r="C382" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="B382" s="22"/>
+      <c r="C382" s="7"/>
       <c r="D382" s="4"/>
     </row>
     <row r="383" spans="2:4" s="6" customFormat="1">
-      <c r="B383" s="20" t="s">
-        <v>137</v>
+      <c r="B383" s="22" t="s">
+        <v>78</v>
       </c>
       <c r="C383" s="7" t="s">
         <v>14</v>
@@ -5368,87 +5350,87 @@
       <c r="D383" s="4"/>
     </row>
     <row r="384" spans="2:4" s="6" customFormat="1">
-      <c r="B384" s="20" t="s">
-        <v>140</v>
-      </c>
-      <c r="C384" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="B384" s="22" t="s">
+        <v>179</v>
+      </c>
+      <c r="C384" s="7"/>
       <c r="D384" s="4"/>
     </row>
-    <row r="385" spans="2:4" s="6" customFormat="1">
-      <c r="B385" s="20" t="s">
-        <v>141</v>
-      </c>
-      <c r="C385" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D385" s="4"/>
-    </row>
-    <row r="386" spans="2:4" s="6" customFormat="1">
-      <c r="B386" s="20" t="s">
-        <v>144</v>
-      </c>
-      <c r="C386" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D386" s="4"/>
-    </row>
-    <row r="387" spans="2:4" s="6" customFormat="1">
-      <c r="B387" s="22"/>
-      <c r="C387" s="7"/>
-      <c r="D387" s="4"/>
+    <row r="385" spans="2:4">
+      <c r="C385" s="9"/>
+    </row>
+    <row r="386" spans="2:4">
+      <c r="C386" s="9"/>
     </row>
     <row r="388" spans="2:4" s="6" customFormat="1">
-      <c r="B388" s="22" t="s">
-        <v>146</v>
-      </c>
-      <c r="C388" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="B388" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C388" s="7"/>
       <c r="D388" s="4"/>
     </row>
     <row r="389" spans="2:4" s="6" customFormat="1">
-      <c r="B389" s="22" t="s">
-        <v>147</v>
-      </c>
-      <c r="C389" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="B389" s="22"/>
+      <c r="C389" s="7"/>
       <c r="D389" s="4"/>
     </row>
     <row r="390" spans="2:4" s="6" customFormat="1">
-      <c r="B390" s="22"/>
-      <c r="C390" s="7"/>
+      <c r="B390" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C390" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D390" s="4"/>
     </row>
     <row r="391" spans="2:4" s="6" customFormat="1">
       <c r="B391" s="22" t="s">
-        <v>78</v>
+        <v>33</v>
       </c>
       <c r="C391" s="7" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D391" s="4"/>
     </row>
     <row r="392" spans="2:4" s="6" customFormat="1">
       <c r="B392" s="22" t="s">
-        <v>185</v>
-      </c>
-      <c r="C392" s="7"/>
+        <v>36</v>
+      </c>
+      <c r="C392" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D392" s="4"/>
     </row>
-    <row r="393" spans="2:4">
-      <c r="C393" s="9"/>
-    </row>
-    <row r="394" spans="2:4">
-      <c r="C394" s="9"/>
+    <row r="393" spans="2:4" s="6" customFormat="1">
+      <c r="B393" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C393" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D393" s="4"/>
+    </row>
+    <row r="394" spans="2:4" s="6" customFormat="1">
+      <c r="B394" s="22"/>
+      <c r="C394" s="7"/>
+      <c r="D394" s="4"/>
+    </row>
+    <row r="395" spans="2:4" s="6" customFormat="1">
+      <c r="B395" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="C395" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D395" s="4"/>
     </row>
     <row r="396" spans="2:4" s="6" customFormat="1">
-      <c r="B396" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C396" s="7"/>
+      <c r="B396" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="C396" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D396" s="4"/>
     </row>
     <row r="397" spans="2:4" s="6" customFormat="1">
@@ -5458,7 +5440,7 @@
     </row>
     <row r="398" spans="2:4" s="6" customFormat="1">
       <c r="B398" s="22" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C398" s="7" t="s">
         <v>14</v>
@@ -5467,16 +5449,16 @@
     </row>
     <row r="399" spans="2:4" s="6" customFormat="1">
       <c r="B399" s="22" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="C399" s="7" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="D399" s="4"/>
     </row>
     <row r="400" spans="2:4" s="6" customFormat="1">
       <c r="B400" s="22" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C400" s="7" t="s">
         <v>14</v>
@@ -5484,31 +5466,27 @@
       <c r="D400" s="4"/>
     </row>
     <row r="401" spans="2:4" s="6" customFormat="1">
-      <c r="B401" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="C401" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="B401" s="22"/>
+      <c r="C401" s="7"/>
       <c r="D401" s="4"/>
     </row>
     <row r="402" spans="2:4" s="6" customFormat="1">
-      <c r="B402" s="22"/>
-      <c r="C402" s="7"/>
+      <c r="B402" s="22" t="s">
+        <v>114</v>
+      </c>
+      <c r="C402" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D402" s="4"/>
     </row>
     <row r="403" spans="2:4" s="6" customFormat="1">
-      <c r="B403" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="C403" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="B403" s="22"/>
+      <c r="C403" s="7"/>
       <c r="D403" s="4"/>
     </row>
     <row r="404" spans="2:4" s="6" customFormat="1">
       <c r="B404" s="22" t="s">
-        <v>38</v>
+        <v>151</v>
       </c>
       <c r="C404" s="7" t="s">
         <v>14</v>
@@ -5522,7 +5500,7 @@
     </row>
     <row r="406" spans="2:4" s="6" customFormat="1">
       <c r="B406" s="22" t="s">
-        <v>39</v>
+        <v>211</v>
       </c>
       <c r="C406" s="7" t="s">
         <v>14</v>
@@ -5530,21 +5508,13 @@
       <c r="D406" s="4"/>
     </row>
     <row r="407" spans="2:4" s="6" customFormat="1">
-      <c r="B407" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="C407" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="B407" s="22"/>
+      <c r="C407" s="7"/>
       <c r="D407" s="4"/>
     </row>
     <row r="408" spans="2:4" s="6" customFormat="1">
-      <c r="B408" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="C408" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="B408" s="22"/>
+      <c r="C408" s="7"/>
       <c r="D408" s="4"/>
     </row>
     <row r="409" spans="2:4" s="6" customFormat="1">
@@ -5553,8 +5523,8 @@
       <c r="D409" s="4"/>
     </row>
     <row r="410" spans="2:4" s="6" customFormat="1">
-      <c r="B410" s="22" t="s">
-        <v>118</v>
+      <c r="B410" s="3" t="s">
+        <v>152</v>
       </c>
       <c r="C410" s="7" t="s">
         <v>14</v>
@@ -5568,7 +5538,7 @@
     </row>
     <row r="412" spans="2:4" s="6" customFormat="1">
       <c r="B412" s="22" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C412" s="7" t="s">
         <v>14</v>
@@ -5582,7 +5552,7 @@
     </row>
     <row r="414" spans="2:4" s="6" customFormat="1">
       <c r="B414" s="22" t="s">
-        <v>217</v>
+        <v>154</v>
       </c>
       <c r="C414" s="7" t="s">
         <v>14</v>
@@ -5590,22 +5560,30 @@
       <c r="D414" s="4"/>
     </row>
     <row r="415" spans="2:4" s="6" customFormat="1">
-      <c r="B415" s="22"/>
-      <c r="C415" s="7"/>
+      <c r="B415" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="C415" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D415" s="4"/>
     </row>
     <row r="416" spans="2:4" s="6" customFormat="1">
-      <c r="B416" s="22"/>
-      <c r="C416" s="7"/>
+      <c r="B416" s="22" t="s">
+        <v>156</v>
+      </c>
+      <c r="C416" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D416" s="4"/>
     </row>
-    <row r="417" spans="2:4" s="6" customFormat="1">
+    <row r="417" spans="1:4" s="6" customFormat="1">
       <c r="B417" s="22"/>
       <c r="C417" s="7"/>
       <c r="D417" s="4"/>
     </row>
-    <row r="418" spans="2:4" s="6" customFormat="1">
-      <c r="B418" s="3" t="s">
+    <row r="418" spans="1:4" s="6" customFormat="1">
+      <c r="B418" s="22" t="s">
         <v>157</v>
       </c>
       <c r="C418" s="7" t="s">
@@ -5613,194 +5591,134 @@
       </c>
       <c r="D418" s="4"/>
     </row>
-    <row r="419" spans="2:4" s="6" customFormat="1">
-      <c r="B419" s="22"/>
-      <c r="C419" s="7"/>
+    <row r="419" spans="1:4" s="6" customFormat="1">
+      <c r="B419" s="22" t="s">
+        <v>158</v>
+      </c>
+      <c r="C419" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D419" s="4"/>
     </row>
-    <row r="420" spans="2:4" s="6" customFormat="1">
-      <c r="B420" s="22" t="s">
-        <v>158</v>
-      </c>
-      <c r="C420" s="7" t="s">
-        <v>14</v>
-      </c>
+    <row r="420" spans="1:4" s="6" customFormat="1">
+      <c r="B420" s="22"/>
+      <c r="C420" s="7"/>
       <c r="D420" s="4"/>
     </row>
-    <row r="421" spans="2:4" s="6" customFormat="1">
-      <c r="B421" s="22"/>
-      <c r="C421" s="7"/>
+    <row r="421" spans="1:4" s="6" customFormat="1">
+      <c r="B421" s="22" t="s">
+        <v>159</v>
+      </c>
+      <c r="C421" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D421" s="4"/>
     </row>
-    <row r="422" spans="2:4" s="6" customFormat="1">
-      <c r="B422" s="22" t="s">
-        <v>159</v>
-      </c>
-      <c r="C422" s="7" t="s">
-        <v>14</v>
-      </c>
+    <row r="422" spans="1:4" s="6" customFormat="1">
+      <c r="B422" s="22"/>
+      <c r="C422" s="7"/>
       <c r="D422" s="4"/>
     </row>
-    <row r="423" spans="2:4" s="6" customFormat="1">
-      <c r="B423" s="22" t="s">
-        <v>160</v>
-      </c>
-      <c r="C423" s="7" t="s">
-        <v>14</v>
-      </c>
+    <row r="423" spans="1:4" s="6" customFormat="1">
+      <c r="B423" s="22"/>
+      <c r="C423" s="7"/>
       <c r="D423" s="4"/>
     </row>
-    <row r="424" spans="2:4" s="6" customFormat="1">
-      <c r="B424" s="22" t="s">
-        <v>161</v>
-      </c>
-      <c r="C424" s="7" t="s">
-        <v>14</v>
-      </c>
+    <row r="424" spans="1:4" s="6" customFormat="1">
+      <c r="B424" s="22"/>
+      <c r="C424" s="7"/>
       <c r="D424" s="4"/>
     </row>
-    <row r="425" spans="2:4" s="6" customFormat="1">
+    <row r="425" spans="1:4" s="6" customFormat="1">
       <c r="B425" s="22"/>
-      <c r="C425" s="7"/>
+      <c r="C425" s="4"/>
       <c r="D425" s="4"/>
     </row>
-    <row r="426" spans="2:4" s="6" customFormat="1">
-      <c r="B426" s="22" t="s">
-        <v>162</v>
-      </c>
-      <c r="C426" s="7" t="s">
-        <v>14</v>
-      </c>
+    <row r="426" spans="1:4" s="6" customFormat="1">
+      <c r="B426" s="19"/>
+      <c r="C426" s="4"/>
       <c r="D426" s="4"/>
     </row>
-    <row r="427" spans="2:4" s="6" customFormat="1">
-      <c r="B427" s="22" t="s">
-        <v>163</v>
-      </c>
-      <c r="C427" s="7" t="s">
-        <v>14</v>
-      </c>
+    <row r="427" spans="1:4" s="6" customFormat="1">
+      <c r="B427" s="21"/>
+      <c r="C427" s="4"/>
       <c r="D427" s="4"/>
     </row>
-    <row r="428" spans="2:4" s="6" customFormat="1">
-      <c r="B428" s="22"/>
-      <c r="C428" s="7"/>
+    <row r="428" spans="1:4" s="6" customFormat="1">
+      <c r="B428" s="21"/>
+      <c r="C428" s="4"/>
       <c r="D428" s="4"/>
     </row>
-    <row r="429" spans="2:4" s="6" customFormat="1">
-      <c r="B429" s="22" t="s">
-        <v>164</v>
-      </c>
-      <c r="C429" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D429" s="4"/>
-    </row>
-    <row r="430" spans="2:4" s="6" customFormat="1">
-      <c r="B430" s="22"/>
-      <c r="C430" s="7"/>
-      <c r="D430" s="4"/>
-    </row>
-    <row r="431" spans="2:4" s="6" customFormat="1">
-      <c r="B431" s="22"/>
-      <c r="C431" s="7"/>
-      <c r="D431" s="4"/>
-    </row>
-    <row r="432" spans="2:4" s="6" customFormat="1">
-      <c r="B432" s="22"/>
-      <c r="C432" s="7"/>
-      <c r="D432" s="4"/>
-    </row>
-    <row r="433" spans="1:4" s="6" customFormat="1">
-      <c r="B433" s="22"/>
-      <c r="C433" s="4"/>
-      <c r="D433" s="4"/>
-    </row>
-    <row r="434" spans="1:4" s="6" customFormat="1">
-      <c r="B434" s="19"/>
-      <c r="C434" s="4"/>
-      <c r="D434" s="4"/>
-    </row>
-    <row r="435" spans="1:4" s="6" customFormat="1">
-      <c r="B435" s="21"/>
-      <c r="C435" s="4"/>
-      <c r="D435" s="4"/>
-    </row>
-    <row r="436" spans="1:4" s="6" customFormat="1">
-      <c r="B436" s="21"/>
-      <c r="C436" s="4"/>
-      <c r="D436" s="4"/>
-    </row>
-    <row r="437" spans="1:4">
-      <c r="A437" s="3"/>
-      <c r="B437" s="11"/>
-      <c r="C437" s="11"/>
-      <c r="D437" s="3"/>
-    </row>
-    <row r="438" spans="1:4">
-      <c r="A438" s="3"/>
-      <c r="B438" s="8" t="s">
+    <row r="429" spans="1:4">
+      <c r="A429" s="3"/>
+      <c r="B429" s="11"/>
+      <c r="C429" s="11"/>
+      <c r="D429" s="3"/>
+    </row>
+    <row r="430" spans="1:4">
+      <c r="A430" s="3"/>
+      <c r="B430" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C438" s="6">
-        <f>COUNTIF(C5:C437,"y")</f>
-        <v>102</v>
-      </c>
-      <c r="D438" s="2"/>
-    </row>
-    <row r="439" spans="1:4">
-      <c r="A439" s="3"/>
-      <c r="B439" s="8" t="s">
+      <c r="C430" s="6">
+        <f>COUNTIF(C5:C429,"y")</f>
+        <v>106</v>
+      </c>
+      <c r="D430" s="2"/>
+    </row>
+    <row r="431" spans="1:4">
+      <c r="A431" s="3"/>
+      <c r="B431" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C439" s="6">
-        <f>COUNTIF(C5:C437,"n")</f>
-        <v>159</v>
-      </c>
-      <c r="D439" s="2"/>
-    </row>
-    <row r="440" spans="1:4">
-      <c r="A440" s="3"/>
-      <c r="B440" s="8" t="s">
+      <c r="C431" s="6">
+        <f>COUNTIF(C5:C429,"n")</f>
+        <v>149</v>
+      </c>
+      <c r="D431" s="2"/>
+    </row>
+    <row r="432" spans="1:4">
+      <c r="A432" s="3"/>
+      <c r="B432" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C440" s="7">
-        <f>COUNTIF(C5:C437,"TBD")</f>
+      <c r="C432" s="7">
+        <f>COUNTIF(C5:C429,"TBD")</f>
         <v>0</v>
       </c>
-      <c r="D440" s="2"/>
-    </row>
-    <row r="441" spans="1:4">
-      <c r="A441" s="3"/>
-      <c r="B441" s="8" t="s">
+      <c r="D432" s="2"/>
+    </row>
+    <row r="433" spans="1:4">
+      <c r="A433" s="3"/>
+      <c r="B433" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C441">
-        <f>SUM(C438:C440)</f>
-        <v>261</v>
-      </c>
-      <c r="D441" s="2"/>
-    </row>
-    <row r="442" spans="1:4" ht="18">
-      <c r="A442" s="3"/>
-      <c r="B442" s="10"/>
-      <c r="C442" s="10" t="s">
+      <c r="C433">
+        <f>SUM(C430:C432)</f>
+        <v>255</v>
+      </c>
+      <c r="D433" s="2"/>
+    </row>
+    <row r="434" spans="1:4" ht="18">
+      <c r="A434" s="3"/>
+      <c r="B434" s="10"/>
+      <c r="C434" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D442" s="41">
-        <f>C438/(C439+C438 + C440)</f>
-        <v>0.39080459770114945</v>
-      </c>
-    </row>
-    <row r="443" spans="1:4">
-      <c r="A443" s="3"/>
-      <c r="B443" s="11"/>
-      <c r="C443" s="11"/>
-      <c r="D443" s="3"/>
+      <c r="D434" s="41">
+        <f>C430/(C431+C430 + C432)</f>
+        <v>0.41568627450980394</v>
+      </c>
+    </row>
+    <row r="435" spans="1:4">
+      <c r="A435" s="3"/>
+      <c r="B435" s="11"/>
+      <c r="C435" s="11"/>
+      <c r="D435" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
-  <conditionalFormatting sqref="C360:C394 C396:C65191 C1:C3 C6:C346">
+  <conditionalFormatting sqref="C352:C386 C388:C65183 C1:C3 C6:C338">
     <cfRule type="cellIs" dxfId="2" priority="19" stopIfTrue="1" operator="equal">
       <formula>"y"</formula>
     </cfRule>
@@ -5827,7 +5745,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="10020" topLeftCell="A46" activePane="bottomLeft"/>
       <selection activeCell="R30" sqref="R30"/>
-      <selection pane="bottomLeft" activeCell="D54" sqref="D54"/>
+      <selection pane="bottomLeft" activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5"/>
@@ -5848,7 +5766,7 @@
   <sheetData>
     <row r="1" spans="2:6" ht="18">
       <c r="E1" s="37" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="F1" s="12"/>
     </row>
@@ -6203,13 +6121,13 @@
     </row>
     <row r="54" spans="1:10">
       <c r="A54" s="47">
-        <v>43972</v>
+        <v>43974</v>
       </c>
       <c r="B54" s="4">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="C54" s="4">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="D54" s="4">
         <v>0</v>
@@ -6220,7 +6138,7 @@
       <c r="F54" s="48"/>
       <c r="G54" s="30">
         <f t="shared" ref="G54" si="3">B54/SUM(B54:E54)</f>
-        <v>0.39080459770114945</v>
+        <v>0.41568627450980394</v>
       </c>
       <c r="H54" s="7"/>
     </row>
@@ -6265,25 +6183,25 @@
       </c>
       <c r="G57" s="38">
         <f>MIN(G54)</f>
-        <v>0.39080459770114945</v>
+        <v>0.41568627450980394</v>
       </c>
       <c r="H57" s="7"/>
     </row>
     <row r="58" spans="1:10">
       <c r="A58" s="39">
         <f>SUM(B58:D58)</f>
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="B58" s="15">
-        <f>Features!C438</f>
-        <v>102</v>
+        <f>Features!C430</f>
+        <v>106</v>
       </c>
       <c r="C58" s="16">
-        <f>Features!C439</f>
-        <v>159</v>
+        <f>Features!C431</f>
+        <v>149</v>
       </c>
       <c r="D58" s="17">
-        <f>Features!C440</f>
+        <f>Features!C432</f>
         <v>0</v>
       </c>
       <c r="E58" s="18">
@@ -6327,11 +6245,11 @@
     </row>
     <row r="62" spans="1:10">
       <c r="A62" s="46" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B62" s="49">
         <f>(A54-A48)*A58/B58 +A48</f>
-        <v>44558.117647058825</v>
+        <v>44505.339622641506</v>
       </c>
       <c r="C62" s="4"/>
       <c r="D62" s="7"/>

</xml_diff>

<commit_message>
do not go beyond eof
</commit_message>
<xml_diff>
--- a/FxTextEditor Features.xlsx
+++ b/FxTextEditor Features.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="262">
   <si>
     <t>Feature</t>
   </si>
@@ -786,6 +786,24 @@
   </si>
   <si>
     <t>copies to clipboard</t>
+  </si>
+  <si>
+    <t>shift-home: select to beginning of line</t>
+  </si>
+  <si>
+    <t>shift-end: select to end of line</t>
+  </si>
+  <si>
+    <t>ctrl-shift-home: selecto to start of document</t>
+  </si>
+  <si>
+    <t>ctrl-shift-end: select to end of document</t>
+  </si>
+  <si>
+    <t>shift-command-up-arrow on mac</t>
+  </si>
+  <si>
+    <t>shift-command-down-arrow on mac</t>
   </si>
 </sst>
 </file>
@@ -1048,7 +1066,7 @@
           <c:yMode val="edge"/>
           <c:x val="3.8461559098965002E-2"/>
           <c:y val="2.2690437601296611E-2"/>
-          <c:w val="0.91978071330955535"/>
+          <c:w val="0.91978071330955546"/>
           <c:h val="0.89627228525119951"/>
         </c:manualLayout>
       </c:layout>
@@ -1081,10 +1099,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Progress!$A$48:$A$56</c:f>
+              <c:f>Progress!$A$48:$A$57</c:f>
               <c:numCache>
                 <c:formatCode>yyyy\/mm\/dd</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>43596</c:v>
                 </c:pt>
@@ -1110,17 +1128,20 @@
                   <c:v>43993</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43999</c:v>
+                  <c:v>44003</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Progress!$B$48:$B$56</c:f>
+              <c:f>Progress!$B$48:$B$57</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1146,6 +1167,9 @@
                   <c:v>166</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>171</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>171</c:v>
                 </c:pt>
               </c:numCache>
@@ -1179,10 +1203,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Progress!$A$48:$A$56</c:f>
+              <c:f>Progress!$A$48:$A$57</c:f>
               <c:numCache>
                 <c:formatCode>yyyy\/mm\/dd</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>43596</c:v>
                 </c:pt>
@@ -1208,17 +1232,20 @@
                   <c:v>43993</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43999</c:v>
+                  <c:v>44003</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Progress!$C$48:$C$56</c:f>
+              <c:f>Progress!$C$48:$C$57</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1245,6 +1272,9 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>104</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1277,10 +1307,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Progress!$A$48:$A$56</c:f>
+              <c:f>Progress!$A$48:$A$57</c:f>
               <c:numCache>
                 <c:formatCode>yyyy\/mm\/dd</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>43596</c:v>
                 </c:pt>
@@ -1306,17 +1336,20 @@
                   <c:v>43993</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43999</c:v>
+                  <c:v>44003</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Progress!$D$48:$D$56</c:f>
+              <c:f>Progress!$D$48:$D$57</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1342,6 +1375,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1375,10 +1411,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Progress!$A$48:$A$56</c:f>
+              <c:f>Progress!$A$48:$A$57</c:f>
               <c:numCache>
                 <c:formatCode>yyyy\/mm\/dd</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>43596</c:v>
                 </c:pt>
@@ -1404,17 +1440,20 @@
                   <c:v>43993</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43999</c:v>
+                  <c:v>44003</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Progress!$E$48:$E$60</c:f>
+              <c:f>Progress!$E$48:$E$61</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1442,21 +1481,24 @@
                 <c:pt idx="8">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="9">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="166125568"/>
-        <c:axId val="166127104"/>
+        <c:axId val="122111872"/>
+        <c:axId val="122113408"/>
       </c:areaChart>
       <c:dateAx>
-        <c:axId val="166125568"/>
+        <c:axId val="122111872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1489,7 +1531,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="166127104"/>
+        <c:crossAx val="122113408"/>
         <c:crosses val="autoZero"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
@@ -1499,7 +1541,7 @@
         <c:minorTimeUnit val="months"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="166127104"/>
+        <c:axId val="122113408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1541,7 +1583,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="166125568"/>
+        <c:crossAx val="122111872"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1564,7 +1606,7 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="4.5828229804607823E-2"/>
-          <c:y val="0.33819556996218614"/>
+          <c:y val="0.33819556996218625"/>
           <c:w val="0.12857154394162268"/>
           <c:h val="0.11669367909238262"/>
         </c:manualLayout>
@@ -1685,7 +1727,7 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="4.4510450248127949E-2"/>
+          <c:x val="4.4510450248127963E-2"/>
           <c:y val="0.10032394165889739"/>
           <c:w val="0.79228601441663349"/>
           <c:h val="0.79935527708863363"/>
@@ -1720,10 +1762,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Progress!$A$48:$A$56</c:f>
+              <c:f>Progress!$A$48:$A$57</c:f>
               <c:numCache>
                 <c:formatCode>yyyy\/mm\/dd</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>43596</c:v>
                 </c:pt>
@@ -1749,17 +1791,20 @@
                   <c:v>43993</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43999</c:v>
+                  <c:v>44003</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Progress!$G$48:$G$56</c:f>
+              <c:f>Progress!$G$48:$G$57</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1787,15 +1832,18 @@
                 <c:pt idx="8">
                   <c:v>0.63568773234200748</c:v>
                 </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.62181818181818183</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="166216448"/>
-        <c:axId val="166217984"/>
+        <c:axId val="122436224"/>
+        <c:axId val="121647488"/>
       </c:areaChart>
       <c:dateAx>
-        <c:axId val="166216448"/>
+        <c:axId val="122436224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1803,13 +1851,13 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="yyyy\/mm\/dd" sourceLinked="1"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="166217984"/>
+        <c:crossAx val="121647488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="166217984"/>
+        <c:axId val="121647488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1852,7 +1900,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="166216448"/>
+        <c:crossAx val="122436224"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1952,10 +2000,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Progress!$A$48:$A$56</c:f>
+              <c:f>Progress!$A$48:$A$57</c:f>
               <c:numCache>
                 <c:formatCode>yyyy\/mm\/dd</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>43596</c:v>
                 </c:pt>
@@ -1981,17 +2029,20 @@
                   <c:v>43993</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43999</c:v>
+                  <c:v>44003</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Progress!$C$48:$C$56</c:f>
+              <c:f>Progress!$C$48:$C$57</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -2018,6 +2069,9 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>104</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2050,10 +2104,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Progress!$A$48:$A$56</c:f>
+              <c:f>Progress!$A$48:$A$57</c:f>
               <c:numCache>
                 <c:formatCode>yyyy\/mm\/dd</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>43596</c:v>
                 </c:pt>
@@ -2079,17 +2133,20 @@
                   <c:v>43993</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43999</c:v>
+                  <c:v>44003</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Progress!$D$48:$D$56</c:f>
+              <c:f>Progress!$D$48:$D$57</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -2117,15 +2174,18 @@
                 <c:pt idx="8">
                   <c:v>0</c:v>
                 </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="166238464"/>
-        <c:axId val="166322176"/>
+        <c:axId val="122454400"/>
+        <c:axId val="122455936"/>
       </c:areaChart>
       <c:dateAx>
-        <c:axId val="166238464"/>
+        <c:axId val="122454400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2158,7 +2218,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="166322176"/>
+        <c:crossAx val="122455936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -2167,7 +2227,7 @@
         <c:minorTimeUnit val="months"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="166322176"/>
+        <c:axId val="122455936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2209,7 +2269,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="166238464"/>
+        <c:crossAx val="122454400"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2308,7 +2368,7 @@
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>63</xdr:row>
+      <xdr:row>64</xdr:row>
       <xdr:rowOff>123826</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2716,10 +2776,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D445"/>
+  <dimension ref="A1:D452"/>
   <sheetViews>
-    <sheetView topLeftCell="A332" workbookViewId="0">
-      <selection activeCell="A367" sqref="A367:XFD367"/>
+    <sheetView topLeftCell="A278" workbookViewId="0">
+      <selection activeCell="C322" sqref="C322"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5"/>
@@ -5121,49 +5181,80 @@
     </row>
     <row r="316" spans="2:3">
       <c r="B316" s="44" t="s">
+        <v>256</v>
+      </c>
+      <c r="C316" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="317" spans="2:3">
+      <c r="B317" s="44" t="s">
+        <v>257</v>
+      </c>
+      <c r="C317" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="318" spans="2:3">
+      <c r="B318" s="44" t="s">
+        <v>258</v>
+      </c>
+      <c r="C318" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="319" spans="2:3">
+      <c r="B319" s="50" t="s">
+        <v>261</v>
+      </c>
+      <c r="C319" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="320" spans="2:3">
+      <c r="B320" s="44" t="s">
+        <v>259</v>
+      </c>
+      <c r="C320" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="321" spans="2:3">
+      <c r="B321" s="50" t="s">
+        <v>260</v>
+      </c>
+      <c r="C321" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="322" spans="2:3">
+      <c r="B322" s="44"/>
+      <c r="C322" s="7"/>
+    </row>
+    <row r="323" spans="2:3">
+      <c r="B323" s="44" t="s">
         <v>95</v>
       </c>
-      <c r="C316" s="7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="317" spans="2:3">
-      <c r="C317" s="9"/>
-    </row>
-    <row r="318" spans="2:3">
-      <c r="B318" s="43" t="s">
-        <v>229</v>
-      </c>
-      <c r="C318" s="7"/>
-    </row>
-    <row r="319" spans="2:3">
-      <c r="B319" s="44" t="s">
-        <v>36</v>
-      </c>
-      <c r="C319" s="7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="320" spans="2:3">
-      <c r="C320" s="9"/>
-    </row>
-    <row r="321" spans="2:3">
-      <c r="C321" s="9"/>
-    </row>
-    <row r="322" spans="2:3">
-      <c r="C322" s="9"/>
-    </row>
-    <row r="323" spans="2:3">
-      <c r="C323" s="9"/>
+      <c r="C323" s="7" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="324" spans="2:3">
       <c r="C324" s="9"/>
     </row>
     <row r="325" spans="2:3">
-      <c r="C325" s="9"/>
+      <c r="B325" s="43" t="s">
+        <v>229</v>
+      </c>
+      <c r="C325" s="7"/>
     </row>
     <row r="326" spans="2:3">
-      <c r="C326" s="9"/>
+      <c r="B326" s="44" t="s">
+        <v>36</v>
+      </c>
+      <c r="C326" s="7" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="327" spans="2:3">
       <c r="C327" s="9"/>
@@ -5175,330 +5266,292 @@
       <c r="C329" s="9"/>
     </row>
     <row r="330" spans="2:3">
-      <c r="B330" s="3" t="s">
+      <c r="C330" s="9"/>
+    </row>
+    <row r="331" spans="2:3">
+      <c r="C331" s="9"/>
+    </row>
+    <row r="332" spans="2:3">
+      <c r="C332" s="9"/>
+    </row>
+    <row r="333" spans="2:3">
+      <c r="C333" s="9"/>
+    </row>
+    <row r="334" spans="2:3">
+      <c r="C334" s="9"/>
+    </row>
+    <row r="335" spans="2:3">
+      <c r="C335" s="9"/>
+    </row>
+    <row r="336" spans="2:3">
+      <c r="C336" s="9"/>
+    </row>
+    <row r="337" spans="2:3">
+      <c r="B337" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="C330" s="9"/>
-    </row>
-    <row r="332" spans="2:3">
-      <c r="B332" t="s">
+      <c r="C337" s="9"/>
+    </row>
+    <row r="339" spans="2:3">
+      <c r="B339" t="s">
         <v>60</v>
       </c>
-      <c r="C332" s="7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="333" spans="2:3">
-      <c r="B333" s="44" t="s">
+      <c r="C339" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="340" spans="2:3">
+      <c r="B340" s="44" t="s">
         <v>87</v>
       </c>
-      <c r="C333" s="7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="334" spans="2:3">
-      <c r="B334" s="44" t="s">
+      <c r="C340" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="341" spans="2:3">
+      <c r="B341" s="44" t="s">
         <v>148</v>
       </c>
-      <c r="C334" s="7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="335" spans="2:3">
-      <c r="B335" s="44"/>
-      <c r="C335" s="7"/>
-    </row>
-    <row r="336" spans="2:3">
-      <c r="B336" s="45" t="s">
+      <c r="C341" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="342" spans="2:3">
+      <c r="B342" s="44"/>
+      <c r="C342" s="7"/>
+    </row>
+    <row r="343" spans="2:3">
+      <c r="B343" s="45" t="s">
         <v>246</v>
       </c>
-      <c r="C336" s="7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="337" spans="2:3">
-      <c r="B337" s="44" t="s">
+      <c r="C343" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="344" spans="2:3">
+      <c r="B344" s="44" t="s">
         <v>224</v>
       </c>
-      <c r="C337" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="338" spans="2:3">
-      <c r="B338" s="44" t="s">
-        <v>225</v>
-      </c>
-      <c r="C338" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="339" spans="2:3">
-      <c r="B339" s="45"/>
-      <c r="C339" s="7"/>
-    </row>
-    <row r="340" spans="2:3">
-      <c r="B340" s="45" t="s">
-        <v>247</v>
-      </c>
-      <c r="C340" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="341" spans="2:3">
-      <c r="B341" s="44"/>
-      <c r="C341" s="7"/>
-    </row>
-    <row r="342" spans="2:3">
-      <c r="B342" t="s">
-        <v>71</v>
-      </c>
-      <c r="C342" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="343" spans="2:3">
-      <c r="C343" s="9"/>
-    </row>
-    <row r="344" spans="2:3">
-      <c r="B344" s="45" t="s">
-        <v>239</v>
-      </c>
-      <c r="C344" s="9" t="s">
+      <c r="C344" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="345" spans="2:3">
       <c r="B345" s="44" t="s">
-        <v>240</v>
+        <v>225</v>
       </c>
       <c r="C345" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="346" spans="2:3">
-      <c r="B346" s="44" t="s">
-        <v>241</v>
-      </c>
-      <c r="C346" s="7" t="s">
+      <c r="B346" s="45"/>
+      <c r="C346" s="7"/>
+    </row>
+    <row r="347" spans="2:3">
+      <c r="B347" s="45" t="s">
+        <v>247</v>
+      </c>
+      <c r="C347" s="7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="347" spans="2:3">
-      <c r="B347" s="44"/>
-      <c r="C347" s="9"/>
-    </row>
     <row r="348" spans="2:3">
-      <c r="B348" s="45" t="s">
-        <v>166</v>
-      </c>
-      <c r="C348" s="7" t="s">
+      <c r="B348" s="44"/>
+      <c r="C348" s="7"/>
+    </row>
+    <row r="349" spans="2:3">
+      <c r="B349" t="s">
+        <v>71</v>
+      </c>
+      <c r="C349" s="7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="349" spans="2:3">
-      <c r="B349" s="44"/>
-      <c r="C349" s="9"/>
-    </row>
     <row r="350" spans="2:3">
-      <c r="B350" t="s">
-        <v>121</v>
-      </c>
-      <c r="C350" s="7" t="s">
+      <c r="C350" s="9"/>
+    </row>
+    <row r="351" spans="2:3">
+      <c r="B351" s="45" t="s">
+        <v>239</v>
+      </c>
+      <c r="C351" s="9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="351" spans="2:3">
-      <c r="C351" s="9"/>
-    </row>
     <row r="352" spans="2:3">
-      <c r="B352" t="s">
-        <v>36</v>
+      <c r="B352" s="44" t="s">
+        <v>240</v>
       </c>
       <c r="C352" s="7" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
     </row>
     <row r="353" spans="2:3">
       <c r="B353" s="44" t="s">
-        <v>236</v>
+        <v>241</v>
       </c>
       <c r="C353" s="7" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
     </row>
     <row r="354" spans="2:3">
-      <c r="B354" s="44" t="s">
-        <v>226</v>
-      </c>
-      <c r="C354" s="7" t="s">
-        <v>2</v>
-      </c>
+      <c r="B354" s="44"/>
+      <c r="C354" s="9"/>
     </row>
     <row r="355" spans="2:3">
-      <c r="B355" s="44" t="s">
-        <v>234</v>
+      <c r="B355" s="45" t="s">
+        <v>166</v>
       </c>
       <c r="C355" s="7" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
     </row>
     <row r="356" spans="2:3">
-      <c r="B356" s="44" t="s">
-        <v>235</v>
-      </c>
-      <c r="C356" s="7" t="s">
-        <v>2</v>
-      </c>
+      <c r="B356" s="44"/>
+      <c r="C356" s="9"/>
     </row>
     <row r="357" spans="2:3">
-      <c r="B357" s="44"/>
-      <c r="C357" s="7"/>
+      <c r="B357" t="s">
+        <v>121</v>
+      </c>
+      <c r="C357" s="7" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="358" spans="2:3">
-      <c r="B358" t="s">
-        <v>37</v>
-      </c>
-      <c r="C358" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="C358" s="9"/>
     </row>
     <row r="359" spans="2:3">
-      <c r="B359" s="44" t="s">
-        <v>237</v>
+      <c r="B359" t="s">
+        <v>36</v>
       </c>
       <c r="C359" s="7" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
     <row r="360" spans="2:3">
       <c r="B360" s="44" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="C360" s="7" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
     <row r="361" spans="2:3">
       <c r="B361" s="44" t="s">
+        <v>226</v>
+      </c>
+      <c r="C361" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="362" spans="2:3">
+      <c r="B362" s="44" t="s">
+        <v>234</v>
+      </c>
+      <c r="C362" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="363" spans="2:3">
+      <c r="B363" s="44" t="s">
         <v>235</v>
       </c>
-      <c r="C361" s="7" t="s">
+      <c r="C363" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="364" spans="2:3">
+      <c r="B364" s="44"/>
+      <c r="C364" s="7"/>
+    </row>
+    <row r="365" spans="2:3">
+      <c r="B365" t="s">
+        <v>37</v>
+      </c>
+      <c r="C365" s="7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="362" spans="2:3">
-      <c r="C362" s="7"/>
-    </row>
-    <row r="363" spans="2:3">
-      <c r="B363" t="s">
-        <v>38</v>
-      </c>
-      <c r="C363" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="364" spans="2:3">
-      <c r="B364" s="44" t="s">
-        <v>255</v>
-      </c>
-      <c r="C364" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="365" spans="2:3">
-      <c r="C365" s="9"/>
-    </row>
     <row r="366" spans="2:3">
-      <c r="B366" t="s">
-        <v>72</v>
+      <c r="B366" s="44" t="s">
+        <v>237</v>
       </c>
       <c r="C366" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="367" spans="2:3">
-      <c r="C367" s="7"/>
+      <c r="B367" s="44" t="s">
+        <v>234</v>
+      </c>
+      <c r="C367" s="7" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="368" spans="2:3">
-      <c r="B368" t="s">
-        <v>73</v>
+      <c r="B368" s="44" t="s">
+        <v>235</v>
       </c>
       <c r="C368" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="369" spans="2:4">
-      <c r="C369" s="9"/>
-    </row>
-    <row r="370" spans="2:4" s="6" customFormat="1">
-      <c r="B370" s="22" t="s">
-        <v>114</v>
-      </c>
-      <c r="C370" s="7"/>
-      <c r="D370" s="4"/>
-    </row>
-    <row r="371" spans="2:4" s="6" customFormat="1">
-      <c r="B371" s="20" t="s">
-        <v>108</v>
+      <c r="C369" s="7"/>
+    </row>
+    <row r="370" spans="2:4">
+      <c r="B370" t="s">
+        <v>38</v>
+      </c>
+      <c r="C370" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="371" spans="2:4">
+      <c r="B371" s="44" t="s">
+        <v>255</v>
       </c>
       <c r="C371" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D371" s="4"/>
-    </row>
-    <row r="372" spans="2:4" s="6" customFormat="1">
-      <c r="B372" s="20" t="s">
-        <v>109</v>
-      </c>
-      <c r="C372" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D372" s="4"/>
-    </row>
-    <row r="373" spans="2:4" s="6" customFormat="1">
-      <c r="B373" s="20" t="s">
-        <v>112</v>
+    </row>
+    <row r="372" spans="2:4">
+      <c r="C372" s="9"/>
+    </row>
+    <row r="373" spans="2:4">
+      <c r="B373" t="s">
+        <v>72</v>
       </c>
       <c r="C373" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D373" s="4"/>
-    </row>
-    <row r="374" spans="2:4" s="6" customFormat="1">
-      <c r="B374" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="C374" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D374" s="4"/>
-    </row>
-    <row r="375" spans="2:4" s="6" customFormat="1">
-      <c r="B375" s="20" t="s">
-        <v>116</v>
+    </row>
+    <row r="374" spans="2:4">
+      <c r="C374" s="7"/>
+    </row>
+    <row r="375" spans="2:4">
+      <c r="B375" t="s">
+        <v>73</v>
       </c>
       <c r="C375" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D375" s="4"/>
-    </row>
-    <row r="376" spans="2:4" s="6" customFormat="1">
-      <c r="B376" s="22"/>
-      <c r="C376" s="7"/>
-      <c r="D376" s="4"/>
+    </row>
+    <row r="376" spans="2:4">
+      <c r="C376" s="9"/>
     </row>
     <row r="377" spans="2:4" s="6" customFormat="1">
       <c r="B377" s="22" t="s">
-        <v>118</v>
-      </c>
-      <c r="C377" s="7" t="s">
-        <v>14</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="C377" s="7"/>
       <c r="D377" s="4"/>
     </row>
     <row r="378" spans="2:4" s="6" customFormat="1">
-      <c r="B378" s="22" t="s">
-        <v>119</v>
+      <c r="B378" s="20" t="s">
+        <v>108</v>
       </c>
       <c r="C378" s="7" t="s">
         <v>14</v>
@@ -5506,66 +5559,104 @@
       <c r="D378" s="4"/>
     </row>
     <row r="379" spans="2:4" s="6" customFormat="1">
-      <c r="B379" s="22"/>
-      <c r="C379" s="7"/>
+      <c r="B379" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="C379" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D379" s="4"/>
     </row>
     <row r="380" spans="2:4" s="6" customFormat="1">
-      <c r="B380" s="22" t="s">
-        <v>74</v>
+      <c r="B380" s="20" t="s">
+        <v>112</v>
       </c>
       <c r="C380" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D380" t="s">
-        <v>248</v>
-      </c>
+      <c r="D380" s="4"/>
     </row>
     <row r="381" spans="2:4" s="6" customFormat="1">
-      <c r="B381" s="22" t="s">
-        <v>150</v>
+      <c r="B381" s="20" t="s">
+        <v>113</v>
       </c>
       <c r="C381" s="7" t="s">
         <v>14</v>
       </c>
       <c r="D381" s="4"/>
     </row>
-    <row r="382" spans="2:4">
-      <c r="B382" s="45" t="s">
+    <row r="382" spans="2:4" s="6" customFormat="1">
+      <c r="B382" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="C382" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D382" s="4"/>
+    </row>
+    <row r="383" spans="2:4" s="6" customFormat="1">
+      <c r="B383" s="22"/>
+      <c r="C383" s="7"/>
+      <c r="D383" s="4"/>
+    </row>
+    <row r="384" spans="2:4" s="6" customFormat="1">
+      <c r="B384" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="C384" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D384" s="4"/>
+    </row>
+    <row r="385" spans="2:4" s="6" customFormat="1">
+      <c r="B385" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="C385" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D385" s="4"/>
+    </row>
+    <row r="386" spans="2:4" s="6" customFormat="1">
+      <c r="B386" s="22"/>
+      <c r="C386" s="7"/>
+      <c r="D386" s="4"/>
+    </row>
+    <row r="387" spans="2:4" s="6" customFormat="1">
+      <c r="B387" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="C382" s="9" t="s">
+      <c r="C387" s="7" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="383" spans="2:4">
-      <c r="B383" t="s">
+      <c r="D387" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="388" spans="2:4" s="6" customFormat="1">
+      <c r="B388" s="22" t="s">
+        <v>150</v>
+      </c>
+      <c r="C388" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D388" s="4"/>
+    </row>
+    <row r="389" spans="2:4">
+      <c r="B389" s="45" t="s">
+        <v>74</v>
+      </c>
+      <c r="C389" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="390" spans="2:4">
+      <c r="B390" t="s">
         <v>75</v>
       </c>
-      <c r="C383" s="9" t="s">
+      <c r="C390" s="9" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="384" spans="2:4">
-      <c r="C384" s="9"/>
-    </row>
-    <row r="385" spans="2:4">
-      <c r="C385" s="9"/>
-    </row>
-    <row r="386" spans="2:4">
-      <c r="C386" s="9"/>
-    </row>
-    <row r="387" spans="2:4">
-      <c r="C387" s="9"/>
-    </row>
-    <row r="388" spans="2:4">
-      <c r="C388" s="9"/>
-    </row>
-    <row r="389" spans="2:4">
-      <c r="C389" s="9"/>
-    </row>
-    <row r="390" spans="2:4">
-      <c r="C390" s="9"/>
     </row>
     <row r="391" spans="2:4">
       <c r="C391" s="9"/>
@@ -5579,85 +5670,51 @@
     <row r="394" spans="2:4">
       <c r="C394" s="9"/>
     </row>
-    <row r="396" spans="2:4" s="6" customFormat="1">
-      <c r="B396" s="3" t="s">
+    <row r="395" spans="2:4">
+      <c r="C395" s="9"/>
+    </row>
+    <row r="396" spans="2:4">
+      <c r="C396" s="9"/>
+    </row>
+    <row r="397" spans="2:4">
+      <c r="C397" s="9"/>
+    </row>
+    <row r="398" spans="2:4">
+      <c r="C398" s="9"/>
+    </row>
+    <row r="399" spans="2:4">
+      <c r="C399" s="9"/>
+    </row>
+    <row r="400" spans="2:4">
+      <c r="C400" s="9"/>
+    </row>
+    <row r="401" spans="2:4">
+      <c r="C401" s="9"/>
+    </row>
+    <row r="403" spans="2:4" s="6" customFormat="1">
+      <c r="B403" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C396" s="7"/>
-      <c r="D396" s="4"/>
-    </row>
-    <row r="397" spans="2:4" s="6" customFormat="1">
-      <c r="B397" s="22"/>
-      <c r="C397" s="7"/>
-      <c r="D397" s="4"/>
-    </row>
-    <row r="398" spans="2:4" s="6" customFormat="1">
-      <c r="B398" s="22" t="s">
+      <c r="C403" s="7"/>
+      <c r="D403" s="4"/>
+    </row>
+    <row r="404" spans="2:4" s="6" customFormat="1">
+      <c r="B404" s="22"/>
+      <c r="C404" s="7"/>
+      <c r="D404" s="4"/>
+    </row>
+    <row r="405" spans="2:4" s="6" customFormat="1">
+      <c r="B405" s="22" t="s">
         <v>220</v>
       </c>
-      <c r="C398" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D398" s="4"/>
-    </row>
-    <row r="399" spans="2:4" s="6" customFormat="1">
-      <c r="B399" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="C399" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D399" s="4"/>
-    </row>
-    <row r="400" spans="2:4" s="6" customFormat="1">
-      <c r="B400" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="C400" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D400" s="4"/>
-    </row>
-    <row r="401" spans="2:4" s="6" customFormat="1">
-      <c r="B401" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="C401" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D401" s="4"/>
-    </row>
-    <row r="402" spans="2:4" s="6" customFormat="1">
-      <c r="B402" s="22"/>
-      <c r="C402" s="7"/>
-      <c r="D402" s="4"/>
-    </row>
-    <row r="403" spans="2:4" s="6" customFormat="1">
-      <c r="B403" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="C403" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D403" s="4"/>
-    </row>
-    <row r="404" spans="2:4" s="6" customFormat="1">
-      <c r="B404" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="C404" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D404" s="4"/>
-    </row>
-    <row r="405" spans="2:4" s="6" customFormat="1">
-      <c r="B405" s="22"/>
-      <c r="C405" s="7"/>
+      <c r="C405" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="D405" s="4"/>
     </row>
     <row r="406" spans="2:4" s="6" customFormat="1">
       <c r="B406" s="22" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C406" s="7" t="s">
         <v>2</v>
@@ -5665,8 +5722,8 @@
       <c r="D406" s="4"/>
     </row>
     <row r="407" spans="2:4" s="6" customFormat="1">
-      <c r="B407" s="20" t="s">
-        <v>237</v>
+      <c r="B407" s="22" t="s">
+        <v>33</v>
       </c>
       <c r="C407" s="7" t="s">
         <v>2</v>
@@ -5674,31 +5731,31 @@
       <c r="D407" s="4"/>
     </row>
     <row r="408" spans="2:4" s="6" customFormat="1">
-      <c r="B408" s="20" t="s">
-        <v>234</v>
+      <c r="B408" s="22" t="s">
+        <v>32</v>
       </c>
       <c r="C408" s="7" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="D408" s="4"/>
     </row>
     <row r="409" spans="2:4" s="6" customFormat="1">
-      <c r="B409" s="20" t="s">
-        <v>235</v>
-      </c>
-      <c r="C409" s="7" t="s">
-        <v>2</v>
-      </c>
+      <c r="B409" s="22"/>
+      <c r="C409" s="7"/>
       <c r="D409" s="4"/>
     </row>
     <row r="410" spans="2:4" s="6" customFormat="1">
-      <c r="B410" s="20"/>
-      <c r="C410" s="7"/>
+      <c r="B410" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C410" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D410" s="4"/>
     </row>
     <row r="411" spans="2:4" s="6" customFormat="1">
       <c r="B411" s="22" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C411" s="7" t="s">
         <v>14</v>
@@ -5706,36 +5763,40 @@
       <c r="D411" s="4"/>
     </row>
     <row r="412" spans="2:4" s="6" customFormat="1">
-      <c r="B412" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="C412" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="B412" s="22"/>
+      <c r="C412" s="7"/>
       <c r="D412" s="4"/>
     </row>
     <row r="413" spans="2:4" s="6" customFormat="1">
-      <c r="B413" s="22"/>
-      <c r="C413" s="7"/>
+      <c r="B413" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="C413" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="D413" s="4"/>
     </row>
     <row r="414" spans="2:4" s="6" customFormat="1">
-      <c r="B414" s="22" t="s">
-        <v>91</v>
+      <c r="B414" s="20" t="s">
+        <v>237</v>
       </c>
       <c r="C414" s="7" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D414" s="4"/>
     </row>
     <row r="415" spans="2:4" s="6" customFormat="1">
-      <c r="B415" s="22"/>
-      <c r="C415" s="7"/>
+      <c r="B415" s="20" t="s">
+        <v>234</v>
+      </c>
+      <c r="C415" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="D415" s="4"/>
     </row>
     <row r="416" spans="2:4" s="6" customFormat="1">
-      <c r="B416" s="22" t="s">
-        <v>231</v>
+      <c r="B416" s="20" t="s">
+        <v>235</v>
       </c>
       <c r="C416" s="7" t="s">
         <v>2</v>
@@ -5743,92 +5804,88 @@
       <c r="D416" s="4"/>
     </row>
     <row r="417" spans="2:4" s="6" customFormat="1">
-      <c r="B417" s="22"/>
+      <c r="B417" s="20"/>
       <c r="C417" s="7"/>
       <c r="D417" s="4"/>
     </row>
     <row r="418" spans="2:4" s="6" customFormat="1">
-      <c r="B418" s="22"/>
-      <c r="C418" s="7"/>
+      <c r="B418" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="C418" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D418" s="4"/>
     </row>
     <row r="419" spans="2:4" s="6" customFormat="1">
-      <c r="B419" s="22"/>
-      <c r="C419" s="7"/>
+      <c r="B419" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="C419" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D419" s="4"/>
     </row>
     <row r="420" spans="2:4" s="6" customFormat="1">
-      <c r="B420" s="3" t="s">
+      <c r="B420" s="22"/>
+      <c r="C420" s="7"/>
+      <c r="D420" s="4"/>
+    </row>
+    <row r="421" spans="2:4" s="6" customFormat="1">
+      <c r="B421" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="C421" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D421" s="4"/>
+    </row>
+    <row r="422" spans="2:4" s="6" customFormat="1">
+      <c r="B422" s="22"/>
+      <c r="C422" s="7"/>
+      <c r="D422" s="4"/>
+    </row>
+    <row r="423" spans="2:4" s="6" customFormat="1">
+      <c r="B423" s="22" t="s">
+        <v>231</v>
+      </c>
+      <c r="C423" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D423" s="4"/>
+    </row>
+    <row r="424" spans="2:4" s="6" customFormat="1">
+      <c r="B424" s="22"/>
+      <c r="C424" s="7"/>
+      <c r="D424" s="4"/>
+    </row>
+    <row r="425" spans="2:4" s="6" customFormat="1">
+      <c r="B425" s="22"/>
+      <c r="C425" s="7"/>
+      <c r="D425" s="4"/>
+    </row>
+    <row r="426" spans="2:4" s="6" customFormat="1">
+      <c r="B426" s="22"/>
+      <c r="C426" s="7"/>
+      <c r="D426" s="4"/>
+    </row>
+    <row r="427" spans="2:4" s="6" customFormat="1">
+      <c r="B427" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="C420" s="7" t="s">
+      <c r="C427" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D420" s="4"/>
-    </row>
-    <row r="421" spans="2:4" s="6" customFormat="1">
-      <c r="B421" s="22"/>
-      <c r="C421" s="7"/>
-      <c r="D421" s="4"/>
-    </row>
-    <row r="422" spans="2:4" s="6" customFormat="1">
-      <c r="B422" s="22" t="s">
-        <v>126</v>
-      </c>
-      <c r="C422" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D422" s="4"/>
-    </row>
-    <row r="423" spans="2:4" s="6" customFormat="1">
-      <c r="B423" s="22"/>
-      <c r="C423" s="7"/>
-      <c r="D423" s="4"/>
-    </row>
-    <row r="424" spans="2:4" s="6" customFormat="1">
-      <c r="B424" s="22" t="s">
-        <v>127</v>
-      </c>
-      <c r="C424" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D424" s="4"/>
-    </row>
-    <row r="425" spans="2:4" s="6" customFormat="1">
-      <c r="B425" s="22" t="s">
-        <v>128</v>
-      </c>
-      <c r="C425" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D425" s="4"/>
-    </row>
-    <row r="426" spans="2:4" s="6" customFormat="1">
-      <c r="B426" s="22" t="s">
-        <v>129</v>
-      </c>
-      <c r="C426" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D426" s="4"/>
-    </row>
-    <row r="427" spans="2:4" s="6" customFormat="1">
-      <c r="B427" s="22"/>
-      <c r="C427" s="7"/>
       <c r="D427" s="4"/>
     </row>
     <row r="428" spans="2:4" s="6" customFormat="1">
-      <c r="B428" s="22" t="s">
-        <v>130</v>
-      </c>
-      <c r="C428" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="B428" s="22"/>
+      <c r="C428" s="7"/>
       <c r="D428" s="4"/>
     </row>
     <row r="429" spans="2:4" s="6" customFormat="1">
       <c r="B429" s="22" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="C429" s="7" t="s">
         <v>14</v>
@@ -5842,7 +5899,7 @@
     </row>
     <row r="431" spans="2:4" s="6" customFormat="1">
       <c r="B431" s="22" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="C431" s="7" t="s">
         <v>14</v>
@@ -5850,13 +5907,21 @@
       <c r="D431" s="4"/>
     </row>
     <row r="432" spans="2:4" s="6" customFormat="1">
-      <c r="B432" s="22"/>
-      <c r="C432" s="7"/>
+      <c r="B432" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="C432" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D432" s="4"/>
     </row>
     <row r="433" spans="1:4" s="6" customFormat="1">
-      <c r="B433" s="22"/>
-      <c r="C433" s="7"/>
+      <c r="B433" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="C433" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D433" s="4"/>
     </row>
     <row r="434" spans="1:4" s="6" customFormat="1">
@@ -5865,95 +5930,142 @@
       <c r="D434" s="4"/>
     </row>
     <row r="435" spans="1:4" s="6" customFormat="1">
-      <c r="B435" s="22"/>
-      <c r="C435" s="4"/>
+      <c r="B435" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="C435" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D435" s="4"/>
     </row>
     <row r="436" spans="1:4" s="6" customFormat="1">
-      <c r="B436" s="19"/>
-      <c r="C436" s="4"/>
+      <c r="B436" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="C436" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D436" s="4"/>
     </row>
     <row r="437" spans="1:4" s="6" customFormat="1">
-      <c r="B437" s="21"/>
-      <c r="C437" s="4"/>
+      <c r="B437" s="22"/>
+      <c r="C437" s="7"/>
       <c r="D437" s="4"/>
     </row>
     <row r="438" spans="1:4" s="6" customFormat="1">
-      <c r="B438" s="21"/>
-      <c r="C438" s="4"/>
+      <c r="B438" s="22" t="s">
+        <v>132</v>
+      </c>
+      <c r="C438" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D438" s="4"/>
     </row>
-    <row r="439" spans="1:4">
-      <c r="A439" s="3"/>
-      <c r="B439" s="11"/>
-      <c r="C439" s="11"/>
-      <c r="D439" s="3"/>
-    </row>
-    <row r="440" spans="1:4">
-      <c r="A440" s="3"/>
-      <c r="B440" s="8" t="s">
+    <row r="439" spans="1:4" s="6" customFormat="1">
+      <c r="B439" s="22"/>
+      <c r="C439" s="7"/>
+      <c r="D439" s="4"/>
+    </row>
+    <row r="440" spans="1:4" s="6" customFormat="1">
+      <c r="B440" s="22"/>
+      <c r="C440" s="7"/>
+      <c r="D440" s="4"/>
+    </row>
+    <row r="441" spans="1:4" s="6" customFormat="1">
+      <c r="B441" s="22"/>
+      <c r="C441" s="7"/>
+      <c r="D441" s="4"/>
+    </row>
+    <row r="442" spans="1:4" s="6" customFormat="1">
+      <c r="B442" s="22"/>
+      <c r="C442" s="4"/>
+      <c r="D442" s="4"/>
+    </row>
+    <row r="443" spans="1:4" s="6" customFormat="1">
+      <c r="B443" s="19"/>
+      <c r="C443" s="4"/>
+      <c r="D443" s="4"/>
+    </row>
+    <row r="444" spans="1:4" s="6" customFormat="1">
+      <c r="B444" s="21"/>
+      <c r="C444" s="4"/>
+      <c r="D444" s="4"/>
+    </row>
+    <row r="445" spans="1:4" s="6" customFormat="1">
+      <c r="B445" s="21"/>
+      <c r="C445" s="4"/>
+      <c r="D445" s="4"/>
+    </row>
+    <row r="446" spans="1:4">
+      <c r="A446" s="3"/>
+      <c r="B446" s="11"/>
+      <c r="C446" s="11"/>
+      <c r="D446" s="3"/>
+    </row>
+    <row r="447" spans="1:4">
+      <c r="A447" s="3"/>
+      <c r="B447" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C440" s="6">
-        <f>COUNTIF(C5:C439,"y")</f>
+      <c r="C447" s="6">
+        <f>COUNTIF(C5:C446,"y")</f>
         <v>171</v>
       </c>
-      <c r="D440" s="2"/>
-    </row>
-    <row r="441" spans="1:4">
-      <c r="A441" s="3"/>
-      <c r="B441" s="8" t="s">
+      <c r="D447" s="2"/>
+    </row>
+    <row r="448" spans="1:4">
+      <c r="A448" s="3"/>
+      <c r="B448" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C441" s="6">
-        <f>COUNTIF(C5:C439,"n")</f>
-        <v>98</v>
-      </c>
-      <c r="D441" s="2"/>
-    </row>
-    <row r="442" spans="1:4">
-      <c r="A442" s="3"/>
-      <c r="B442" s="8" t="s">
+      <c r="C448" s="6">
+        <f>COUNTIF(C5:C446,"n")</f>
+        <v>104</v>
+      </c>
+      <c r="D448" s="2"/>
+    </row>
+    <row r="449" spans="1:4">
+      <c r="A449" s="3"/>
+      <c r="B449" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C442" s="7">
-        <f>COUNTIF(C5:C439,"TBD")</f>
+      <c r="C449" s="7">
+        <f>COUNTIF(C5:C446,"TBD")</f>
         <v>0</v>
       </c>
-      <c r="D442" s="2"/>
-    </row>
-    <row r="443" spans="1:4">
-      <c r="A443" s="3"/>
-      <c r="B443" s="8" t="s">
+      <c r="D449" s="2"/>
+    </row>
+    <row r="450" spans="1:4">
+      <c r="A450" s="3"/>
+      <c r="B450" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C443">
-        <f>SUM(C440:C442)</f>
-        <v>269</v>
-      </c>
-      <c r="D443" s="2"/>
-    </row>
-    <row r="444" spans="1:4" ht="18">
-      <c r="A444" s="3"/>
-      <c r="B444" s="10"/>
-      <c r="C444" s="10" t="s">
+      <c r="C450">
+        <f>SUM(C447:C449)</f>
+        <v>275</v>
+      </c>
+      <c r="D450" s="2"/>
+    </row>
+    <row r="451" spans="1:4" ht="18">
+      <c r="A451" s="3"/>
+      <c r="B451" s="10"/>
+      <c r="C451" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D444" s="41">
-        <f>C440/(C441+C440 + C442)</f>
-        <v>0.63568773234200748</v>
-      </c>
-    </row>
-    <row r="445" spans="1:4">
-      <c r="A445" s="3"/>
-      <c r="B445" s="11"/>
-      <c r="C445" s="11"/>
-      <c r="D445" s="3"/>
+      <c r="D451" s="41">
+        <f>C447/(C448+C447 + C449)</f>
+        <v>0.62181818181818183</v>
+      </c>
+    </row>
+    <row r="452" spans="1:4">
+      <c r="A452" s="3"/>
+      <c r="B452" s="11"/>
+      <c r="C452" s="11"/>
+      <c r="D452" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
-  <conditionalFormatting sqref="C396:C65193 C332:C394 C300:C330 C1:C3 C6:C298">
+  <conditionalFormatting sqref="C403:C65200 C339:C401 C300:C337 C1:C3 C6:C298">
     <cfRule type="cellIs" dxfId="2" priority="19" stopIfTrue="1" operator="equal">
       <formula>"y"</formula>
     </cfRule>
@@ -5975,12 +6087,12 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IT870"/>
+  <dimension ref="A1:IT871"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="10020" topLeftCell="A46" activePane="bottomLeft"/>
       <selection activeCell="R30" sqref="R30"/>
-      <selection pane="bottomLeft" activeCell="C57" sqref="C57"/>
+      <selection pane="bottomLeft" activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5"/>
@@ -6303,7 +6415,7 @@
       </c>
       <c r="F51" s="48"/>
       <c r="G51" s="30">
-        <f t="shared" ref="G51:G55" si="2">B51/SUM(B51:E51)</f>
+        <f t="shared" ref="G51:G56" si="2">B51/SUM(B51:E51)</f>
         <v>9.8654708520179366E-2</v>
       </c>
       <c r="H51" s="7"/>
@@ -6402,7 +6514,7 @@
     </row>
     <row r="56" spans="1:10">
       <c r="A56" s="47">
-        <v>43999</v>
+        <v>44003</v>
       </c>
       <c r="B56" s="4">
         <v>171</v>
@@ -6418,19 +6530,32 @@
       </c>
       <c r="F56" s="48"/>
       <c r="G56" s="30">
-        <f t="shared" ref="G56" si="3">B56/SUM(B56:E56)</f>
+        <f t="shared" si="2"/>
         <v>0.63568773234200748</v>
       </c>
       <c r="H56" s="7"/>
     </row>
     <row r="57" spans="1:10">
-      <c r="A57" s="47"/>
-      <c r="B57" s="4"/>
-      <c r="C57" s="4"/>
-      <c r="D57" s="4"/>
-      <c r="E57" s="4"/>
-      <c r="F57" s="28"/>
-      <c r="G57" s="30"/>
+      <c r="A57" s="47">
+        <v>44004</v>
+      </c>
+      <c r="B57" s="4">
+        <v>171</v>
+      </c>
+      <c r="C57" s="4">
+        <v>104</v>
+      </c>
+      <c r="D57" s="7">
+        <v>0</v>
+      </c>
+      <c r="E57" s="4">
+        <v>0</v>
+      </c>
+      <c r="F57" s="48"/>
+      <c r="G57" s="30">
+        <f t="shared" ref="G57" si="3">B57/SUM(B57:E57)</f>
+        <v>0.62181818181818183</v>
+      </c>
       <c r="H57" s="7"/>
     </row>
     <row r="58" spans="1:10">
@@ -6439,84 +6564,84 @@
       <c r="C58" s="4"/>
       <c r="D58" s="4"/>
       <c r="E58" s="4"/>
-      <c r="F58" s="31"/>
+      <c r="F58" s="28"/>
       <c r="G58" s="30"/>
       <c r="H58" s="7"/>
     </row>
     <row r="59" spans="1:10">
-      <c r="A59" s="14" t="s">
+      <c r="A59" s="47"/>
+      <c r="B59" s="4"/>
+      <c r="C59" s="4"/>
+      <c r="D59" s="4"/>
+      <c r="E59" s="4"/>
+      <c r="F59" s="31"/>
+      <c r="G59" s="30"/>
+      <c r="H59" s="7"/>
+    </row>
+    <row r="60" spans="1:10">
+      <c r="A60" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="B59" s="14" t="s">
+      <c r="B60" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C59" s="14" t="s">
+      <c r="C60" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="D59" s="14" t="s">
+      <c r="D60" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E59" s="14" t="s">
+      <c r="E60" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="F59" s="14" t="s">
+      <c r="F60" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="G59" s="38">
-        <f>MIN(G56)</f>
-        <v>0.63568773234200748</v>
-      </c>
-      <c r="H59" s="7"/>
-    </row>
-    <row r="60" spans="1:10">
-      <c r="A60" s="39">
-        <f>SUM(B60:D60)</f>
-        <v>269</v>
-      </c>
-      <c r="B60" s="15">
-        <f>Features!C440</f>
+      <c r="G60" s="38">
+        <f>MIN(G57)</f>
+        <v>0.62181818181818183</v>
+      </c>
+      <c r="H60" s="7"/>
+    </row>
+    <row r="61" spans="1:10">
+      <c r="A61" s="39">
+        <f>SUM(B61:D61)</f>
+        <v>275</v>
+      </c>
+      <c r="B61" s="15">
+        <f>Features!C447</f>
         <v>171</v>
       </c>
-      <c r="C60" s="16">
-        <f>Features!C441</f>
-        <v>98</v>
-      </c>
-      <c r="D60" s="17">
-        <f>Features!C442</f>
+      <c r="C61" s="16">
+        <f>Features!C448</f>
+        <v>104</v>
+      </c>
+      <c r="D61" s="17">
+        <f>Features!C449</f>
         <v>0</v>
       </c>
-      <c r="E60" s="18">
-        <f>MIN(E56)</f>
+      <c r="E61" s="18">
+        <f>MIN(E57)</f>
         <v>0</v>
       </c>
-      <c r="F60" s="7"/>
-      <c r="G60" s="30"/>
-      <c r="H60" s="7"/>
-    </row>
-    <row r="61" spans="1:10">
-      <c r="A61" s="4"/>
-      <c r="B61" s="19"/>
-      <c r="C61" s="4"/>
-      <c r="D61" s="7"/>
-      <c r="E61" s="7"/>
       <c r="F61" s="7"/>
       <c r="G61" s="30"/>
       <c r="H61" s="7"/>
-      <c r="J61" s="36"/>
     </row>
     <row r="62" spans="1:10">
       <c r="A62" s="4"/>
-      <c r="B62" s="4"/>
+      <c r="B62" s="19"/>
       <c r="C62" s="4"/>
       <c r="D62" s="7"/>
       <c r="E62" s="7"/>
       <c r="F62" s="7"/>
       <c r="G62" s="30"/>
       <c r="H62" s="7"/>
+      <c r="J62" s="36"/>
     </row>
     <row r="63" spans="1:10">
       <c r="A63" s="4"/>
-      <c r="B63" s="19"/>
+      <c r="B63" s="4"/>
       <c r="C63" s="4"/>
       <c r="D63" s="7"/>
       <c r="E63" s="7"/>
@@ -6525,13 +6650,8 @@
       <c r="H63" s="7"/>
     </row>
     <row r="64" spans="1:10">
-      <c r="A64" s="46" t="s">
-        <v>93</v>
-      </c>
-      <c r="B64" s="49">
-        <f>(A56-A48)*A60/B60 +A48</f>
-        <v>44229.959064327486</v>
-      </c>
+      <c r="A64" s="4"/>
+      <c r="B64" s="19"/>
       <c r="C64" s="4"/>
       <c r="D64" s="7"/>
       <c r="E64" s="7"/>
@@ -6540,8 +6660,13 @@
       <c r="H64" s="7"/>
     </row>
     <row r="65" spans="1:8">
-      <c r="A65" s="4"/>
-      <c r="B65" s="4"/>
+      <c r="A65" s="46" t="s">
+        <v>93</v>
+      </c>
+      <c r="B65" s="49">
+        <f>(A57-A48)*A61/B61 +A48</f>
+        <v>44252.140350877191</v>
+      </c>
       <c r="C65" s="4"/>
       <c r="D65" s="7"/>
       <c r="E65" s="7"/>
@@ -6551,7 +6676,7 @@
     </row>
     <row r="66" spans="1:8">
       <c r="A66" s="4"/>
-      <c r="B66" s="19"/>
+      <c r="B66" s="4"/>
       <c r="C66" s="4"/>
       <c r="D66" s="7"/>
       <c r="E66" s="7"/>
@@ -6571,7 +6696,7 @@
     </row>
     <row r="68" spans="1:8">
       <c r="A68" s="4"/>
-      <c r="B68" s="4"/>
+      <c r="B68" s="19"/>
       <c r="C68" s="4"/>
       <c r="D68" s="7"/>
       <c r="E68" s="7"/>
@@ -6591,7 +6716,7 @@
     </row>
     <row r="70" spans="1:8">
       <c r="A70" s="4"/>
-      <c r="B70" s="7"/>
+      <c r="B70" s="4"/>
       <c r="C70" s="4"/>
       <c r="D70" s="7"/>
       <c r="E70" s="7"/>
@@ -6601,7 +6726,7 @@
     </row>
     <row r="71" spans="1:8">
       <c r="A71" s="4"/>
-      <c r="B71" s="20"/>
+      <c r="B71" s="7"/>
       <c r="C71" s="4"/>
       <c r="D71" s="7"/>
       <c r="E71" s="7"/>
@@ -6620,7 +6745,7 @@
       <c r="H72" s="7"/>
     </row>
     <row r="73" spans="1:8">
-      <c r="A73" s="7"/>
+      <c r="A73" s="4"/>
       <c r="B73" s="20"/>
       <c r="C73" s="4"/>
       <c r="D73" s="7"/>
@@ -6631,7 +6756,7 @@
     </row>
     <row r="74" spans="1:8">
       <c r="A74" s="7"/>
-      <c r="B74" s="7"/>
+      <c r="B74" s="20"/>
       <c r="C74" s="4"/>
       <c r="D74" s="7"/>
       <c r="E74" s="7"/>
@@ -6762,7 +6887,7 @@
     <row r="87" spans="1:8">
       <c r="A87" s="7"/>
       <c r="B87" s="7"/>
-      <c r="C87" s="7"/>
+      <c r="C87" s="4"/>
       <c r="D87" s="7"/>
       <c r="E87" s="7"/>
       <c r="F87" s="7"/>
@@ -6771,7 +6896,7 @@
     </row>
     <row r="88" spans="1:8">
       <c r="A88" s="7"/>
-      <c r="B88" s="6"/>
+      <c r="B88" s="7"/>
       <c r="C88" s="7"/>
       <c r="D88" s="7"/>
       <c r="E88" s="7"/>
@@ -6779,15 +6904,15 @@
       <c r="G88" s="30"/>
       <c r="H88" s="7"/>
     </row>
-    <row r="89" spans="1:8" s="2" customFormat="1">
-      <c r="A89" s="4"/>
-      <c r="B89" s="4"/>
-      <c r="C89" s="4"/>
-      <c r="D89" s="4"/>
-      <c r="E89" s="4"/>
-      <c r="F89" s="4"/>
-      <c r="G89" s="34"/>
-      <c r="H89" s="4"/>
+    <row r="89" spans="1:8">
+      <c r="A89" s="7"/>
+      <c r="B89" s="6"/>
+      <c r="C89" s="7"/>
+      <c r="D89" s="7"/>
+      <c r="E89" s="7"/>
+      <c r="F89" s="7"/>
+      <c r="G89" s="30"/>
+      <c r="H89" s="7"/>
     </row>
     <row r="90" spans="1:8" s="2" customFormat="1">
       <c r="A90" s="4"/>
@@ -6961,7 +7086,7 @@
     </row>
     <row r="107" spans="1:8" s="2" customFormat="1">
       <c r="A107" s="4"/>
-      <c r="B107" s="6"/>
+      <c r="B107" s="4"/>
       <c r="C107" s="4"/>
       <c r="D107" s="4"/>
       <c r="E107" s="4"/>
@@ -6971,7 +7096,7 @@
     </row>
     <row r="108" spans="1:8" s="2" customFormat="1">
       <c r="A108" s="4"/>
-      <c r="B108" s="4"/>
+      <c r="B108" s="6"/>
       <c r="C108" s="4"/>
       <c r="D108" s="4"/>
       <c r="E108" s="4"/>
@@ -7001,7 +7126,7 @@
     </row>
     <row r="111" spans="1:8" s="2" customFormat="1">
       <c r="A111" s="4"/>
-      <c r="B111" s="19"/>
+      <c r="B111" s="4"/>
       <c r="C111" s="4"/>
       <c r="D111" s="4"/>
       <c r="E111" s="4"/>
@@ -7041,7 +7166,7 @@
     </row>
     <row r="115" spans="1:8" s="2" customFormat="1">
       <c r="A115" s="4"/>
-      <c r="B115" s="21"/>
+      <c r="B115" s="19"/>
       <c r="C115" s="4"/>
       <c r="D115" s="4"/>
       <c r="E115" s="4"/>
@@ -7051,7 +7176,7 @@
     </row>
     <row r="116" spans="1:8" s="2" customFormat="1">
       <c r="A116" s="4"/>
-      <c r="B116" s="4"/>
+      <c r="B116" s="21"/>
       <c r="C116" s="4"/>
       <c r="D116" s="4"/>
       <c r="E116" s="4"/>
@@ -7061,7 +7186,7 @@
     </row>
     <row r="117" spans="1:8" s="2" customFormat="1">
       <c r="A117" s="4"/>
-      <c r="B117" s="6"/>
+      <c r="B117" s="4"/>
       <c r="C117" s="4"/>
       <c r="D117" s="4"/>
       <c r="E117" s="4"/>
@@ -7071,7 +7196,7 @@
     </row>
     <row r="118" spans="1:8" s="2" customFormat="1">
       <c r="A118" s="4"/>
-      <c r="B118" s="4"/>
+      <c r="B118" s="6"/>
       <c r="C118" s="4"/>
       <c r="D118" s="4"/>
       <c r="E118" s="4"/>
@@ -7081,7 +7206,7 @@
     </row>
     <row r="119" spans="1:8" s="2" customFormat="1">
       <c r="A119" s="4"/>
-      <c r="B119" s="19"/>
+      <c r="B119" s="4"/>
       <c r="C119" s="4"/>
       <c r="D119" s="4"/>
       <c r="E119" s="4"/>
@@ -7101,7 +7226,7 @@
     </row>
     <row r="121" spans="1:8" s="2" customFormat="1">
       <c r="A121" s="4"/>
-      <c r="B121" s="4"/>
+      <c r="B121" s="19"/>
       <c r="C121" s="4"/>
       <c r="D121" s="4"/>
       <c r="E121" s="4"/>
@@ -7161,7 +7286,7 @@
     </row>
     <row r="127" spans="1:8" s="2" customFormat="1">
       <c r="A127" s="4"/>
-      <c r="B127" s="19"/>
+      <c r="B127" s="4"/>
       <c r="C127" s="4"/>
       <c r="D127" s="4"/>
       <c r="E127" s="4"/>
@@ -7261,7 +7386,7 @@
     </row>
     <row r="137" spans="1:8" s="2" customFormat="1">
       <c r="A137" s="4"/>
-      <c r="B137" s="4"/>
+      <c r="B137" s="19"/>
       <c r="C137" s="4"/>
       <c r="D137" s="4"/>
       <c r="E137" s="4"/>
@@ -7311,7 +7436,7 @@
     </row>
     <row r="142" spans="1:8" s="2" customFormat="1">
       <c r="A142" s="4"/>
-      <c r="B142" s="19"/>
+      <c r="B142" s="4"/>
       <c r="C142" s="4"/>
       <c r="D142" s="4"/>
       <c r="E142" s="4"/>
@@ -7331,7 +7456,7 @@
     </row>
     <row r="144" spans="1:8" s="2" customFormat="1">
       <c r="A144" s="4"/>
-      <c r="B144" s="4"/>
+      <c r="B144" s="19"/>
       <c r="C144" s="4"/>
       <c r="D144" s="4"/>
       <c r="E144" s="4"/>
@@ -7370,284 +7495,284 @@
       <c r="H147" s="4"/>
     </row>
     <row r="148" spans="1:254" s="2" customFormat="1">
-      <c r="A148" s="21"/>
-      <c r="B148" s="21"/>
-      <c r="C148" s="21"/>
-      <c r="D148" s="21"/>
-      <c r="E148" s="21"/>
-      <c r="F148" s="21"/>
-      <c r="G148" s="35"/>
-      <c r="H148" s="21"/>
-      <c r="I148" s="5"/>
-      <c r="J148" s="5"/>
-      <c r="K148" s="5"/>
-      <c r="L148" s="5"/>
-      <c r="M148" s="5"/>
-      <c r="N148" s="5"/>
-      <c r="O148" s="5"/>
-      <c r="P148" s="5"/>
-      <c r="Q148" s="5"/>
-      <c r="R148" s="5"/>
-      <c r="S148" s="5"/>
-      <c r="T148" s="5"/>
-      <c r="U148" s="5"/>
-      <c r="V148" s="5"/>
-      <c r="W148" s="5"/>
-      <c r="X148" s="5"/>
-      <c r="Y148" s="5"/>
-      <c r="Z148" s="5"/>
-      <c r="AA148" s="5"/>
-      <c r="AB148" s="5"/>
-      <c r="AC148" s="5"/>
-      <c r="AD148" s="5"/>
-      <c r="AE148" s="5"/>
-      <c r="AF148" s="5"/>
-      <c r="AG148" s="5"/>
-      <c r="AH148" s="5"/>
-      <c r="AI148" s="5"/>
-      <c r="AJ148" s="5"/>
-      <c r="AK148" s="5"/>
-      <c r="AL148" s="5"/>
-      <c r="AM148" s="5"/>
-      <c r="AN148" s="5"/>
-      <c r="AO148" s="5"/>
-      <c r="AP148" s="5"/>
-      <c r="AQ148" s="5"/>
-      <c r="AR148" s="5"/>
-      <c r="AS148" s="5"/>
-      <c r="AT148" s="5"/>
-      <c r="AU148" s="5"/>
-      <c r="AV148" s="5"/>
-      <c r="AW148" s="5"/>
-      <c r="AX148" s="5"/>
-      <c r="AY148" s="5"/>
-      <c r="AZ148" s="5"/>
-      <c r="BA148" s="5"/>
-      <c r="BB148" s="5"/>
-      <c r="BC148" s="5"/>
-      <c r="BD148" s="5"/>
-      <c r="BE148" s="5"/>
-      <c r="BF148" s="5"/>
-      <c r="BG148" s="5"/>
-      <c r="BH148" s="5"/>
-      <c r="BI148" s="5"/>
-      <c r="BJ148" s="5"/>
-      <c r="BK148" s="5"/>
-      <c r="BL148" s="5"/>
-      <c r="BM148" s="5"/>
-      <c r="BN148" s="5"/>
-      <c r="BO148" s="5"/>
-      <c r="BP148" s="5"/>
-      <c r="BQ148" s="5"/>
-      <c r="BR148" s="5"/>
-      <c r="BS148" s="5"/>
-      <c r="BT148" s="5"/>
-      <c r="BU148" s="5"/>
-      <c r="BV148" s="5"/>
-      <c r="BW148" s="5"/>
-      <c r="BX148" s="5"/>
-      <c r="BY148" s="5"/>
-      <c r="BZ148" s="5"/>
-      <c r="CA148" s="5"/>
-      <c r="CB148" s="5"/>
-      <c r="CC148" s="5"/>
-      <c r="CD148" s="5"/>
-      <c r="CE148" s="5"/>
-      <c r="CF148" s="5"/>
-      <c r="CG148" s="5"/>
-      <c r="CH148" s="5"/>
-      <c r="CI148" s="5"/>
-      <c r="CJ148" s="5"/>
-      <c r="CK148" s="5"/>
-      <c r="CL148" s="5"/>
-      <c r="CM148" s="5"/>
-      <c r="CN148" s="5"/>
-      <c r="CO148" s="5"/>
-      <c r="CP148" s="5"/>
-      <c r="CQ148" s="5"/>
-      <c r="CR148" s="5"/>
-      <c r="CS148" s="5"/>
-      <c r="CT148" s="5"/>
-      <c r="CU148" s="5"/>
-      <c r="CV148" s="5"/>
-      <c r="CW148" s="5"/>
-      <c r="CX148" s="5"/>
-      <c r="CY148" s="5"/>
-      <c r="CZ148" s="5"/>
-      <c r="DA148" s="5"/>
-      <c r="DB148" s="5"/>
-      <c r="DC148" s="5"/>
-      <c r="DD148" s="5"/>
-      <c r="DE148" s="5"/>
-      <c r="DF148" s="5"/>
-      <c r="DG148" s="5"/>
-      <c r="DH148" s="5"/>
-      <c r="DI148" s="5"/>
-      <c r="DJ148" s="5"/>
-      <c r="DK148" s="5"/>
-      <c r="DL148" s="5"/>
-      <c r="DM148" s="5"/>
-      <c r="DN148" s="5"/>
-      <c r="DO148" s="5"/>
-      <c r="DP148" s="5"/>
-      <c r="DQ148" s="5"/>
-      <c r="DR148" s="5"/>
-      <c r="DS148" s="5"/>
-      <c r="DT148" s="5"/>
-      <c r="DU148" s="5"/>
-      <c r="DV148" s="5"/>
-      <c r="DW148" s="5"/>
-      <c r="DX148" s="5"/>
-      <c r="DY148" s="5"/>
-      <c r="DZ148" s="5"/>
-      <c r="EA148" s="5"/>
-      <c r="EB148" s="5"/>
-      <c r="EC148" s="5"/>
-      <c r="ED148" s="5"/>
-      <c r="EE148" s="5"/>
-      <c r="EF148" s="5"/>
-      <c r="EG148" s="5"/>
-      <c r="EH148" s="5"/>
-      <c r="EI148" s="5"/>
-      <c r="EJ148" s="5"/>
-      <c r="EK148" s="5"/>
-      <c r="EL148" s="5"/>
-      <c r="EM148" s="5"/>
-      <c r="EN148" s="5"/>
-      <c r="EO148" s="5"/>
-      <c r="EP148" s="5"/>
-      <c r="EQ148" s="5"/>
-      <c r="ER148" s="5"/>
-      <c r="ES148" s="5"/>
-      <c r="ET148" s="5"/>
-      <c r="EU148" s="5"/>
-      <c r="EV148" s="5"/>
-      <c r="EW148" s="5"/>
-      <c r="EX148" s="5"/>
-      <c r="EY148" s="5"/>
-      <c r="EZ148" s="5"/>
-      <c r="FA148" s="5"/>
-      <c r="FB148" s="5"/>
-      <c r="FC148" s="5"/>
-      <c r="FD148" s="5"/>
-      <c r="FE148" s="5"/>
-      <c r="FF148" s="5"/>
-      <c r="FG148" s="5"/>
-      <c r="FH148" s="5"/>
-      <c r="FI148" s="5"/>
-      <c r="FJ148" s="5"/>
-      <c r="FK148" s="5"/>
-      <c r="FL148" s="5"/>
-      <c r="FM148" s="5"/>
-      <c r="FN148" s="5"/>
-      <c r="FO148" s="5"/>
-      <c r="FP148" s="5"/>
-      <c r="FQ148" s="5"/>
-      <c r="FR148" s="5"/>
-      <c r="FS148" s="5"/>
-      <c r="FT148" s="5"/>
-      <c r="FU148" s="5"/>
-      <c r="FV148" s="5"/>
-      <c r="FW148" s="5"/>
-      <c r="FX148" s="5"/>
-      <c r="FY148" s="5"/>
-      <c r="FZ148" s="5"/>
-      <c r="GA148" s="5"/>
-      <c r="GB148" s="5"/>
-      <c r="GC148" s="5"/>
-      <c r="GD148" s="5"/>
-      <c r="GE148" s="5"/>
-      <c r="GF148" s="5"/>
-      <c r="GG148" s="5"/>
-      <c r="GH148" s="5"/>
-      <c r="GI148" s="5"/>
-      <c r="GJ148" s="5"/>
-      <c r="GK148" s="5"/>
-      <c r="GL148" s="5"/>
-      <c r="GM148" s="5"/>
-      <c r="GN148" s="5"/>
-      <c r="GO148" s="5"/>
-      <c r="GP148" s="5"/>
-      <c r="GQ148" s="5"/>
-      <c r="GR148" s="5"/>
-      <c r="GS148" s="5"/>
-      <c r="GT148" s="5"/>
-      <c r="GU148" s="5"/>
-      <c r="GV148" s="5"/>
-      <c r="GW148" s="5"/>
-      <c r="GX148" s="5"/>
-      <c r="GY148" s="5"/>
-      <c r="GZ148" s="5"/>
-      <c r="HA148" s="5"/>
-      <c r="HB148" s="5"/>
-      <c r="HC148" s="5"/>
-      <c r="HD148" s="5"/>
-      <c r="HE148" s="5"/>
-      <c r="HF148" s="5"/>
-      <c r="HG148" s="5"/>
-      <c r="HH148" s="5"/>
-      <c r="HI148" s="5"/>
-      <c r="HJ148" s="5"/>
-      <c r="HK148" s="5"/>
-      <c r="HL148" s="5"/>
-      <c r="HM148" s="5"/>
-      <c r="HN148" s="5"/>
-      <c r="HO148" s="5"/>
-      <c r="HP148" s="5"/>
-      <c r="HQ148" s="5"/>
-      <c r="HR148" s="5"/>
-      <c r="HS148" s="5"/>
-      <c r="HT148" s="5"/>
-      <c r="HU148" s="5"/>
-      <c r="HV148" s="5"/>
-      <c r="HW148" s="5"/>
-      <c r="HX148" s="5"/>
-      <c r="HY148" s="5"/>
-      <c r="HZ148" s="5"/>
-      <c r="IA148" s="5"/>
-      <c r="IB148" s="5"/>
-      <c r="IC148" s="5"/>
-      <c r="ID148" s="5"/>
-      <c r="IE148" s="5"/>
-      <c r="IF148" s="5"/>
-      <c r="IG148" s="5"/>
-      <c r="IH148" s="5"/>
-      <c r="II148" s="5"/>
-      <c r="IJ148" s="5"/>
-      <c r="IK148" s="5"/>
-      <c r="IL148" s="5"/>
-      <c r="IM148" s="5"/>
-      <c r="IN148" s="5"/>
-      <c r="IO148" s="5"/>
-      <c r="IP148" s="5"/>
-      <c r="IQ148" s="5"/>
-      <c r="IR148" s="5"/>
-      <c r="IS148" s="5"/>
-      <c r="IT148" s="5"/>
+      <c r="A148" s="4"/>
+      <c r="B148" s="4"/>
+      <c r="C148" s="4"/>
+      <c r="D148" s="4"/>
+      <c r="E148" s="4"/>
+      <c r="F148" s="4"/>
+      <c r="G148" s="34"/>
+      <c r="H148" s="4"/>
     </row>
     <row r="149" spans="1:254" s="2" customFormat="1">
-      <c r="A149" s="4"/>
-      <c r="B149" s="4"/>
-      <c r="C149" s="4"/>
-      <c r="D149" s="4"/>
-      <c r="E149" s="4"/>
-      <c r="F149" s="4"/>
-      <c r="G149" s="34"/>
-      <c r="H149" s="4"/>
-    </row>
-    <row r="150" spans="1:254">
-      <c r="A150" s="7"/>
-      <c r="B150" s="6"/>
-      <c r="C150" s="7"/>
-      <c r="D150" s="7"/>
-      <c r="E150" s="7"/>
-      <c r="F150" s="7"/>
-      <c r="G150" s="30"/>
-      <c r="H150" s="7"/>
+      <c r="A149" s="21"/>
+      <c r="B149" s="21"/>
+      <c r="C149" s="21"/>
+      <c r="D149" s="21"/>
+      <c r="E149" s="21"/>
+      <c r="F149" s="21"/>
+      <c r="G149" s="35"/>
+      <c r="H149" s="21"/>
+      <c r="I149" s="5"/>
+      <c r="J149" s="5"/>
+      <c r="K149" s="5"/>
+      <c r="L149" s="5"/>
+      <c r="M149" s="5"/>
+      <c r="N149" s="5"/>
+      <c r="O149" s="5"/>
+      <c r="P149" s="5"/>
+      <c r="Q149" s="5"/>
+      <c r="R149" s="5"/>
+      <c r="S149" s="5"/>
+      <c r="T149" s="5"/>
+      <c r="U149" s="5"/>
+      <c r="V149" s="5"/>
+      <c r="W149" s="5"/>
+      <c r="X149" s="5"/>
+      <c r="Y149" s="5"/>
+      <c r="Z149" s="5"/>
+      <c r="AA149" s="5"/>
+      <c r="AB149" s="5"/>
+      <c r="AC149" s="5"/>
+      <c r="AD149" s="5"/>
+      <c r="AE149" s="5"/>
+      <c r="AF149" s="5"/>
+      <c r="AG149" s="5"/>
+      <c r="AH149" s="5"/>
+      <c r="AI149" s="5"/>
+      <c r="AJ149" s="5"/>
+      <c r="AK149" s="5"/>
+      <c r="AL149" s="5"/>
+      <c r="AM149" s="5"/>
+      <c r="AN149" s="5"/>
+      <c r="AO149" s="5"/>
+      <c r="AP149" s="5"/>
+      <c r="AQ149" s="5"/>
+      <c r="AR149" s="5"/>
+      <c r="AS149" s="5"/>
+      <c r="AT149" s="5"/>
+      <c r="AU149" s="5"/>
+      <c r="AV149" s="5"/>
+      <c r="AW149" s="5"/>
+      <c r="AX149" s="5"/>
+      <c r="AY149" s="5"/>
+      <c r="AZ149" s="5"/>
+      <c r="BA149" s="5"/>
+      <c r="BB149" s="5"/>
+      <c r="BC149" s="5"/>
+      <c r="BD149" s="5"/>
+      <c r="BE149" s="5"/>
+      <c r="BF149" s="5"/>
+      <c r="BG149" s="5"/>
+      <c r="BH149" s="5"/>
+      <c r="BI149" s="5"/>
+      <c r="BJ149" s="5"/>
+      <c r="BK149" s="5"/>
+      <c r="BL149" s="5"/>
+      <c r="BM149" s="5"/>
+      <c r="BN149" s="5"/>
+      <c r="BO149" s="5"/>
+      <c r="BP149" s="5"/>
+      <c r="BQ149" s="5"/>
+      <c r="BR149" s="5"/>
+      <c r="BS149" s="5"/>
+      <c r="BT149" s="5"/>
+      <c r="BU149" s="5"/>
+      <c r="BV149" s="5"/>
+      <c r="BW149" s="5"/>
+      <c r="BX149" s="5"/>
+      <c r="BY149" s="5"/>
+      <c r="BZ149" s="5"/>
+      <c r="CA149" s="5"/>
+      <c r="CB149" s="5"/>
+      <c r="CC149" s="5"/>
+      <c r="CD149" s="5"/>
+      <c r="CE149" s="5"/>
+      <c r="CF149" s="5"/>
+      <c r="CG149" s="5"/>
+      <c r="CH149" s="5"/>
+      <c r="CI149" s="5"/>
+      <c r="CJ149" s="5"/>
+      <c r="CK149" s="5"/>
+      <c r="CL149" s="5"/>
+      <c r="CM149" s="5"/>
+      <c r="CN149" s="5"/>
+      <c r="CO149" s="5"/>
+      <c r="CP149" s="5"/>
+      <c r="CQ149" s="5"/>
+      <c r="CR149" s="5"/>
+      <c r="CS149" s="5"/>
+      <c r="CT149" s="5"/>
+      <c r="CU149" s="5"/>
+      <c r="CV149" s="5"/>
+      <c r="CW149" s="5"/>
+      <c r="CX149" s="5"/>
+      <c r="CY149" s="5"/>
+      <c r="CZ149" s="5"/>
+      <c r="DA149" s="5"/>
+      <c r="DB149" s="5"/>
+      <c r="DC149" s="5"/>
+      <c r="DD149" s="5"/>
+      <c r="DE149" s="5"/>
+      <c r="DF149" s="5"/>
+      <c r="DG149" s="5"/>
+      <c r="DH149" s="5"/>
+      <c r="DI149" s="5"/>
+      <c r="DJ149" s="5"/>
+      <c r="DK149" s="5"/>
+      <c r="DL149" s="5"/>
+      <c r="DM149" s="5"/>
+      <c r="DN149" s="5"/>
+      <c r="DO149" s="5"/>
+      <c r="DP149" s="5"/>
+      <c r="DQ149" s="5"/>
+      <c r="DR149" s="5"/>
+      <c r="DS149" s="5"/>
+      <c r="DT149" s="5"/>
+      <c r="DU149" s="5"/>
+      <c r="DV149" s="5"/>
+      <c r="DW149" s="5"/>
+      <c r="DX149" s="5"/>
+      <c r="DY149" s="5"/>
+      <c r="DZ149" s="5"/>
+      <c r="EA149" s="5"/>
+      <c r="EB149" s="5"/>
+      <c r="EC149" s="5"/>
+      <c r="ED149" s="5"/>
+      <c r="EE149" s="5"/>
+      <c r="EF149" s="5"/>
+      <c r="EG149" s="5"/>
+      <c r="EH149" s="5"/>
+      <c r="EI149" s="5"/>
+      <c r="EJ149" s="5"/>
+      <c r="EK149" s="5"/>
+      <c r="EL149" s="5"/>
+      <c r="EM149" s="5"/>
+      <c r="EN149" s="5"/>
+      <c r="EO149" s="5"/>
+      <c r="EP149" s="5"/>
+      <c r="EQ149" s="5"/>
+      <c r="ER149" s="5"/>
+      <c r="ES149" s="5"/>
+      <c r="ET149" s="5"/>
+      <c r="EU149" s="5"/>
+      <c r="EV149" s="5"/>
+      <c r="EW149" s="5"/>
+      <c r="EX149" s="5"/>
+      <c r="EY149" s="5"/>
+      <c r="EZ149" s="5"/>
+      <c r="FA149" s="5"/>
+      <c r="FB149" s="5"/>
+      <c r="FC149" s="5"/>
+      <c r="FD149" s="5"/>
+      <c r="FE149" s="5"/>
+      <c r="FF149" s="5"/>
+      <c r="FG149" s="5"/>
+      <c r="FH149" s="5"/>
+      <c r="FI149" s="5"/>
+      <c r="FJ149" s="5"/>
+      <c r="FK149" s="5"/>
+      <c r="FL149" s="5"/>
+      <c r="FM149" s="5"/>
+      <c r="FN149" s="5"/>
+      <c r="FO149" s="5"/>
+      <c r="FP149" s="5"/>
+      <c r="FQ149" s="5"/>
+      <c r="FR149" s="5"/>
+      <c r="FS149" s="5"/>
+      <c r="FT149" s="5"/>
+      <c r="FU149" s="5"/>
+      <c r="FV149" s="5"/>
+      <c r="FW149" s="5"/>
+      <c r="FX149" s="5"/>
+      <c r="FY149" s="5"/>
+      <c r="FZ149" s="5"/>
+      <c r="GA149" s="5"/>
+      <c r="GB149" s="5"/>
+      <c r="GC149" s="5"/>
+      <c r="GD149" s="5"/>
+      <c r="GE149" s="5"/>
+      <c r="GF149" s="5"/>
+      <c r="GG149" s="5"/>
+      <c r="GH149" s="5"/>
+      <c r="GI149" s="5"/>
+      <c r="GJ149" s="5"/>
+      <c r="GK149" s="5"/>
+      <c r="GL149" s="5"/>
+      <c r="GM149" s="5"/>
+      <c r="GN149" s="5"/>
+      <c r="GO149" s="5"/>
+      <c r="GP149" s="5"/>
+      <c r="GQ149" s="5"/>
+      <c r="GR149" s="5"/>
+      <c r="GS149" s="5"/>
+      <c r="GT149" s="5"/>
+      <c r="GU149" s="5"/>
+      <c r="GV149" s="5"/>
+      <c r="GW149" s="5"/>
+      <c r="GX149" s="5"/>
+      <c r="GY149" s="5"/>
+      <c r="GZ149" s="5"/>
+      <c r="HA149" s="5"/>
+      <c r="HB149" s="5"/>
+      <c r="HC149" s="5"/>
+      <c r="HD149" s="5"/>
+      <c r="HE149" s="5"/>
+      <c r="HF149" s="5"/>
+      <c r="HG149" s="5"/>
+      <c r="HH149" s="5"/>
+      <c r="HI149" s="5"/>
+      <c r="HJ149" s="5"/>
+      <c r="HK149" s="5"/>
+      <c r="HL149" s="5"/>
+      <c r="HM149" s="5"/>
+      <c r="HN149" s="5"/>
+      <c r="HO149" s="5"/>
+      <c r="HP149" s="5"/>
+      <c r="HQ149" s="5"/>
+      <c r="HR149" s="5"/>
+      <c r="HS149" s="5"/>
+      <c r="HT149" s="5"/>
+      <c r="HU149" s="5"/>
+      <c r="HV149" s="5"/>
+      <c r="HW149" s="5"/>
+      <c r="HX149" s="5"/>
+      <c r="HY149" s="5"/>
+      <c r="HZ149" s="5"/>
+      <c r="IA149" s="5"/>
+      <c r="IB149" s="5"/>
+      <c r="IC149" s="5"/>
+      <c r="ID149" s="5"/>
+      <c r="IE149" s="5"/>
+      <c r="IF149" s="5"/>
+      <c r="IG149" s="5"/>
+      <c r="IH149" s="5"/>
+      <c r="II149" s="5"/>
+      <c r="IJ149" s="5"/>
+      <c r="IK149" s="5"/>
+      <c r="IL149" s="5"/>
+      <c r="IM149" s="5"/>
+      <c r="IN149" s="5"/>
+      <c r="IO149" s="5"/>
+      <c r="IP149" s="5"/>
+      <c r="IQ149" s="5"/>
+      <c r="IR149" s="5"/>
+      <c r="IS149" s="5"/>
+      <c r="IT149" s="5"/>
+    </row>
+    <row r="150" spans="1:254" s="2" customFormat="1">
+      <c r="A150" s="4"/>
+      <c r="B150" s="4"/>
+      <c r="C150" s="4"/>
+      <c r="D150" s="4"/>
+      <c r="E150" s="4"/>
+      <c r="F150" s="4"/>
+      <c r="G150" s="34"/>
+      <c r="H150" s="4"/>
     </row>
     <row r="151" spans="1:254">
       <c r="A151" s="7"/>
-      <c r="B151" s="7"/>
+      <c r="B151" s="6"/>
       <c r="C151" s="7"/>
       <c r="D151" s="7"/>
       <c r="E151" s="7"/>
@@ -7657,7 +7782,7 @@
     </row>
     <row r="152" spans="1:254">
       <c r="A152" s="7"/>
-      <c r="B152" s="20"/>
+      <c r="B152" s="7"/>
       <c r="C152" s="7"/>
       <c r="D152" s="7"/>
       <c r="E152" s="7"/>
@@ -7667,7 +7792,7 @@
     </row>
     <row r="153" spans="1:254">
       <c r="A153" s="7"/>
-      <c r="B153" s="7"/>
+      <c r="B153" s="20"/>
       <c r="C153" s="7"/>
       <c r="D153" s="7"/>
       <c r="E153" s="7"/>
@@ -7678,7 +7803,7 @@
     <row r="154" spans="1:254">
       <c r="A154" s="7"/>
       <c r="B154" s="7"/>
-      <c r="C154" s="4"/>
+      <c r="C154" s="7"/>
       <c r="D154" s="7"/>
       <c r="E154" s="7"/>
       <c r="F154" s="7"/>
@@ -7718,7 +7843,7 @@
     <row r="158" spans="1:254">
       <c r="A158" s="7"/>
       <c r="B158" s="7"/>
-      <c r="C158" s="7"/>
+      <c r="C158" s="4"/>
       <c r="D158" s="7"/>
       <c r="E158" s="7"/>
       <c r="F158" s="7"/>
@@ -7727,7 +7852,7 @@
     </row>
     <row r="159" spans="1:254">
       <c r="A159" s="7"/>
-      <c r="B159" s="22"/>
+      <c r="B159" s="7"/>
       <c r="C159" s="7"/>
       <c r="D159" s="7"/>
       <c r="E159" s="7"/>
@@ -7747,7 +7872,7 @@
     </row>
     <row r="161" spans="1:8">
       <c r="A161" s="7"/>
-      <c r="B161" s="7"/>
+      <c r="B161" s="22"/>
       <c r="C161" s="7"/>
       <c r="D161" s="7"/>
       <c r="E161" s="7"/>
@@ -7757,7 +7882,7 @@
     </row>
     <row r="162" spans="1:8">
       <c r="A162" s="7"/>
-      <c r="B162" s="20"/>
+      <c r="B162" s="7"/>
       <c r="C162" s="7"/>
       <c r="D162" s="7"/>
       <c r="E162" s="7"/>
@@ -7777,7 +7902,7 @@
     </row>
     <row r="164" spans="1:8">
       <c r="A164" s="7"/>
-      <c r="B164" s="7"/>
+      <c r="B164" s="20"/>
       <c r="C164" s="7"/>
       <c r="D164" s="7"/>
       <c r="E164" s="7"/>
@@ -7797,7 +7922,7 @@
     </row>
     <row r="166" spans="1:8">
       <c r="A166" s="7"/>
-      <c r="B166" s="20"/>
+      <c r="B166" s="7"/>
       <c r="C166" s="7"/>
       <c r="D166" s="7"/>
       <c r="E166" s="7"/>
@@ -7817,7 +7942,7 @@
     </row>
     <row r="168" spans="1:8">
       <c r="A168" s="7"/>
-      <c r="B168" s="7"/>
+      <c r="B168" s="20"/>
       <c r="C168" s="7"/>
       <c r="D168" s="7"/>
       <c r="E168" s="7"/>
@@ -7837,7 +7962,7 @@
     </row>
     <row r="170" spans="1:8">
       <c r="A170" s="7"/>
-      <c r="B170" s="20"/>
+      <c r="B170" s="7"/>
       <c r="C170" s="7"/>
       <c r="D170" s="7"/>
       <c r="E170" s="7"/>
@@ -7857,7 +7982,7 @@
     </row>
     <row r="172" spans="1:8">
       <c r="A172" s="7"/>
-      <c r="B172" s="7"/>
+      <c r="B172" s="20"/>
       <c r="C172" s="7"/>
       <c r="D172" s="7"/>
       <c r="E172" s="7"/>
@@ -7897,7 +8022,7 @@
     </row>
     <row r="176" spans="1:8">
       <c r="A176" s="7"/>
-      <c r="B176" s="6"/>
+      <c r="B176" s="7"/>
       <c r="C176" s="7"/>
       <c r="D176" s="7"/>
       <c r="E176" s="7"/>
@@ -7907,8 +8032,8 @@
     </row>
     <row r="177" spans="1:8">
       <c r="A177" s="7"/>
-      <c r="B177" s="4"/>
-      <c r="C177" s="4"/>
+      <c r="B177" s="6"/>
+      <c r="C177" s="7"/>
       <c r="D177" s="7"/>
       <c r="E177" s="7"/>
       <c r="F177" s="7"/>
@@ -7917,7 +8042,7 @@
     </row>
     <row r="178" spans="1:8">
       <c r="A178" s="7"/>
-      <c r="B178" s="19"/>
+      <c r="B178" s="4"/>
       <c r="C178" s="4"/>
       <c r="D178" s="7"/>
       <c r="E178" s="7"/>
@@ -7987,7 +8112,7 @@
     </row>
     <row r="185" spans="1:8">
       <c r="A185" s="7"/>
-      <c r="B185" s="4"/>
+      <c r="B185" s="19"/>
       <c r="C185" s="4"/>
       <c r="D185" s="7"/>
       <c r="E185" s="7"/>
@@ -7997,7 +8122,7 @@
     </row>
     <row r="186" spans="1:8">
       <c r="A186" s="7"/>
-      <c r="B186" s="19"/>
+      <c r="B186" s="4"/>
       <c r="C186" s="4"/>
       <c r="D186" s="7"/>
       <c r="E186" s="7"/>
@@ -8007,7 +8132,7 @@
     </row>
     <row r="187" spans="1:8">
       <c r="A187" s="7"/>
-      <c r="B187" s="21"/>
+      <c r="B187" s="19"/>
       <c r="C187" s="4"/>
       <c r="D187" s="7"/>
       <c r="E187" s="7"/>
@@ -8027,7 +8152,7 @@
     </row>
     <row r="189" spans="1:8">
       <c r="A189" s="7"/>
-      <c r="B189" s="19"/>
+      <c r="B189" s="21"/>
       <c r="C189" s="4"/>
       <c r="D189" s="7"/>
       <c r="E189" s="7"/>
@@ -8068,7 +8193,7 @@
     <row r="193" spans="1:8">
       <c r="A193" s="7"/>
       <c r="B193" s="19"/>
-      <c r="C193" s="7"/>
+      <c r="C193" s="4"/>
       <c r="D193" s="7"/>
       <c r="E193" s="7"/>
       <c r="F193" s="7"/>
@@ -8077,7 +8202,7 @@
     </row>
     <row r="194" spans="1:8">
       <c r="A194" s="7"/>
-      <c r="B194" s="4"/>
+      <c r="B194" s="19"/>
       <c r="C194" s="7"/>
       <c r="D194" s="7"/>
       <c r="E194" s="7"/>
@@ -8097,7 +8222,7 @@
     </row>
     <row r="196" spans="1:8">
       <c r="A196" s="7"/>
-      <c r="B196" s="19"/>
+      <c r="B196" s="4"/>
       <c r="C196" s="7"/>
       <c r="D196" s="7"/>
       <c r="E196" s="7"/>
@@ -8157,7 +8282,7 @@
     </row>
     <row r="202" spans="1:8">
       <c r="A202" s="7"/>
-      <c r="B202" s="21"/>
+      <c r="B202" s="19"/>
       <c r="C202" s="7"/>
       <c r="D202" s="7"/>
       <c r="E202" s="7"/>
@@ -8197,7 +8322,7 @@
     </row>
     <row r="206" spans="1:8">
       <c r="A206" s="7"/>
-      <c r="B206" s="4"/>
+      <c r="B206" s="21"/>
       <c r="C206" s="7"/>
       <c r="D206" s="7"/>
       <c r="E206" s="7"/>
@@ -8207,7 +8332,7 @@
     </row>
     <row r="207" spans="1:8">
       <c r="A207" s="7"/>
-      <c r="B207" s="6"/>
+      <c r="B207" s="4"/>
       <c r="C207" s="7"/>
       <c r="D207" s="7"/>
       <c r="E207" s="7"/>
@@ -8217,7 +8342,7 @@
     </row>
     <row r="208" spans="1:8">
       <c r="A208" s="7"/>
-      <c r="B208" s="4"/>
+      <c r="B208" s="6"/>
       <c r="C208" s="7"/>
       <c r="D208" s="7"/>
       <c r="E208" s="7"/>
@@ -8227,7 +8352,7 @@
     </row>
     <row r="209" spans="1:8">
       <c r="A209" s="7"/>
-      <c r="B209" s="19"/>
+      <c r="B209" s="4"/>
       <c r="C209" s="7"/>
       <c r="D209" s="7"/>
       <c r="E209" s="7"/>
@@ -8277,7 +8402,7 @@
     </row>
     <row r="214" spans="1:8">
       <c r="A214" s="7"/>
-      <c r="B214" s="21"/>
+      <c r="B214" s="19"/>
       <c r="C214" s="7"/>
       <c r="D214" s="7"/>
       <c r="E214" s="7"/>
@@ -8287,7 +8412,7 @@
     </row>
     <row r="215" spans="1:8">
       <c r="A215" s="7"/>
-      <c r="B215" s="19"/>
+      <c r="B215" s="21"/>
       <c r="C215" s="7"/>
       <c r="D215" s="7"/>
       <c r="E215" s="7"/>
@@ -8337,7 +8462,7 @@
     </row>
     <row r="220" spans="1:8">
       <c r="A220" s="7"/>
-      <c r="B220" s="21"/>
+      <c r="B220" s="19"/>
       <c r="C220" s="7"/>
       <c r="D220" s="7"/>
       <c r="E220" s="7"/>
@@ -8397,7 +8522,7 @@
     </row>
     <row r="226" spans="1:8">
       <c r="A226" s="7"/>
-      <c r="B226" s="4"/>
+      <c r="B226" s="21"/>
       <c r="C226" s="7"/>
       <c r="D226" s="7"/>
       <c r="E226" s="7"/>
@@ -8407,7 +8532,7 @@
     </row>
     <row r="227" spans="1:8">
       <c r="A227" s="7"/>
-      <c r="B227" s="6"/>
+      <c r="B227" s="4"/>
       <c r="C227" s="7"/>
       <c r="D227" s="7"/>
       <c r="E227" s="7"/>
@@ -8417,8 +8542,8 @@
     </row>
     <row r="228" spans="1:8">
       <c r="A228" s="7"/>
-      <c r="B228" s="4"/>
-      <c r="C228" s="4"/>
+      <c r="B228" s="6"/>
+      <c r="C228" s="7"/>
       <c r="D228" s="7"/>
       <c r="E228" s="7"/>
       <c r="F228" s="7"/>
@@ -8427,7 +8552,7 @@
     </row>
     <row r="229" spans="1:8">
       <c r="A229" s="7"/>
-      <c r="B229" s="19"/>
+      <c r="B229" s="4"/>
       <c r="C229" s="4"/>
       <c r="D229" s="7"/>
       <c r="E229" s="7"/>
@@ -8437,7 +8562,7 @@
     </row>
     <row r="230" spans="1:8">
       <c r="A230" s="7"/>
-      <c r="B230" s="7"/>
+      <c r="B230" s="19"/>
       <c r="C230" s="4"/>
       <c r="D230" s="7"/>
       <c r="E230" s="7"/>
@@ -8447,7 +8572,7 @@
     </row>
     <row r="231" spans="1:8">
       <c r="A231" s="7"/>
-      <c r="B231" s="20"/>
+      <c r="B231" s="7"/>
       <c r="C231" s="4"/>
       <c r="D231" s="7"/>
       <c r="E231" s="7"/>
@@ -8487,7 +8612,7 @@
     </row>
     <row r="235" spans="1:8">
       <c r="A235" s="7"/>
-      <c r="B235" s="7"/>
+      <c r="B235" s="20"/>
       <c r="C235" s="4"/>
       <c r="D235" s="7"/>
       <c r="E235" s="7"/>
@@ -8497,7 +8622,7 @@
     </row>
     <row r="236" spans="1:8">
       <c r="A236" s="7"/>
-      <c r="B236" s="20"/>
+      <c r="B236" s="7"/>
       <c r="C236" s="4"/>
       <c r="D236" s="7"/>
       <c r="E236" s="7"/>
@@ -8507,7 +8632,7 @@
     </row>
     <row r="237" spans="1:8">
       <c r="A237" s="7"/>
-      <c r="B237" s="23"/>
+      <c r="B237" s="20"/>
       <c r="C237" s="4"/>
       <c r="D237" s="7"/>
       <c r="E237" s="7"/>
@@ -8527,7 +8652,7 @@
     </row>
     <row r="239" spans="1:8">
       <c r="A239" s="7"/>
-      <c r="B239" s="20"/>
+      <c r="B239" s="23"/>
       <c r="C239" s="4"/>
       <c r="D239" s="7"/>
       <c r="E239" s="7"/>
@@ -8567,7 +8692,7 @@
     </row>
     <row r="243" spans="1:8">
       <c r="A243" s="7"/>
-      <c r="B243" s="7"/>
+      <c r="B243" s="20"/>
       <c r="C243" s="4"/>
       <c r="D243" s="7"/>
       <c r="E243" s="7"/>
@@ -8577,7 +8702,7 @@
     </row>
     <row r="244" spans="1:8">
       <c r="A244" s="7"/>
-      <c r="B244" s="20"/>
+      <c r="B244" s="7"/>
       <c r="C244" s="4"/>
       <c r="D244" s="7"/>
       <c r="E244" s="7"/>
@@ -8627,7 +8752,7 @@
     </row>
     <row r="249" spans="1:8">
       <c r="A249" s="7"/>
-      <c r="B249" s="7"/>
+      <c r="B249" s="20"/>
       <c r="C249" s="4"/>
       <c r="D249" s="7"/>
       <c r="E249" s="7"/>
@@ -8637,8 +8762,8 @@
     </row>
     <row r="250" spans="1:8">
       <c r="A250" s="7"/>
-      <c r="B250" s="20"/>
-      <c r="C250" s="7"/>
+      <c r="B250" s="7"/>
+      <c r="C250" s="4"/>
       <c r="D250" s="7"/>
       <c r="E250" s="7"/>
       <c r="F250" s="7"/>
@@ -8647,7 +8772,7 @@
     </row>
     <row r="251" spans="1:8">
       <c r="A251" s="7"/>
-      <c r="B251" s="7"/>
+      <c r="B251" s="20"/>
       <c r="C251" s="7"/>
       <c r="D251" s="7"/>
       <c r="E251" s="7"/>
@@ -8657,7 +8782,7 @@
     </row>
     <row r="252" spans="1:8">
       <c r="A252" s="7"/>
-      <c r="B252" s="20"/>
+      <c r="B252" s="7"/>
       <c r="C252" s="7"/>
       <c r="D252" s="7"/>
       <c r="E252" s="7"/>
@@ -8667,7 +8792,7 @@
     </row>
     <row r="253" spans="1:8">
       <c r="A253" s="7"/>
-      <c r="B253" s="23"/>
+      <c r="B253" s="20"/>
       <c r="C253" s="7"/>
       <c r="D253" s="7"/>
       <c r="E253" s="7"/>
@@ -8717,8 +8842,8 @@
     </row>
     <row r="258" spans="1:8">
       <c r="A258" s="7"/>
-      <c r="B258" s="20"/>
-      <c r="C258" s="4"/>
+      <c r="B258" s="23"/>
+      <c r="C258" s="7"/>
       <c r="D258" s="7"/>
       <c r="E258" s="7"/>
       <c r="F258" s="7"/>
@@ -8727,7 +8852,7 @@
     </row>
     <row r="259" spans="1:8">
       <c r="A259" s="7"/>
-      <c r="B259" s="23"/>
+      <c r="B259" s="20"/>
       <c r="C259" s="4"/>
       <c r="D259" s="7"/>
       <c r="E259" s="7"/>
@@ -8737,7 +8862,7 @@
     </row>
     <row r="260" spans="1:8">
       <c r="A260" s="7"/>
-      <c r="B260" s="24"/>
+      <c r="B260" s="23"/>
       <c r="C260" s="4"/>
       <c r="D260" s="7"/>
       <c r="E260" s="7"/>
@@ -8765,9 +8890,9 @@
       <c r="G262" s="30"/>
       <c r="H262" s="7"/>
     </row>
-    <row r="263" spans="1:8" ht="11.25">
+    <row r="263" spans="1:8">
       <c r="A263" s="7"/>
-      <c r="B263" s="25"/>
+      <c r="B263" s="24"/>
       <c r="C263" s="4"/>
       <c r="D263" s="7"/>
       <c r="E263" s="7"/>
@@ -8775,9 +8900,9 @@
       <c r="G263" s="30"/>
       <c r="H263" s="7"/>
     </row>
-    <row r="264" spans="1:8">
+    <row r="264" spans="1:8" ht="11.25">
       <c r="A264" s="7"/>
-      <c r="B264" s="23"/>
+      <c r="B264" s="25"/>
       <c r="C264" s="4"/>
       <c r="D264" s="7"/>
       <c r="E264" s="7"/>
@@ -8817,7 +8942,7 @@
     </row>
     <row r="268" spans="1:8">
       <c r="A268" s="7"/>
-      <c r="B268" s="24"/>
+      <c r="B268" s="23"/>
       <c r="C268" s="4"/>
       <c r="D268" s="7"/>
       <c r="E268" s="7"/>
@@ -8847,7 +8972,7 @@
     </row>
     <row r="271" spans="1:8">
       <c r="A271" s="7"/>
-      <c r="B271" s="23"/>
+      <c r="B271" s="24"/>
       <c r="C271" s="4"/>
       <c r="D271" s="7"/>
       <c r="E271" s="7"/>
@@ -8857,7 +8982,7 @@
     </row>
     <row r="272" spans="1:8">
       <c r="A272" s="7"/>
-      <c r="B272" s="24"/>
+      <c r="B272" s="23"/>
       <c r="C272" s="4"/>
       <c r="D272" s="7"/>
       <c r="E272" s="7"/>
@@ -8865,15 +8990,15 @@
       <c r="G272" s="30"/>
       <c r="H272" s="7"/>
     </row>
-    <row r="273" spans="1:8" s="2" customFormat="1">
-      <c r="A273" s="4"/>
+    <row r="273" spans="1:8">
+      <c r="A273" s="7"/>
       <c r="B273" s="24"/>
       <c r="C273" s="4"/>
-      <c r="D273" s="4"/>
-      <c r="E273" s="4"/>
-      <c r="F273" s="4"/>
-      <c r="G273" s="34"/>
-      <c r="H273" s="4"/>
+      <c r="D273" s="7"/>
+      <c r="E273" s="7"/>
+      <c r="F273" s="7"/>
+      <c r="G273" s="30"/>
+      <c r="H273" s="7"/>
     </row>
     <row r="274" spans="1:8" s="2" customFormat="1">
       <c r="A274" s="4"/>
@@ -8885,19 +9010,19 @@
       <c r="G274" s="34"/>
       <c r="H274" s="4"/>
     </row>
-    <row r="275" spans="1:8">
-      <c r="A275" s="7"/>
+    <row r="275" spans="1:8" s="2" customFormat="1">
+      <c r="A275" s="4"/>
       <c r="B275" s="24"/>
       <c r="C275" s="4"/>
-      <c r="D275" s="7"/>
-      <c r="E275" s="7"/>
-      <c r="F275" s="7"/>
-      <c r="G275" s="30"/>
-      <c r="H275" s="7"/>
+      <c r="D275" s="4"/>
+      <c r="E275" s="4"/>
+      <c r="F275" s="4"/>
+      <c r="G275" s="34"/>
+      <c r="H275" s="4"/>
     </row>
     <row r="276" spans="1:8">
       <c r="A276" s="7"/>
-      <c r="B276" s="23"/>
+      <c r="B276" s="24"/>
       <c r="C276" s="4"/>
       <c r="D276" s="7"/>
       <c r="E276" s="7"/>
@@ -8907,7 +9032,7 @@
     </row>
     <row r="277" spans="1:8">
       <c r="A277" s="7"/>
-      <c r="B277" s="24"/>
+      <c r="B277" s="23"/>
       <c r="C277" s="4"/>
       <c r="D277" s="7"/>
       <c r="E277" s="7"/>
@@ -8937,7 +9062,7 @@
     </row>
     <row r="280" spans="1:8">
       <c r="A280" s="7"/>
-      <c r="B280" s="22"/>
+      <c r="B280" s="24"/>
       <c r="C280" s="4"/>
       <c r="D280" s="7"/>
       <c r="E280" s="7"/>
@@ -8947,7 +9072,7 @@
     </row>
     <row r="281" spans="1:8">
       <c r="A281" s="7"/>
-      <c r="B281" s="7"/>
+      <c r="B281" s="22"/>
       <c r="C281" s="4"/>
       <c r="D281" s="7"/>
       <c r="E281" s="7"/>
@@ -8967,7 +9092,7 @@
     </row>
     <row r="283" spans="1:8">
       <c r="A283" s="7"/>
-      <c r="B283" s="20"/>
+      <c r="B283" s="7"/>
       <c r="C283" s="4"/>
       <c r="D283" s="7"/>
       <c r="E283" s="7"/>
@@ -8987,7 +9112,7 @@
     </row>
     <row r="285" spans="1:8">
       <c r="A285" s="7"/>
-      <c r="B285" s="7"/>
+      <c r="B285" s="20"/>
       <c r="C285" s="4"/>
       <c r="D285" s="7"/>
       <c r="E285" s="7"/>
@@ -9018,7 +9143,7 @@
     <row r="288" spans="1:8">
       <c r="A288" s="7"/>
       <c r="B288" s="7"/>
-      <c r="C288" s="7"/>
+      <c r="C288" s="4"/>
       <c r="D288" s="7"/>
       <c r="E288" s="7"/>
       <c r="F288" s="7"/>
@@ -9027,7 +9152,7 @@
     </row>
     <row r="289" spans="1:8">
       <c r="A289" s="7"/>
-      <c r="B289" s="6"/>
+      <c r="B289" s="7"/>
       <c r="C289" s="7"/>
       <c r="D289" s="7"/>
       <c r="E289" s="7"/>
@@ -9037,7 +9162,7 @@
     </row>
     <row r="290" spans="1:8">
       <c r="A290" s="7"/>
-      <c r="B290" s="7"/>
+      <c r="B290" s="6"/>
       <c r="C290" s="7"/>
       <c r="D290" s="7"/>
       <c r="E290" s="7"/>
@@ -9117,7 +9242,7 @@
     </row>
     <row r="298" spans="1:8">
       <c r="A298" s="7"/>
-      <c r="B298" s="6"/>
+      <c r="B298" s="7"/>
       <c r="C298" s="7"/>
       <c r="D298" s="7"/>
       <c r="E298" s="7"/>
@@ -9127,8 +9252,8 @@
     </row>
     <row r="299" spans="1:8">
       <c r="A299" s="7"/>
-      <c r="B299" s="4"/>
-      <c r="C299" s="4"/>
+      <c r="B299" s="6"/>
+      <c r="C299" s="7"/>
       <c r="D299" s="7"/>
       <c r="E299" s="7"/>
       <c r="F299" s="7"/>
@@ -9137,7 +9262,7 @@
     </row>
     <row r="300" spans="1:8">
       <c r="A300" s="7"/>
-      <c r="B300" s="19"/>
+      <c r="B300" s="4"/>
       <c r="C300" s="4"/>
       <c r="D300" s="7"/>
       <c r="E300" s="7"/>
@@ -9167,7 +9292,7 @@
     </row>
     <row r="303" spans="1:8">
       <c r="A303" s="7"/>
-      <c r="B303" s="4"/>
+      <c r="B303" s="19"/>
       <c r="C303" s="4"/>
       <c r="D303" s="7"/>
       <c r="E303" s="7"/>
@@ -9227,7 +9352,7 @@
     </row>
     <row r="309" spans="1:8">
       <c r="A309" s="7"/>
-      <c r="B309" s="19"/>
+      <c r="B309" s="4"/>
       <c r="C309" s="4"/>
       <c r="D309" s="7"/>
       <c r="E309" s="7"/>
@@ -9247,7 +9372,7 @@
     </row>
     <row r="311" spans="1:8">
       <c r="A311" s="7"/>
-      <c r="B311" s="21"/>
+      <c r="B311" s="19"/>
       <c r="C311" s="4"/>
       <c r="D311" s="7"/>
       <c r="E311" s="7"/>
@@ -9257,8 +9382,8 @@
     </row>
     <row r="312" spans="1:8">
       <c r="A312" s="7"/>
-      <c r="B312" s="7"/>
-      <c r="C312" s="7"/>
+      <c r="B312" s="21"/>
+      <c r="C312" s="4"/>
       <c r="D312" s="7"/>
       <c r="E312" s="7"/>
       <c r="F312" s="7"/>
@@ -9267,7 +9392,7 @@
     </row>
     <row r="313" spans="1:8">
       <c r="A313" s="7"/>
-      <c r="B313" s="6"/>
+      <c r="B313" s="7"/>
       <c r="C313" s="7"/>
       <c r="D313" s="7"/>
       <c r="E313" s="7"/>
@@ -9275,15 +9400,15 @@
       <c r="G313" s="30"/>
       <c r="H313" s="7"/>
     </row>
-    <row r="314" spans="1:8" s="2" customFormat="1">
-      <c r="A314" s="4"/>
-      <c r="B314" s="4"/>
-      <c r="C314" s="9"/>
-      <c r="D314" s="4"/>
-      <c r="E314" s="4"/>
-      <c r="F314" s="4"/>
-      <c r="G314" s="34"/>
-      <c r="H314" s="4"/>
+    <row r="314" spans="1:8">
+      <c r="A314" s="7"/>
+      <c r="B314" s="6"/>
+      <c r="C314" s="7"/>
+      <c r="D314" s="7"/>
+      <c r="E314" s="7"/>
+      <c r="F314" s="7"/>
+      <c r="G314" s="30"/>
+      <c r="H314" s="7"/>
     </row>
     <row r="315" spans="1:8" s="2" customFormat="1">
       <c r="A315" s="4"/>
@@ -9307,7 +9432,7 @@
     </row>
     <row r="317" spans="1:8" s="2" customFormat="1">
       <c r="A317" s="4"/>
-      <c r="B317" s="19"/>
+      <c r="B317" s="4"/>
       <c r="C317" s="9"/>
       <c r="D317" s="4"/>
       <c r="E317" s="4"/>
@@ -9357,8 +9482,8 @@
     </row>
     <row r="322" spans="1:8" s="2" customFormat="1">
       <c r="A322" s="4"/>
-      <c r="B322" s="26"/>
-      <c r="C322" s="4"/>
+      <c r="B322" s="19"/>
+      <c r="C322" s="9"/>
       <c r="D322" s="4"/>
       <c r="E322" s="4"/>
       <c r="F322" s="4"/>
@@ -9407,7 +9532,7 @@
     </row>
     <row r="327" spans="1:8" s="2" customFormat="1">
       <c r="A327" s="4"/>
-      <c r="B327" s="21"/>
+      <c r="B327" s="26"/>
       <c r="C327" s="4"/>
       <c r="D327" s="4"/>
       <c r="E327" s="4"/>
@@ -9457,7 +9582,7 @@
     </row>
     <row r="332" spans="1:8" s="2" customFormat="1">
       <c r="A332" s="4"/>
-      <c r="B332" s="19"/>
+      <c r="B332" s="21"/>
       <c r="C332" s="4"/>
       <c r="D332" s="4"/>
       <c r="E332" s="4"/>
@@ -9467,7 +9592,7 @@
     </row>
     <row r="333" spans="1:8" s="2" customFormat="1">
       <c r="A333" s="4"/>
-      <c r="B333" s="21"/>
+      <c r="B333" s="19"/>
       <c r="C333" s="4"/>
       <c r="D333" s="4"/>
       <c r="E333" s="4"/>
@@ -9477,7 +9602,7 @@
     </row>
     <row r="334" spans="1:8" s="2" customFormat="1">
       <c r="A334" s="4"/>
-      <c r="B334" s="4"/>
+      <c r="B334" s="21"/>
       <c r="C334" s="4"/>
       <c r="D334" s="4"/>
       <c r="E334" s="4"/>
@@ -9485,20 +9610,20 @@
       <c r="G334" s="34"/>
       <c r="H334" s="4"/>
     </row>
-    <row r="335" spans="1:8">
-      <c r="A335" s="7"/>
-      <c r="B335" s="6"/>
-      <c r="C335" s="7"/>
-      <c r="D335" s="7"/>
-      <c r="E335" s="7"/>
-      <c r="F335" s="7"/>
-      <c r="G335" s="30"/>
-      <c r="H335" s="7"/>
+    <row r="335" spans="1:8" s="2" customFormat="1">
+      <c r="A335" s="4"/>
+      <c r="B335" s="4"/>
+      <c r="C335" s="4"/>
+      <c r="D335" s="4"/>
+      <c r="E335" s="4"/>
+      <c r="F335" s="4"/>
+      <c r="G335" s="34"/>
+      <c r="H335" s="4"/>
     </row>
     <row r="336" spans="1:8">
       <c r="A336" s="7"/>
-      <c r="B336" s="7"/>
-      <c r="C336" s="4"/>
+      <c r="B336" s="6"/>
+      <c r="C336" s="7"/>
       <c r="D336" s="7"/>
       <c r="E336" s="7"/>
       <c r="F336" s="7"/>
@@ -9567,7 +9692,7 @@
     </row>
     <row r="343" spans="1:8">
       <c r="A343" s="7"/>
-      <c r="B343" s="4"/>
+      <c r="B343" s="7"/>
       <c r="C343" s="4"/>
       <c r="D343" s="7"/>
       <c r="E343" s="7"/>
@@ -9578,7 +9703,7 @@
     <row r="344" spans="1:8">
       <c r="A344" s="7"/>
       <c r="B344" s="4"/>
-      <c r="C344" s="7"/>
+      <c r="C344" s="4"/>
       <c r="D344" s="7"/>
       <c r="E344" s="7"/>
       <c r="F344" s="7"/>
@@ -9587,7 +9712,7 @@
     </row>
     <row r="345" spans="1:8">
       <c r="A345" s="7"/>
-      <c r="B345" s="6"/>
+      <c r="B345" s="4"/>
       <c r="C345" s="7"/>
       <c r="D345" s="7"/>
       <c r="E345" s="7"/>
@@ -9597,7 +9722,7 @@
     </row>
     <row r="346" spans="1:8">
       <c r="A346" s="7"/>
-      <c r="B346" s="7"/>
+      <c r="B346" s="6"/>
       <c r="C346" s="7"/>
       <c r="D346" s="7"/>
       <c r="E346" s="7"/>
@@ -9607,7 +9732,7 @@
     </row>
     <row r="347" spans="1:8">
       <c r="A347" s="7"/>
-      <c r="B347" s="22"/>
+      <c r="B347" s="7"/>
       <c r="C347" s="7"/>
       <c r="D347" s="7"/>
       <c r="E347" s="7"/>
@@ -9617,7 +9742,7 @@
     </row>
     <row r="348" spans="1:8">
       <c r="A348" s="7"/>
-      <c r="B348" s="7"/>
+      <c r="B348" s="22"/>
       <c r="C348" s="7"/>
       <c r="D348" s="7"/>
       <c r="E348" s="7"/>
@@ -9657,7 +9782,7 @@
     </row>
     <row r="352" spans="1:8">
       <c r="A352" s="7"/>
-      <c r="B352" s="6"/>
+      <c r="B352" s="7"/>
       <c r="C352" s="7"/>
       <c r="D352" s="7"/>
       <c r="E352" s="7"/>
@@ -9667,7 +9792,7 @@
     </row>
     <row r="353" spans="1:8">
       <c r="A353" s="7"/>
-      <c r="B353" s="7"/>
+      <c r="B353" s="6"/>
       <c r="C353" s="7"/>
       <c r="D353" s="7"/>
       <c r="E353" s="7"/>
@@ -9677,7 +9802,7 @@
     </row>
     <row r="354" spans="1:8">
       <c r="A354" s="7"/>
-      <c r="B354" s="20"/>
+      <c r="B354" s="7"/>
       <c r="C354" s="7"/>
       <c r="D354" s="7"/>
       <c r="E354" s="7"/>
@@ -9707,7 +9832,7 @@
     </row>
     <row r="357" spans="1:8">
       <c r="A357" s="7"/>
-      <c r="B357" s="22"/>
+      <c r="B357" s="20"/>
       <c r="C357" s="7"/>
       <c r="D357" s="7"/>
       <c r="E357" s="7"/>
@@ -9717,7 +9842,7 @@
     </row>
     <row r="358" spans="1:8">
       <c r="A358" s="7"/>
-      <c r="B358" s="20"/>
+      <c r="B358" s="22"/>
       <c r="C358" s="7"/>
       <c r="D358" s="7"/>
       <c r="E358" s="7"/>
@@ -9737,7 +9862,7 @@
     </row>
     <row r="360" spans="1:8">
       <c r="A360" s="7"/>
-      <c r="B360" s="22"/>
+      <c r="B360" s="20"/>
       <c r="C360" s="7"/>
       <c r="D360" s="7"/>
       <c r="E360" s="7"/>
@@ -9747,7 +9872,7 @@
     </row>
     <row r="361" spans="1:8">
       <c r="A361" s="7"/>
-      <c r="B361" s="20"/>
+      <c r="B361" s="22"/>
       <c r="C361" s="7"/>
       <c r="D361" s="7"/>
       <c r="E361" s="7"/>
@@ -9757,7 +9882,7 @@
     </row>
     <row r="362" spans="1:8">
       <c r="A362" s="7"/>
-      <c r="B362" s="22"/>
+      <c r="B362" s="20"/>
       <c r="C362" s="7"/>
       <c r="D362" s="7"/>
       <c r="E362" s="7"/>
@@ -9767,7 +9892,7 @@
     </row>
     <row r="363" spans="1:8">
       <c r="A363" s="7"/>
-      <c r="B363" s="20"/>
+      <c r="B363" s="22"/>
       <c r="C363" s="7"/>
       <c r="D363" s="7"/>
       <c r="E363" s="7"/>
@@ -9797,7 +9922,7 @@
     </row>
     <row r="366" spans="1:8">
       <c r="A366" s="7"/>
-      <c r="B366" s="7"/>
+      <c r="B366" s="20"/>
       <c r="C366" s="7"/>
       <c r="D366" s="7"/>
       <c r="E366" s="7"/>
@@ -9807,7 +9932,7 @@
     </row>
     <row r="367" spans="1:8">
       <c r="A367" s="7"/>
-      <c r="B367" s="27"/>
+      <c r="B367" s="7"/>
       <c r="C367" s="7"/>
       <c r="D367" s="7"/>
       <c r="E367" s="7"/>
@@ -9817,7 +9942,7 @@
     </row>
     <row r="368" spans="1:8">
       <c r="A368" s="7"/>
-      <c r="B368" s="22"/>
+      <c r="B368" s="27"/>
       <c r="C368" s="7"/>
       <c r="D368" s="7"/>
       <c r="E368" s="7"/>
@@ -9827,8 +9952,8 @@
     </row>
     <row r="369" spans="1:8">
       <c r="A369" s="7"/>
-      <c r="B369" s="7"/>
-      <c r="C369" s="4"/>
+      <c r="B369" s="22"/>
+      <c r="C369" s="7"/>
       <c r="D369" s="7"/>
       <c r="E369" s="7"/>
       <c r="F369" s="7"/>
@@ -9837,7 +9962,7 @@
     </row>
     <row r="370" spans="1:8">
       <c r="A370" s="7"/>
-      <c r="B370" s="20"/>
+      <c r="B370" s="7"/>
       <c r="C370" s="4"/>
       <c r="D370" s="7"/>
       <c r="E370" s="7"/>
@@ -9867,7 +9992,7 @@
     </row>
     <row r="373" spans="1:8">
       <c r="A373" s="7"/>
-      <c r="B373" s="7"/>
+      <c r="B373" s="20"/>
       <c r="C373" s="4"/>
       <c r="D373" s="7"/>
       <c r="E373" s="7"/>
@@ -9897,7 +10022,7 @@
     </row>
     <row r="376" spans="1:8">
       <c r="A376" s="7"/>
-      <c r="B376" s="20"/>
+      <c r="B376" s="7"/>
       <c r="C376" s="4"/>
       <c r="D376" s="7"/>
       <c r="E376" s="7"/>
@@ -9917,8 +10042,8 @@
     </row>
     <row r="378" spans="1:8">
       <c r="A378" s="7"/>
-      <c r="B378" s="7"/>
-      <c r="C378" s="7"/>
+      <c r="B378" s="20"/>
+      <c r="C378" s="4"/>
       <c r="D378" s="7"/>
       <c r="E378" s="7"/>
       <c r="F378" s="7"/>
@@ -9927,7 +10052,7 @@
     </row>
     <row r="379" spans="1:8">
       <c r="A379" s="7"/>
-      <c r="B379" s="6"/>
+      <c r="B379" s="7"/>
       <c r="C379" s="7"/>
       <c r="D379" s="7"/>
       <c r="E379" s="7"/>
@@ -9937,7 +10062,7 @@
     </row>
     <row r="380" spans="1:8">
       <c r="A380" s="7"/>
-      <c r="B380" s="7"/>
+      <c r="B380" s="6"/>
       <c r="C380" s="7"/>
       <c r="D380" s="7"/>
       <c r="E380" s="7"/>
@@ -9997,7 +10122,7 @@
     </row>
     <row r="386" spans="1:8">
       <c r="A386" s="7"/>
-      <c r="B386" s="6"/>
+      <c r="B386" s="7"/>
       <c r="C386" s="7"/>
       <c r="D386" s="7"/>
       <c r="E386" s="7"/>
@@ -10007,7 +10132,7 @@
     </row>
     <row r="387" spans="1:8">
       <c r="A387" s="7"/>
-      <c r="B387" s="7"/>
+      <c r="B387" s="6"/>
       <c r="C387" s="7"/>
       <c r="D387" s="7"/>
       <c r="E387" s="7"/>
@@ -10028,7 +10153,7 @@
     <row r="389" spans="1:8">
       <c r="A389" s="7"/>
       <c r="B389" s="7"/>
-      <c r="C389" s="4"/>
+      <c r="C389" s="7"/>
       <c r="D389" s="7"/>
       <c r="E389" s="7"/>
       <c r="F389" s="7"/>
@@ -10037,7 +10162,7 @@
     </row>
     <row r="390" spans="1:8">
       <c r="A390" s="7"/>
-      <c r="B390" s="20"/>
+      <c r="B390" s="7"/>
       <c r="C390" s="4"/>
       <c r="D390" s="7"/>
       <c r="E390" s="7"/>
@@ -10048,7 +10173,7 @@
     <row r="391" spans="1:8">
       <c r="A391" s="7"/>
       <c r="B391" s="20"/>
-      <c r="C391" s="7"/>
+      <c r="C391" s="4"/>
       <c r="D391" s="7"/>
       <c r="E391" s="7"/>
       <c r="F391" s="7"/>
@@ -10057,7 +10182,7 @@
     </row>
     <row r="392" spans="1:8">
       <c r="A392" s="7"/>
-      <c r="B392" s="27"/>
+      <c r="B392" s="20"/>
       <c r="C392" s="7"/>
       <c r="D392" s="7"/>
       <c r="E392" s="7"/>
@@ -10067,7 +10192,7 @@
     </row>
     <row r="393" spans="1:8">
       <c r="A393" s="7"/>
-      <c r="B393" s="22"/>
+      <c r="B393" s="27"/>
       <c r="C393" s="7"/>
       <c r="D393" s="7"/>
       <c r="E393" s="7"/>
@@ -10117,7 +10242,7 @@
     </row>
     <row r="398" spans="1:8">
       <c r="A398" s="7"/>
-      <c r="B398" s="7"/>
+      <c r="B398" s="22"/>
       <c r="C398" s="7"/>
       <c r="D398" s="7"/>
       <c r="E398" s="7"/>
@@ -10127,7 +10252,7 @@
     </row>
     <row r="399" spans="1:8">
       <c r="A399" s="7"/>
-      <c r="B399" s="6"/>
+      <c r="B399" s="7"/>
       <c r="C399" s="7"/>
       <c r="D399" s="7"/>
       <c r="E399" s="7"/>
@@ -10137,7 +10262,7 @@
     </row>
     <row r="400" spans="1:8">
       <c r="A400" s="7"/>
-      <c r="B400" s="7"/>
+      <c r="B400" s="6"/>
       <c r="C400" s="7"/>
       <c r="D400" s="7"/>
       <c r="E400" s="7"/>
@@ -10147,7 +10272,7 @@
     </row>
     <row r="401" spans="1:8">
       <c r="A401" s="7"/>
-      <c r="B401" s="20"/>
+      <c r="B401" s="7"/>
       <c r="C401" s="7"/>
       <c r="D401" s="7"/>
       <c r="E401" s="7"/>
@@ -10157,7 +10282,7 @@
     </row>
     <row r="402" spans="1:8">
       <c r="A402" s="7"/>
-      <c r="B402" s="22"/>
+      <c r="B402" s="20"/>
       <c r="C402" s="7"/>
       <c r="D402" s="7"/>
       <c r="E402" s="7"/>
@@ -10177,7 +10302,7 @@
     </row>
     <row r="404" spans="1:8">
       <c r="A404" s="7"/>
-      <c r="B404" s="20"/>
+      <c r="B404" s="22"/>
       <c r="C404" s="7"/>
       <c r="D404" s="7"/>
       <c r="E404" s="7"/>
@@ -10217,7 +10342,7 @@
     </row>
     <row r="408" spans="1:8">
       <c r="A408" s="7"/>
-      <c r="B408" s="7"/>
+      <c r="B408" s="20"/>
       <c r="C408" s="7"/>
       <c r="D408" s="7"/>
       <c r="E408" s="7"/>
@@ -10227,7 +10352,7 @@
     </row>
     <row r="409" spans="1:8">
       <c r="A409" s="7"/>
-      <c r="B409" s="20"/>
+      <c r="B409" s="7"/>
       <c r="C409" s="7"/>
       <c r="D409" s="7"/>
       <c r="E409" s="7"/>
@@ -10247,7 +10372,7 @@
     </row>
     <row r="411" spans="1:8">
       <c r="A411" s="7"/>
-      <c r="B411" s="22"/>
+      <c r="B411" s="20"/>
       <c r="C411" s="7"/>
       <c r="D411" s="7"/>
       <c r="E411" s="7"/>
@@ -10257,7 +10382,7 @@
     </row>
     <row r="412" spans="1:8">
       <c r="A412" s="7"/>
-      <c r="B412" s="7"/>
+      <c r="B412" s="22"/>
       <c r="C412" s="7"/>
       <c r="D412" s="7"/>
       <c r="E412" s="7"/>
@@ -10267,7 +10392,7 @@
     </row>
     <row r="413" spans="1:8">
       <c r="A413" s="7"/>
-      <c r="B413" s="6"/>
+      <c r="B413" s="7"/>
       <c r="C413" s="7"/>
       <c r="D413" s="7"/>
       <c r="E413" s="7"/>
@@ -10277,7 +10402,7 @@
     </row>
     <row r="414" spans="1:8">
       <c r="A414" s="7"/>
-      <c r="B414" s="7"/>
+      <c r="B414" s="6"/>
       <c r="C414" s="7"/>
       <c r="D414" s="7"/>
       <c r="E414" s="7"/>
@@ -10297,7 +10422,7 @@
     </row>
     <row r="416" spans="1:8">
       <c r="A416" s="7"/>
-      <c r="B416" s="6"/>
+      <c r="B416" s="7"/>
       <c r="C416" s="7"/>
       <c r="D416" s="7"/>
       <c r="E416" s="7"/>
@@ -10307,7 +10432,7 @@
     </row>
     <row r="417" spans="1:8">
       <c r="A417" s="7"/>
-      <c r="B417" s="7"/>
+      <c r="B417" s="6"/>
       <c r="C417" s="7"/>
       <c r="D417" s="7"/>
       <c r="E417" s="7"/>
@@ -10317,7 +10442,7 @@
     </row>
     <row r="418" spans="1:8">
       <c r="A418" s="7"/>
-      <c r="B418" s="20"/>
+      <c r="B418" s="7"/>
       <c r="C418" s="7"/>
       <c r="D418" s="7"/>
       <c r="E418" s="7"/>
@@ -10337,7 +10462,7 @@
     </row>
     <row r="420" spans="1:8">
       <c r="A420" s="7"/>
-      <c r="B420" s="7"/>
+      <c r="B420" s="20"/>
       <c r="C420" s="7"/>
       <c r="D420" s="7"/>
       <c r="E420" s="7"/>
@@ -10347,7 +10472,7 @@
     </row>
     <row r="421" spans="1:8">
       <c r="A421" s="7"/>
-      <c r="B421" s="6"/>
+      <c r="B421" s="7"/>
       <c r="C421" s="7"/>
       <c r="D421" s="7"/>
       <c r="E421" s="7"/>
@@ -10357,7 +10482,7 @@
     </row>
     <row r="422" spans="1:8">
       <c r="A422" s="7"/>
-      <c r="B422" s="7"/>
+      <c r="B422" s="6"/>
       <c r="C422" s="7"/>
       <c r="D422" s="7"/>
       <c r="E422" s="7"/>
@@ -10407,7 +10532,7 @@
     </row>
     <row r="427" spans="1:8">
       <c r="A427" s="7"/>
-      <c r="B427" s="6"/>
+      <c r="B427" s="7"/>
       <c r="C427" s="7"/>
       <c r="D427" s="7"/>
       <c r="E427" s="7"/>
@@ -10417,7 +10542,7 @@
     </row>
     <row r="428" spans="1:8">
       <c r="A428" s="7"/>
-      <c r="B428" s="7"/>
+      <c r="B428" s="6"/>
       <c r="C428" s="7"/>
       <c r="D428" s="7"/>
       <c r="E428" s="7"/>
@@ -10477,7 +10602,7 @@
     </row>
     <row r="434" spans="1:8">
       <c r="A434" s="7"/>
-      <c r="B434" s="6"/>
+      <c r="B434" s="7"/>
       <c r="C434" s="7"/>
       <c r="D434" s="7"/>
       <c r="E434" s="7"/>
@@ -10487,7 +10612,7 @@
     </row>
     <row r="435" spans="1:8">
       <c r="A435" s="7"/>
-      <c r="B435" s="7"/>
+      <c r="B435" s="6"/>
       <c r="C435" s="7"/>
       <c r="D435" s="7"/>
       <c r="E435" s="7"/>
@@ -10507,7 +10632,7 @@
     </row>
     <row r="437" spans="1:8">
       <c r="A437" s="7"/>
-      <c r="B437" s="6"/>
+      <c r="B437" s="7"/>
       <c r="C437" s="7"/>
       <c r="D437" s="7"/>
       <c r="E437" s="7"/>
@@ -10517,7 +10642,7 @@
     </row>
     <row r="438" spans="1:8">
       <c r="A438" s="7"/>
-      <c r="B438" s="4"/>
+      <c r="B438" s="6"/>
       <c r="C438" s="7"/>
       <c r="D438" s="7"/>
       <c r="E438" s="7"/>
@@ -10537,7 +10662,7 @@
     </row>
     <row r="440" spans="1:8">
       <c r="A440" s="7"/>
-      <c r="B440" s="7"/>
+      <c r="B440" s="4"/>
       <c r="C440" s="7"/>
       <c r="D440" s="7"/>
       <c r="E440" s="7"/>
@@ -10567,7 +10692,7 @@
     </row>
     <row r="443" spans="1:8">
       <c r="A443" s="7"/>
-      <c r="B443" s="6"/>
+      <c r="B443" s="7"/>
       <c r="C443" s="7"/>
       <c r="D443" s="7"/>
       <c r="E443" s="7"/>
@@ -10577,8 +10702,8 @@
     </row>
     <row r="444" spans="1:8">
       <c r="A444" s="7"/>
-      <c r="B444" s="7"/>
-      <c r="C444" s="4"/>
+      <c r="B444" s="6"/>
+      <c r="C444" s="7"/>
       <c r="D444" s="7"/>
       <c r="E444" s="7"/>
       <c r="F444" s="7"/>
@@ -10628,7 +10753,7 @@
     <row r="449" spans="1:8">
       <c r="A449" s="7"/>
       <c r="B449" s="7"/>
-      <c r="C449" s="7"/>
+      <c r="C449" s="4"/>
       <c r="D449" s="7"/>
       <c r="E449" s="7"/>
       <c r="F449" s="7"/>
@@ -10637,7 +10762,7 @@
     </row>
     <row r="450" spans="1:8">
       <c r="A450" s="7"/>
-      <c r="B450" s="6"/>
+      <c r="B450" s="7"/>
       <c r="C450" s="7"/>
       <c r="D450" s="7"/>
       <c r="E450" s="7"/>
@@ -10647,8 +10772,8 @@
     </row>
     <row r="451" spans="1:8">
       <c r="A451" s="7"/>
-      <c r="B451" s="7"/>
-      <c r="C451" s="4"/>
+      <c r="B451" s="6"/>
+      <c r="C451" s="7"/>
       <c r="D451" s="7"/>
       <c r="E451" s="7"/>
       <c r="F451" s="7"/>
@@ -10688,7 +10813,7 @@
     <row r="455" spans="1:8">
       <c r="A455" s="7"/>
       <c r="B455" s="7"/>
-      <c r="C455" s="7"/>
+      <c r="C455" s="4"/>
       <c r="D455" s="7"/>
       <c r="E455" s="7"/>
       <c r="F455" s="7"/>
@@ -10697,7 +10822,7 @@
     </row>
     <row r="456" spans="1:8">
       <c r="A456" s="7"/>
-      <c r="B456" s="6"/>
+      <c r="B456" s="7"/>
       <c r="C456" s="7"/>
       <c r="D456" s="7"/>
       <c r="E456" s="7"/>
@@ -10707,7 +10832,7 @@
     </row>
     <row r="457" spans="1:8">
       <c r="A457" s="7"/>
-      <c r="B457" s="22"/>
+      <c r="B457" s="6"/>
       <c r="C457" s="7"/>
       <c r="D457" s="7"/>
       <c r="E457" s="7"/>
@@ -10767,7 +10892,7 @@
     </row>
     <row r="463" spans="1:8">
       <c r="A463" s="7"/>
-      <c r="B463" s="7"/>
+      <c r="B463" s="22"/>
       <c r="C463" s="7"/>
       <c r="D463" s="7"/>
       <c r="E463" s="7"/>
@@ -10777,7 +10902,7 @@
     </row>
     <row r="464" spans="1:8">
       <c r="A464" s="7"/>
-      <c r="B464" s="6"/>
+      <c r="B464" s="7"/>
       <c r="C464" s="7"/>
       <c r="D464" s="7"/>
       <c r="E464" s="7"/>
@@ -10787,7 +10912,7 @@
     </row>
     <row r="465" spans="1:8">
       <c r="A465" s="7"/>
-      <c r="B465" s="22"/>
+      <c r="B465" s="6"/>
       <c r="C465" s="7"/>
       <c r="D465" s="7"/>
       <c r="E465" s="7"/>
@@ -10816,8 +10941,8 @@
       <c r="H467" s="7"/>
     </row>
     <row r="468" spans="1:8">
-      <c r="A468" s="6"/>
-      <c r="B468" s="7"/>
+      <c r="A468" s="7"/>
+      <c r="B468" s="22"/>
       <c r="C468" s="7"/>
       <c r="D468" s="7"/>
       <c r="E468" s="7"/>
@@ -10826,7 +10951,7 @@
       <c r="H468" s="7"/>
     </row>
     <row r="469" spans="1:8">
-      <c r="A469" s="7"/>
+      <c r="A469" s="6"/>
       <c r="B469" s="7"/>
       <c r="C469" s="7"/>
       <c r="D469" s="7"/>
@@ -10867,7 +10992,7 @@
     </row>
     <row r="473" spans="1:8">
       <c r="A473" s="7"/>
-      <c r="B473" s="28"/>
+      <c r="B473" s="7"/>
       <c r="C473" s="7"/>
       <c r="D473" s="7"/>
       <c r="E473" s="7"/>
@@ -10897,7 +11022,7 @@
     </row>
     <row r="476" spans="1:8">
       <c r="A476" s="7"/>
-      <c r="B476" s="7"/>
+      <c r="B476" s="28"/>
       <c r="C476" s="7"/>
       <c r="D476" s="7"/>
       <c r="E476" s="7"/>
@@ -10907,7 +11032,7 @@
     </row>
     <row r="477" spans="1:8">
       <c r="A477" s="7"/>
-      <c r="B477" s="28"/>
+      <c r="B477" s="7"/>
       <c r="C477" s="7"/>
       <c r="D477" s="7"/>
       <c r="E477" s="7"/>
@@ -10917,7 +11042,7 @@
     </row>
     <row r="478" spans="1:8">
       <c r="A478" s="7"/>
-      <c r="B478" s="7"/>
+      <c r="B478" s="28"/>
       <c r="C478" s="7"/>
       <c r="D478" s="7"/>
       <c r="E478" s="7"/>
@@ -10927,21 +11052,21 @@
     </row>
     <row r="479" spans="1:8">
       <c r="A479" s="7"/>
-      <c r="B479" s="29"/>
-      <c r="C479" s="30"/>
+      <c r="B479" s="7"/>
+      <c r="C479" s="7"/>
       <c r="D479" s="7"/>
       <c r="E479" s="7"/>
-      <c r="F479" s="29"/>
+      <c r="F479" s="7"/>
       <c r="G479" s="30"/>
       <c r="H479" s="7"/>
     </row>
     <row r="480" spans="1:8">
       <c r="A480" s="7"/>
-      <c r="B480" s="7"/>
-      <c r="C480" s="7"/>
+      <c r="B480" s="29"/>
+      <c r="C480" s="30"/>
       <c r="D480" s="7"/>
       <c r="E480" s="7"/>
-      <c r="F480" s="7"/>
+      <c r="F480" s="29"/>
       <c r="G480" s="30"/>
       <c r="H480" s="7"/>
     </row>
@@ -14845,6 +14970,16 @@
       <c r="G870" s="30"/>
       <c r="H870" s="7"/>
     </row>
+    <row r="871" spans="1:8">
+      <c r="A871" s="7"/>
+      <c r="B871" s="7"/>
+      <c r="C871" s="7"/>
+      <c r="D871" s="7"/>
+      <c r="E871" s="7"/>
+      <c r="F871" s="7"/>
+      <c r="G871" s="30"/>
+      <c r="H871" s="7"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>